<commit_message>
Changed username to friendly_name to distinguish from full_name.
</commit_message>
<xml_diff>
--- a/documents/Testing Schedule.xlsx
+++ b/documents/Testing Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Node\Timelog\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2204A38B-A2A5-4234-9735-DF300D879BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5747E2E1-8BD8-45DF-9C5A-70C10CE6E20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{9AAAF6DA-95E7-49F0-B7DD-46373E33B9E7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="87">
   <si>
     <t>RMPC Timelog Testing Schedule</t>
   </si>
@@ -2445,7 +2445,7 @@
   <dimension ref="B2:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2581,8 +2581,12 @@
       <c r="D8" s="67" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
+      <c r="E8" s="66" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="66" t="s">
+        <v>71</v>
+      </c>
       <c r="G8" s="74" t="s">
         <v>85</v>
       </c>
@@ -2636,7 +2640,9 @@
       <c r="E11" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="F11" s="66"/>
+      <c r="F11" s="66" t="s">
+        <v>71</v>
+      </c>
       <c r="G11" s="74" t="s">
         <v>82</v>
       </c>

</xml_diff>

<commit_message>
#1 - Default account type set to freelance and disabled pending end of Beta Promotion.
</commit_message>
<xml_diff>
--- a/documents/Testing Schedule.xlsx
+++ b/documents/Testing Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Node\Timelog\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA779D4A-2CF9-4F72-9B61-7A686A66BF83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF11C611-A5C1-40D3-86F1-87ACF8DD75E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{9AAAF6DA-95E7-49F0-B7DD-46373E33B9E7}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="124">
   <si>
     <t>RMPC Timelog Testing Schedule</t>
   </si>
@@ -363,9 +363,6 @@
     <t>Click link</t>
   </si>
   <si>
-    <t>Temporarily disabled</t>
-  </si>
-  <si>
     <t>Navigate</t>
   </si>
   <si>
@@ -394,13 +391,31 @@
   </si>
   <si>
     <t>Y - Pass / Fixed</t>
+  </si>
+  <si>
+    <t>Temporarily disabled until payments imposed</t>
+  </si>
+  <si>
+    <t>Issue #</t>
+  </si>
+  <si>
+    <t>#1</t>
+  </si>
+  <si>
+    <t>#2</t>
+  </si>
+  <si>
+    <t>#3</t>
+  </si>
+  <si>
+    <t>SHOWSTOPPER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,8 +463,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFEA8B00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -483,6 +514,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -668,7 +705,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -804,42 +841,39 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -980,6 +1014,42 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -987,6 +1057,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFEA8B00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1295,11 +1370,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDA5C5C7-8B67-4FAF-9315-0E07B94A4E72}">
-  <dimension ref="B2:O76"/>
+  <dimension ref="B2:Q77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
+      <selection pane="bottomLeft" activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,49 +1383,53 @@
     <col min="2" max="2" width="5.7109375" style="3" customWidth="1"/>
     <col min="3" max="7" width="10.7109375" style="2" customWidth="1"/>
     <col min="8" max="8" width="35.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="2" customWidth="1"/>
     <col min="10" max="10" width="29.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" style="102" customWidth="1"/>
-    <col min="13" max="13" width="28.28515625" style="90" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="2"/>
+    <col min="12" max="13" width="11.28515625" style="101" customWidth="1"/>
+    <col min="14" max="14" width="42.7109375" style="89" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="100" t="s">
-        <v>118</v>
-      </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="O2" s="97"/>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="101" t="s">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B2" s="99" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="101"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
-      <c r="G3" s="1" t="s">
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="P2" s="96"/>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B3" s="118" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="115"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="116"/>
+      <c r="F3" s="117"/>
+      <c r="H3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="O3" s="98"/>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="101" t="s">
-        <v>116</v>
-      </c>
-      <c r="C4" s="101"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101"/>
+      <c r="I3" s="1"/>
+      <c r="L3" s="2"/>
+      <c r="N3" s="101"/>
+      <c r="O3" s="89"/>
+      <c r="Q3" s="97"/>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B4" s="100" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="O4" s="99"/>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P4" s="98"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
         <v>30</v>
       </c>
@@ -1362,65 +1441,73 @@
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
       <c r="H6" s="15"/>
-      <c r="I6" s="85" t="s">
+      <c r="I6" s="84" t="s">
         <v>105</v>
       </c>
-      <c r="J6" s="86"/>
+      <c r="J6" s="85"/>
       <c r="K6" s="16" t="s">
         <v>79</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="M6" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="M6" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="N6" s="17" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="11">
         <v>1</v>
       </c>
-      <c r="C7" s="84" t="s">
+      <c r="C7" s="83" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="55"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="54"/>
       <c r="K7" s="4"/>
-      <c r="L7" s="103"/>
-      <c r="M7" s="50"/>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L7" s="102"/>
+      <c r="M7" s="102"/>
+      <c r="N7" s="49"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="11">
         <f>B7+1</f>
         <v>2</v>
       </c>
       <c r="C8" s="41"/>
-      <c r="D8" s="53" t="s">
+      <c r="D8" s="52" t="s">
         <v>104</v>
       </c>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="74" t="s">
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="73" t="s">
         <v>107</v>
       </c>
-      <c r="J8" s="55"/>
+      <c r="J8" s="54"/>
       <c r="K8" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="L8" s="103" t="s">
+        <v>108</v>
+      </c>
+      <c r="L8" s="88" t="s">
         <v>70</v>
       </c>
-      <c r="M8" s="50"/>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="11"/>
+      <c r="M8" s="88"/>
+      <c r="N8" s="49"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="11">
+        <f t="shared" ref="B9:B36" si="0">B8+1</f>
+        <v>3</v>
+      </c>
       <c r="C9" s="41"/>
       <c r="D9" s="42" t="s">
         <v>94</v>
@@ -1432,11 +1519,15 @@
       <c r="I9" s="45"/>
       <c r="J9" s="46"/>
       <c r="K9" s="4"/>
-      <c r="L9" s="103"/>
-      <c r="M9" s="50"/>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
+      <c r="L9" s="102"/>
+      <c r="M9" s="102"/>
+      <c r="N9" s="49"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B10" s="11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
       <c r="C10" s="41"/>
       <c r="D10" s="42"/>
       <c r="E10" s="42" t="s">
@@ -1446,21 +1537,27 @@
       <c r="G10" s="42"/>
       <c r="H10" s="43"/>
       <c r="I10" s="45" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J10" s="46"/>
       <c r="K10" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="L10" s="104" t="s">
+      <c r="L10" s="114" t="s">
         <v>70</v>
       </c>
-      <c r="M10" s="91" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="11"/>
+      <c r="M10" s="111" t="s">
+        <v>122</v>
+      </c>
+      <c r="N10" s="90" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B11" s="11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
       <c r="C11" s="41"/>
       <c r="D11" s="42"/>
       <c r="E11" s="42" t="s">
@@ -1470,19 +1567,23 @@
       <c r="G11" s="42"/>
       <c r="H11" s="43"/>
       <c r="I11" s="45" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J11" s="46"/>
       <c r="K11" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="L11" s="104" t="s">
+      <c r="L11" s="114" t="s">
         <v>70</v>
       </c>
-      <c r="M11" s="92"/>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="11"/>
+      <c r="M11" s="112"/>
+      <c r="N11" s="91"/>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="11">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
       <c r="C12" s="41"/>
       <c r="D12" s="42"/>
       <c r="E12" s="42" t="s">
@@ -1492,19 +1593,23 @@
       <c r="G12" s="42"/>
       <c r="H12" s="43"/>
       <c r="I12" s="45" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J12" s="46"/>
       <c r="K12" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="L12" s="104" t="s">
+      <c r="L12" s="114" t="s">
         <v>70</v>
       </c>
-      <c r="M12" s="92"/>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="11"/>
+      <c r="M12" s="112"/>
+      <c r="N12" s="91"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="11">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
       <c r="C13" s="41"/>
       <c r="D13" s="42"/>
       <c r="E13" s="42" t="s">
@@ -1514,19 +1619,23 @@
       <c r="G13" s="42"/>
       <c r="H13" s="43"/>
       <c r="I13" s="45" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J13" s="46"/>
       <c r="K13" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="L13" s="104" t="s">
+      <c r="L13" s="114" t="s">
         <v>70</v>
       </c>
-      <c r="M13" s="93"/>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="11"/>
+      <c r="M13" s="113"/>
+      <c r="N13" s="92"/>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B14" s="11">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
       <c r="C14" s="41"/>
       <c r="D14" s="42"/>
       <c r="E14" s="42" t="s">
@@ -1536,19 +1645,25 @@
       <c r="G14" s="42"/>
       <c r="H14" s="43"/>
       <c r="I14" s="45" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J14" s="46"/>
       <c r="K14" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="L14" s="104" t="s">
-        <v>115</v>
-      </c>
-      <c r="M14" s="50"/>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="11"/>
+      <c r="L14" s="103" t="s">
+        <v>114</v>
+      </c>
+      <c r="M14" s="103" t="s">
+        <v>121</v>
+      </c>
+      <c r="N14" s="49"/>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B15" s="11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
       <c r="C15" s="41"/>
       <c r="D15" s="42"/>
       <c r="E15" s="42" t="s">
@@ -1558,21 +1673,27 @@
       <c r="G15" s="42"/>
       <c r="H15" s="43"/>
       <c r="I15" s="45" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J15" s="46"/>
       <c r="K15" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="L15" s="104" t="s">
+      <c r="L15" s="114" t="s">
         <v>70</v>
       </c>
-      <c r="M15" s="50" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="11"/>
+      <c r="M15" s="114" t="s">
+        <v>122</v>
+      </c>
+      <c r="N15" s="49" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B16" s="11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="C16" s="41"/>
       <c r="D16" s="42"/>
       <c r="E16" s="42" t="s">
@@ -1581,963 +1702,1043 @@
       <c r="F16" s="42"/>
       <c r="G16" s="42"/>
       <c r="H16" s="43"/>
-      <c r="I16" s="74" t="s">
-        <v>113</v>
-      </c>
-      <c r="J16" s="55"/>
+      <c r="I16" s="73" t="s">
+        <v>112</v>
+      </c>
+      <c r="J16" s="54"/>
       <c r="K16" s="45" t="s">
         <v>97</v>
       </c>
       <c r="L16" s="88" t="s">
-        <v>115</v>
-      </c>
-      <c r="M16" s="50" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="11"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="M16" s="88" t="s">
+        <v>120</v>
+      </c>
+      <c r="N16" s="49" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="108" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="109"/>
+      <c r="D17" s="109"/>
+      <c r="E17" s="109"/>
+      <c r="F17" s="109"/>
+      <c r="G17" s="109"/>
+      <c r="H17" s="109"/>
+      <c r="I17" s="109"/>
+      <c r="J17" s="109"/>
+      <c r="K17" s="109"/>
+      <c r="L17" s="109"/>
+      <c r="M17" s="109"/>
+      <c r="N17" s="110"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="11">
+        <f>B16+1</f>
+        <v>11</v>
+      </c>
+      <c r="C18" s="41"/>
+      <c r="D18" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="46"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="103"/>
-      <c r="M17" s="50"/>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="11"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42" t="s">
-        <v>112</v>
-      </c>
+      <c r="E18" s="42"/>
       <c r="F18" s="42"/>
       <c r="G18" s="42"/>
       <c r="H18" s="43"/>
-      <c r="I18" s="45" t="s">
-        <v>110</v>
-      </c>
+      <c r="I18" s="45"/>
       <c r="J18" s="46"/>
-      <c r="K18" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="L18" s="103"/>
-      <c r="M18" s="50"/>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="11"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="102"/>
+      <c r="M18" s="102"/>
+      <c r="N18" s="49"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="11">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
       <c r="C19" s="41"/>
       <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
+      <c r="E19" s="42" t="s">
+        <v>111</v>
+      </c>
       <c r="F19" s="42"/>
       <c r="G19" s="42"/>
       <c r="H19" s="43"/>
-      <c r="I19" s="45"/>
+      <c r="I19" s="45" t="s">
+        <v>109</v>
+      </c>
       <c r="J19" s="46"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="103"/>
-      <c r="M19" s="50"/>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="K19" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="L19" s="102"/>
+      <c r="M19" s="102"/>
+      <c r="N19" s="49"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="11">
-        <f>B8+1</f>
-        <v>3</v>
-      </c>
-      <c r="C20" s="84" t="s">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C20" s="41"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="102"/>
+      <c r="M20" s="102"/>
+      <c r="N20" s="49"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" s="11">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C21" s="83" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="54"/>
-      <c r="I20" s="74"/>
-      <c r="J20" s="55"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="103"/>
-      <c r="M20" s="50"/>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="11">
-        <f t="shared" ref="B21:B26" si="0">B20+1</f>
-        <v>4</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="53" t="s">
-        <v>88</v>
-      </c>
-      <c r="E21" s="53"/>
-      <c r="F21" s="53"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="74" t="s">
-        <v>89</v>
-      </c>
-      <c r="J21" s="55"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="73"/>
+      <c r="J21" s="54"/>
       <c r="K21" s="4"/>
-      <c r="L21" s="103"/>
-      <c r="M21" s="50"/>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L21" s="102"/>
+      <c r="M21" s="102"/>
+      <c r="N21" s="49"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="11">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C22" s="5"/>
-      <c r="D22" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="74" t="s">
-        <v>5</v>
-      </c>
-      <c r="J22" s="55"/>
+      <c r="D22" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" s="52"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="73" t="s">
+        <v>89</v>
+      </c>
+      <c r="J22" s="54"/>
       <c r="K22" s="4"/>
-      <c r="L22" s="103"/>
-      <c r="M22" s="50"/>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L22" s="102"/>
+      <c r="M22" s="102"/>
+      <c r="N22" s="49"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="11">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C23" s="76" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="68"/>
-      <c r="E23" s="68"/>
-      <c r="F23" s="68"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="69"/>
-      <c r="I23" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="J23" s="55"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="73" t="s">
+        <v>5</v>
+      </c>
+      <c r="J23" s="54"/>
       <c r="K23" s="4"/>
-      <c r="L23" s="103"/>
-      <c r="M23" s="50"/>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L23" s="102"/>
+      <c r="M23" s="102"/>
+      <c r="N23" s="49"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="11">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C24" s="78"/>
-      <c r="D24" s="72"/>
-      <c r="E24" s="72"/>
-      <c r="F24" s="72"/>
-      <c r="G24" s="72"/>
-      <c r="H24" s="73"/>
-      <c r="I24" s="74" t="s">
-        <v>25</v>
-      </c>
-      <c r="J24" s="55"/>
+        <v>17</v>
+      </c>
+      <c r="C24" s="75" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="67"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="67"/>
+      <c r="H24" s="68"/>
+      <c r="I24" s="73" t="s">
+        <v>16</v>
+      </c>
+      <c r="J24" s="54"/>
       <c r="K24" s="4"/>
-      <c r="L24" s="103"/>
-      <c r="M24" s="50"/>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L24" s="102"/>
+      <c r="M24" s="102"/>
+      <c r="N24" s="49"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="11">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C25" s="62"/>
-      <c r="D25" s="68" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="68"/>
-      <c r="F25" s="68"/>
-      <c r="G25" s="68"/>
-      <c r="H25" s="69"/>
-      <c r="I25" s="74" t="s">
-        <v>14</v>
-      </c>
-      <c r="J25" s="55"/>
+        <v>18</v>
+      </c>
+      <c r="C25" s="77"/>
+      <c r="D25" s="71"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="71"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="73" t="s">
+        <v>25</v>
+      </c>
+      <c r="J25" s="54"/>
       <c r="K25" s="4"/>
-      <c r="L25" s="103"/>
-      <c r="M25" s="50"/>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L25" s="102"/>
+      <c r="M25" s="102"/>
+      <c r="N25" s="49"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="11">
         <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="C26" s="61"/>
+      <c r="D26" s="67" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="67"/>
+      <c r="F26" s="67"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="73" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26" s="54"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="102"/>
+      <c r="M26" s="102"/>
+      <c r="N26" s="49"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B27" s="11">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C27" s="65"/>
+      <c r="D27" s="71"/>
+      <c r="E27" s="71"/>
+      <c r="F27" s="71"/>
+      <c r="G27" s="71"/>
+      <c r="H27" s="72"/>
+      <c r="I27" s="73" t="s">
+        <v>49</v>
+      </c>
+      <c r="J27" s="54"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="102"/>
+      <c r="M27" s="102"/>
+      <c r="N27" s="49"/>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B28" s="11">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C28" s="61"/>
+      <c r="D28" s="67" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="67"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="68"/>
+      <c r="I28" s="73" t="s">
+        <v>28</v>
+      </c>
+      <c r="J28" s="54"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="102"/>
+      <c r="M28" s="102"/>
+      <c r="N28" s="49"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B29" s="11">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="C29" s="63"/>
+      <c r="D29" s="69"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="69"/>
+      <c r="G29" s="69"/>
+      <c r="H29" s="70"/>
+      <c r="I29" s="73" t="s">
+        <v>50</v>
+      </c>
+      <c r="J29" s="54"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="102"/>
+      <c r="M29" s="102"/>
+      <c r="N29" s="49"/>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B30" s="11">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="C30" s="65"/>
+      <c r="D30" s="71"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="72"/>
+      <c r="I30" s="73" t="s">
+        <v>54</v>
+      </c>
+      <c r="J30" s="54"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="102"/>
+      <c r="M30" s="102"/>
+      <c r="N30" s="49"/>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B31" s="11">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="C31" s="48"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="53"/>
+      <c r="I31" s="73" t="s">
+        <v>57</v>
+      </c>
+      <c r="J31" s="54"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="102"/>
+      <c r="M31" s="102"/>
+      <c r="N31" s="49"/>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B32" s="11">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C32" s="61"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="62"/>
+      <c r="F32" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" s="67"/>
+      <c r="H32" s="68"/>
+      <c r="I32" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="J32" s="55"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="102"/>
+      <c r="M32" s="102"/>
+      <c r="N32" s="49"/>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B33" s="11">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="C33" s="63"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="69"/>
+      <c r="G33" s="69"/>
+      <c r="H33" s="70"/>
+      <c r="I33" s="90" t="s">
+        <v>33</v>
+      </c>
+      <c r="J33" s="55"/>
+      <c r="K33" s="55"/>
+      <c r="L33" s="86"/>
+      <c r="M33" s="86"/>
+      <c r="N33" s="55"/>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B34" s="11">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="C34" s="63"/>
+      <c r="D34" s="64"/>
+      <c r="E34" s="64"/>
+      <c r="F34" s="69"/>
+      <c r="G34" s="69"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K34" s="4"/>
+      <c r="L34" s="102"/>
+      <c r="M34" s="102"/>
+      <c r="N34" s="49"/>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B35" s="11">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="C35" s="63"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="69"/>
+      <c r="G35" s="69"/>
+      <c r="H35" s="69"/>
+      <c r="I35" s="107"/>
+      <c r="J35" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K35" s="4"/>
+      <c r="L35" s="102"/>
+      <c r="M35" s="102"/>
+      <c r="N35" s="49"/>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B36" s="11">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="C36" s="65"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="66"/>
+      <c r="F36" s="71"/>
+      <c r="G36" s="71"/>
+      <c r="H36" s="72"/>
+      <c r="I36" s="107"/>
+      <c r="J36" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K36" s="10"/>
+      <c r="L36" s="87"/>
+      <c r="M36" s="87"/>
+      <c r="N36" s="49" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B37" s="44">
+        <f>B32+1</f>
+        <v>26</v>
+      </c>
+      <c r="C37" s="56"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="F37" s="52"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="53"/>
+      <c r="I37" s="73" t="s">
+        <v>56</v>
+      </c>
+      <c r="J37" s="54"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="102"/>
+      <c r="M37" s="102"/>
+      <c r="N37" s="49"/>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B38" s="58">
+        <f>B37+1</f>
+        <v>27</v>
+      </c>
+      <c r="C38" s="61"/>
+      <c r="D38" s="62"/>
+      <c r="E38" s="62"/>
+      <c r="F38" s="67" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" s="67"/>
+      <c r="H38" s="68"/>
+      <c r="I38" s="73" t="s">
+        <v>55</v>
+      </c>
+      <c r="J38" s="54"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="102"/>
+      <c r="M38" s="102"/>
+      <c r="N38" s="49"/>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B39" s="60"/>
+      <c r="C39" s="65"/>
+      <c r="D39" s="66"/>
+      <c r="E39" s="66"/>
+      <c r="F39" s="71"/>
+      <c r="G39" s="71"/>
+      <c r="H39" s="72"/>
+      <c r="I39" s="73" t="s">
+        <v>35</v>
+      </c>
+      <c r="J39" s="54"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="102"/>
+      <c r="M39" s="102"/>
+      <c r="N39" s="49"/>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B40" s="44">
+        <f>B38+1</f>
+        <v>28</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="G40" s="52"/>
+      <c r="H40" s="53"/>
+      <c r="I40" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J40" s="8"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="102"/>
+      <c r="M40" s="102"/>
+      <c r="N40" s="49"/>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B41" s="58">
+        <f t="shared" ref="B41:B57" si="1">B40+1</f>
+        <v>29</v>
+      </c>
+      <c r="C41" s="61"/>
+      <c r="D41" s="62"/>
+      <c r="E41" s="62"/>
+      <c r="F41" s="67" t="s">
+        <v>8</v>
+      </c>
+      <c r="G41" s="67"/>
+      <c r="H41" s="68"/>
+      <c r="I41" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="66"/>
-      <c r="D26" s="72"/>
-      <c r="E26" s="72"/>
-      <c r="F26" s="72"/>
-      <c r="G26" s="72"/>
-      <c r="H26" s="73"/>
-      <c r="I26" s="74" t="s">
-        <v>49</v>
-      </c>
-      <c r="J26" s="55"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="103"/>
-      <c r="M26" s="50"/>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="59">
-        <f>B25+1</f>
-        <v>9</v>
-      </c>
-      <c r="C27" s="62"/>
-      <c r="D27" s="68" t="s">
-        <v>53</v>
-      </c>
-      <c r="E27" s="68"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="69"/>
-      <c r="I27" s="74" t="s">
-        <v>28</v>
-      </c>
-      <c r="J27" s="55"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="103"/>
-      <c r="M27" s="50"/>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="60"/>
-      <c r="C28" s="64"/>
-      <c r="D28" s="70"/>
-      <c r="E28" s="70"/>
-      <c r="F28" s="70"/>
-      <c r="G28" s="70"/>
-      <c r="H28" s="71"/>
-      <c r="I28" s="74" t="s">
-        <v>50</v>
-      </c>
-      <c r="J28" s="55"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="103"/>
-      <c r="M28" s="50"/>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="61"/>
-      <c r="C29" s="66"/>
-      <c r="D29" s="72"/>
-      <c r="E29" s="72"/>
-      <c r="F29" s="72"/>
-      <c r="G29" s="72"/>
-      <c r="H29" s="73"/>
-      <c r="I29" s="74" t="s">
-        <v>54</v>
-      </c>
-      <c r="J29" s="55"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="103"/>
-      <c r="M29" s="50"/>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="49">
-        <f>B27+1</f>
+      <c r="J41" s="82"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="104"/>
+      <c r="M41" s="104"/>
+      <c r="N41" s="93"/>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B42" s="60"/>
+      <c r="C42" s="65"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="66"/>
+      <c r="F42" s="71"/>
+      <c r="G42" s="71"/>
+      <c r="H42" s="72"/>
+      <c r="I42" s="73" t="s">
+        <v>37</v>
+      </c>
+      <c r="J42" s="54"/>
+      <c r="K42" s="18"/>
+      <c r="L42" s="104"/>
+      <c r="M42" s="104"/>
+      <c r="N42" s="93"/>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B43" s="58">
+        <f>B41+1</f>
+        <v>30</v>
+      </c>
+      <c r="C43" s="75"/>
+      <c r="D43" s="67"/>
+      <c r="E43" s="67"/>
+      <c r="F43" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="53" t="s">
-        <v>20</v>
-      </c>
-      <c r="F30" s="53"/>
-      <c r="G30" s="53"/>
-      <c r="H30" s="54"/>
-      <c r="I30" s="74" t="s">
-        <v>57</v>
-      </c>
-      <c r="J30" s="55"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="103"/>
-      <c r="M30" s="50"/>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="59">
-        <f>B30+1</f>
-        <v>11</v>
-      </c>
-      <c r="C31" s="62"/>
-      <c r="D31" s="63"/>
-      <c r="E31" s="63"/>
-      <c r="F31" s="68" t="s">
-        <v>10</v>
-      </c>
-      <c r="G31" s="68"/>
-      <c r="H31" s="69"/>
-      <c r="I31" s="56" t="s">
+      <c r="G43" s="67"/>
+      <c r="H43" s="68"/>
+      <c r="I43" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="J31" s="56"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="103"/>
-      <c r="M31" s="50"/>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="60"/>
-      <c r="C32" s="64"/>
-      <c r="D32" s="65"/>
-      <c r="E32" s="65"/>
-      <c r="F32" s="70"/>
-      <c r="G32" s="70"/>
-      <c r="H32" s="71"/>
-      <c r="I32" s="56" t="s">
+      <c r="J43" s="54"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="102"/>
+      <c r="M43" s="102"/>
+      <c r="N43" s="49"/>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B44" s="59"/>
+      <c r="C44" s="76"/>
+      <c r="D44" s="69"/>
+      <c r="E44" s="69"/>
+      <c r="F44" s="69"/>
+      <c r="G44" s="69"/>
+      <c r="H44" s="70"/>
+      <c r="I44" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="J32" s="56"/>
-      <c r="K32" s="56"/>
-      <c r="L32" s="87"/>
-      <c r="M32" s="56"/>
-    </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B33" s="60"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="65"/>
-      <c r="E33" s="65"/>
-      <c r="F33" s="70"/>
-      <c r="G33" s="70"/>
-      <c r="H33" s="71"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K33" s="4"/>
-      <c r="L33" s="103"/>
-      <c r="M33" s="50"/>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B34" s="60"/>
-      <c r="C34" s="64"/>
-      <c r="D34" s="65"/>
-      <c r="E34" s="65"/>
-      <c r="F34" s="70"/>
-      <c r="G34" s="70"/>
-      <c r="H34" s="71"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="K34" s="4"/>
-      <c r="L34" s="103"/>
-      <c r="M34" s="50"/>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B35" s="61"/>
-      <c r="C35" s="66"/>
-      <c r="D35" s="67"/>
-      <c r="E35" s="67"/>
-      <c r="F35" s="72"/>
-      <c r="G35" s="72"/>
-      <c r="H35" s="73"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="K35" s="10"/>
-      <c r="L35" s="88"/>
-      <c r="M35" s="50" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B36" s="44">
-        <f>B31+1</f>
-        <v>12</v>
-      </c>
-      <c r="C36" s="57"/>
-      <c r="D36" s="58"/>
-      <c r="E36" s="53" t="s">
-        <v>21</v>
-      </c>
-      <c r="F36" s="53"/>
-      <c r="G36" s="53"/>
-      <c r="H36" s="54"/>
-      <c r="I36" s="74" t="s">
-        <v>56</v>
-      </c>
-      <c r="J36" s="55"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="103"/>
-      <c r="M36" s="50"/>
-    </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B37" s="59">
-        <f>B36+1</f>
-        <v>13</v>
-      </c>
-      <c r="C37" s="62"/>
-      <c r="D37" s="63"/>
-      <c r="E37" s="63"/>
-      <c r="F37" s="68" t="s">
-        <v>7</v>
-      </c>
-      <c r="G37" s="68"/>
-      <c r="H37" s="69"/>
-      <c r="I37" s="74" t="s">
-        <v>55</v>
-      </c>
-      <c r="J37" s="55"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="103"/>
-      <c r="M37" s="50"/>
-    </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B38" s="61"/>
-      <c r="C38" s="66"/>
-      <c r="D38" s="67"/>
-      <c r="E38" s="67"/>
-      <c r="F38" s="72"/>
-      <c r="G38" s="72"/>
-      <c r="H38" s="73"/>
-      <c r="I38" s="74" t="s">
-        <v>35</v>
-      </c>
-      <c r="J38" s="55"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="103"/>
-      <c r="M38" s="50"/>
-    </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B39" s="44">
-        <f>B37+1</f>
-        <v>14</v>
-      </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="53" t="s">
-        <v>17</v>
-      </c>
-      <c r="G39" s="53"/>
-      <c r="H39" s="54"/>
-      <c r="I39" s="74" t="s">
-        <v>18</v>
-      </c>
-      <c r="J39" s="55"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="103"/>
-      <c r="M39" s="50"/>
-    </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B40" s="59">
-        <f t="shared" ref="B40:B56" si="1">B39+1</f>
-        <v>15</v>
-      </c>
-      <c r="C40" s="62"/>
-      <c r="D40" s="63"/>
-      <c r="E40" s="63"/>
-      <c r="F40" s="68" t="s">
-        <v>8</v>
-      </c>
-      <c r="G40" s="68"/>
-      <c r="H40" s="69"/>
-      <c r="I40" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="J40" s="83"/>
-      <c r="K40" s="18"/>
-      <c r="L40" s="105"/>
-      <c r="M40" s="94"/>
-    </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B41" s="61"/>
-      <c r="C41" s="66"/>
-      <c r="D41" s="67"/>
-      <c r="E41" s="67"/>
-      <c r="F41" s="72"/>
-      <c r="G41" s="72"/>
-      <c r="H41" s="73"/>
-      <c r="I41" s="74" t="s">
-        <v>37</v>
-      </c>
-      <c r="J41" s="55"/>
-      <c r="K41" s="18"/>
-      <c r="L41" s="105"/>
-      <c r="M41" s="94"/>
-    </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B42" s="59">
-        <f>B40+1</f>
-        <v>16</v>
-      </c>
-      <c r="C42" s="76"/>
-      <c r="D42" s="68"/>
-      <c r="E42" s="68"/>
-      <c r="F42" s="68" t="s">
-        <v>10</v>
-      </c>
-      <c r="G42" s="68"/>
-      <c r="H42" s="69"/>
-      <c r="I42" s="74" t="s">
-        <v>31</v>
-      </c>
-      <c r="J42" s="55"/>
-      <c r="K42" s="4"/>
-      <c r="L42" s="103"/>
-      <c r="M42" s="50"/>
-    </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B43" s="60"/>
-      <c r="C43" s="77"/>
-      <c r="D43" s="70"/>
-      <c r="E43" s="70"/>
-      <c r="F43" s="70"/>
-      <c r="G43" s="70"/>
-      <c r="H43" s="71"/>
-      <c r="I43" s="74" t="s">
-        <v>33</v>
-      </c>
-      <c r="J43" s="79"/>
-      <c r="K43" s="79"/>
-      <c r="L43" s="75"/>
-      <c r="M43" s="79"/>
-    </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B44" s="60"/>
-      <c r="C44" s="77"/>
-      <c r="D44" s="70"/>
-      <c r="E44" s="70"/>
-      <c r="F44" s="70"/>
-      <c r="G44" s="70"/>
-      <c r="H44" s="71"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="K44" s="8"/>
-      <c r="L44" s="106"/>
-      <c r="M44" s="50"/>
-    </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B45" s="60"/>
-      <c r="C45" s="77"/>
-      <c r="D45" s="70"/>
-      <c r="E45" s="70"/>
-      <c r="F45" s="70"/>
-      <c r="G45" s="70"/>
-      <c r="H45" s="71"/>
+      <c r="J44" s="78"/>
+      <c r="K44" s="78"/>
+      <c r="L44" s="74"/>
+      <c r="M44" s="74"/>
+      <c r="N44" s="78"/>
+    </row>
+    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B45" s="59"/>
+      <c r="C45" s="76"/>
+      <c r="D45" s="69"/>
+      <c r="E45" s="69"/>
+      <c r="F45" s="69"/>
+      <c r="G45" s="69"/>
+      <c r="H45" s="70"/>
       <c r="I45" s="7"/>
       <c r="J45" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="K45" s="4"/>
-      <c r="L45" s="103"/>
-      <c r="M45" s="50"/>
-    </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B46" s="61"/>
-      <c r="C46" s="78"/>
-      <c r="D46" s="72"/>
-      <c r="E46" s="72"/>
-      <c r="F46" s="72"/>
-      <c r="G46" s="72"/>
-      <c r="H46" s="73"/>
+        <v>32</v>
+      </c>
+      <c r="K45" s="8"/>
+      <c r="L45" s="105"/>
+      <c r="M45" s="105"/>
+      <c r="N45" s="49"/>
+    </row>
+    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B46" s="59"/>
+      <c r="C46" s="76"/>
+      <c r="D46" s="69"/>
+      <c r="E46" s="69"/>
+      <c r="F46" s="69"/>
+      <c r="G46" s="69"/>
+      <c r="H46" s="70"/>
       <c r="I46" s="7"/>
       <c r="J46" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K46" s="4"/>
+      <c r="L46" s="102"/>
+      <c r="M46" s="102"/>
+      <c r="N46" s="49"/>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B47" s="60"/>
+      <c r="C47" s="77"/>
+      <c r="D47" s="71"/>
+      <c r="E47" s="71"/>
+      <c r="F47" s="71"/>
+      <c r="G47" s="71"/>
+      <c r="H47" s="72"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="K46" s="10"/>
-      <c r="L46" s="88"/>
-      <c r="M46" s="50" t="s">
+      <c r="K47" s="10"/>
+      <c r="L47" s="87"/>
+      <c r="M47" s="87"/>
+      <c r="N47" s="49" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B47" s="11">
-        <f>B42+1</f>
-        <v>17</v>
-      </c>
-      <c r="C47" s="78" t="s">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B48" s="11">
+        <f>B43+1</f>
+        <v>31</v>
+      </c>
+      <c r="C48" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="D47" s="72"/>
-      <c r="E47" s="72"/>
-      <c r="F47" s="72"/>
-      <c r="G47" s="72"/>
-      <c r="H47" s="54"/>
-      <c r="I47" s="80" t="s">
+      <c r="D48" s="71"/>
+      <c r="E48" s="71"/>
+      <c r="F48" s="71"/>
+      <c r="G48" s="71"/>
+      <c r="H48" s="53"/>
+      <c r="I48" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="J47" s="81"/>
-      <c r="K47" s="19"/>
-      <c r="L47" s="107"/>
-      <c r="M47" s="95"/>
-    </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B48" s="59">
+      <c r="J48" s="80"/>
+      <c r="K48" s="19"/>
+      <c r="L48" s="106"/>
+      <c r="M48" s="106"/>
+      <c r="N48" s="94"/>
+    </row>
+    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B49" s="58">
         <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="C48" s="62"/>
-      <c r="D48" s="68" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" s="61"/>
+      <c r="D49" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="E48" s="68"/>
-      <c r="F48" s="68"/>
-      <c r="G48" s="68"/>
-      <c r="H48" s="69"/>
-      <c r="I48" s="74" t="s">
+      <c r="E49" s="67"/>
+      <c r="F49" s="67"/>
+      <c r="G49" s="67"/>
+      <c r="H49" s="68"/>
+      <c r="I49" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="J48" s="55"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="103"/>
-      <c r="M48" s="50"/>
-    </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B49" s="61"/>
-      <c r="C49" s="66"/>
-      <c r="D49" s="72"/>
-      <c r="E49" s="72"/>
-      <c r="F49" s="72"/>
-      <c r="G49" s="72"/>
-      <c r="H49" s="73"/>
-      <c r="I49" s="74" t="s">
+      <c r="J49" s="54"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="102"/>
+      <c r="M49" s="102"/>
+      <c r="N49" s="49"/>
+    </row>
+    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B50" s="60"/>
+      <c r="C50" s="65"/>
+      <c r="D50" s="71"/>
+      <c r="E50" s="71"/>
+      <c r="F50" s="71"/>
+      <c r="G50" s="71"/>
+      <c r="H50" s="72"/>
+      <c r="I50" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="J49" s="55"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="103"/>
-      <c r="M49" s="50"/>
-    </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B50" s="11">
-        <f>B48+1</f>
-        <v>19</v>
-      </c>
-      <c r="C50" s="5"/>
-      <c r="D50" s="53" t="s">
+      <c r="J50" s="54"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="102"/>
+      <c r="M50" s="102"/>
+      <c r="N50" s="49"/>
+    </row>
+    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B51" s="11">
+        <f>B49+1</f>
+        <v>33</v>
+      </c>
+      <c r="C51" s="5"/>
+      <c r="D51" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="E50" s="53"/>
-      <c r="F50" s="53"/>
-      <c r="G50" s="53"/>
-      <c r="H50" s="54"/>
-      <c r="I50" s="51"/>
-      <c r="J50" s="75"/>
-      <c r="K50" s="75"/>
-      <c r="L50" s="75"/>
-      <c r="M50" s="75"/>
-    </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B51" s="59">
+      <c r="E51" s="52"/>
+      <c r="F51" s="52"/>
+      <c r="G51" s="52"/>
+      <c r="H51" s="53"/>
+      <c r="I51" s="50"/>
+      <c r="J51" s="74"/>
+      <c r="K51" s="74"/>
+      <c r="L51" s="74"/>
+      <c r="M51" s="74"/>
+      <c r="N51" s="74"/>
+    </row>
+    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B52" s="58">
         <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="C52" s="61"/>
+      <c r="D52" s="62"/>
+      <c r="E52" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C51" s="62"/>
-      <c r="D51" s="63"/>
-      <c r="E51" s="68" t="s">
-        <v>20</v>
-      </c>
-      <c r="F51" s="68"/>
-      <c r="G51" s="68"/>
-      <c r="H51" s="69"/>
-      <c r="I51" s="74" t="s">
+      <c r="F52" s="67"/>
+      <c r="G52" s="67"/>
+      <c r="H52" s="68"/>
+      <c r="I52" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="J51" s="55"/>
-      <c r="K51" s="4"/>
-      <c r="L51" s="103"/>
-      <c r="M51" s="50"/>
-    </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B52" s="60"/>
-      <c r="C52" s="64"/>
-      <c r="D52" s="65"/>
-      <c r="E52" s="70"/>
-      <c r="F52" s="70"/>
-      <c r="G52" s="70"/>
-      <c r="H52" s="71"/>
-      <c r="I52" s="74" t="s">
+      <c r="J52" s="54"/>
+      <c r="K52" s="4"/>
+      <c r="L52" s="102"/>
+      <c r="M52" s="102"/>
+      <c r="N52" s="49"/>
+    </row>
+    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B53" s="59"/>
+      <c r="C53" s="63"/>
+      <c r="D53" s="64"/>
+      <c r="E53" s="69"/>
+      <c r="F53" s="69"/>
+      <c r="G53" s="69"/>
+      <c r="H53" s="70"/>
+      <c r="I53" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="J52" s="55"/>
-      <c r="K52" s="20"/>
-      <c r="L52" s="89"/>
-      <c r="M52" s="96" t="s">
+      <c r="J53" s="54"/>
+      <c r="K53" s="20"/>
+      <c r="L53" s="88"/>
+      <c r="M53" s="88"/>
+      <c r="N53" s="95" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B53" s="60"/>
-      <c r="C53" s="64"/>
-      <c r="D53" s="65"/>
-      <c r="E53" s="70"/>
-      <c r="F53" s="70"/>
-      <c r="G53" s="70"/>
-      <c r="H53" s="71"/>
-      <c r="I53" s="74" t="s">
+    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B54" s="59"/>
+      <c r="C54" s="63"/>
+      <c r="D54" s="64"/>
+      <c r="E54" s="69"/>
+      <c r="F54" s="69"/>
+      <c r="G54" s="69"/>
+      <c r="H54" s="70"/>
+      <c r="I54" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="J53" s="55"/>
-      <c r="K53" s="4"/>
-      <c r="L53" s="103"/>
-      <c r="M53" s="50"/>
-    </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B54" s="61"/>
-      <c r="C54" s="66"/>
-      <c r="D54" s="67"/>
-      <c r="E54" s="72"/>
-      <c r="F54" s="72"/>
-      <c r="G54" s="72"/>
-      <c r="H54" s="73"/>
-      <c r="I54" s="74" t="s">
+      <c r="J54" s="54"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="102"/>
+      <c r="M54" s="102"/>
+      <c r="N54" s="49"/>
+    </row>
+    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B55" s="60"/>
+      <c r="C55" s="65"/>
+      <c r="D55" s="66"/>
+      <c r="E55" s="71"/>
+      <c r="F55" s="71"/>
+      <c r="G55" s="71"/>
+      <c r="H55" s="72"/>
+      <c r="I55" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="J54" s="55"/>
-      <c r="K54" s="20"/>
-      <c r="L54" s="89"/>
-      <c r="M54" s="96" t="s">
+      <c r="J55" s="54"/>
+      <c r="K55" s="20"/>
+      <c r="L55" s="88"/>
+      <c r="M55" s="88"/>
+      <c r="N55" s="95" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B55" s="11">
-        <f>B51+1</f>
+    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B56" s="11">
+        <f>B52+1</f>
+        <v>35</v>
+      </c>
+      <c r="C56" s="5"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="G56" s="52"/>
+      <c r="H56" s="53"/>
+      <c r="I56" s="73" t="s">
+        <v>22</v>
+      </c>
+      <c r="J56" s="54"/>
+      <c r="K56" s="4"/>
+      <c r="L56" s="102"/>
+      <c r="M56" s="102"/>
+      <c r="N56" s="49"/>
+    </row>
+    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B57" s="58">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="C57" s="61"/>
+      <c r="D57" s="62"/>
+      <c r="E57" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="C55" s="5"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="53" t="s">
-        <v>39</v>
-      </c>
-      <c r="G55" s="53"/>
-      <c r="H55" s="54"/>
-      <c r="I55" s="74" t="s">
-        <v>22</v>
-      </c>
-      <c r="J55" s="55"/>
-      <c r="K55" s="4"/>
-      <c r="L55" s="103"/>
-      <c r="M55" s="50"/>
-    </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B56" s="59">
-        <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-      <c r="C56" s="62"/>
-      <c r="D56" s="63"/>
-      <c r="E56" s="68" t="s">
-        <v>21</v>
-      </c>
-      <c r="F56" s="68"/>
-      <c r="G56" s="68"/>
-      <c r="H56" s="69"/>
-      <c r="I56" s="74" t="s">
+      <c r="F57" s="67"/>
+      <c r="G57" s="67"/>
+      <c r="H57" s="68"/>
+      <c r="I57" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="J56" s="55"/>
-      <c r="K56" s="4"/>
-      <c r="L56" s="103"/>
-      <c r="M56" s="50"/>
-    </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B57" s="60"/>
-      <c r="C57" s="64"/>
-      <c r="D57" s="65"/>
-      <c r="E57" s="70"/>
-      <c r="F57" s="70"/>
-      <c r="G57" s="70"/>
-      <c r="H57" s="71"/>
-      <c r="I57" s="74" t="s">
+      <c r="J57" s="54"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="102"/>
+      <c r="M57" s="102"/>
+      <c r="N57" s="49"/>
+    </row>
+    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B58" s="59"/>
+      <c r="C58" s="63"/>
+      <c r="D58" s="64"/>
+      <c r="E58" s="69"/>
+      <c r="F58" s="69"/>
+      <c r="G58" s="69"/>
+      <c r="H58" s="70"/>
+      <c r="I58" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="J57" s="55"/>
-      <c r="K57" s="4"/>
-      <c r="L57" s="103"/>
-      <c r="M57" s="50"/>
-    </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B58" s="60"/>
-      <c r="C58" s="64"/>
-      <c r="D58" s="65"/>
-      <c r="E58" s="70"/>
-      <c r="F58" s="70"/>
-      <c r="G58" s="70"/>
-      <c r="H58" s="71"/>
-      <c r="I58" s="74" t="s">
+      <c r="J58" s="54"/>
+      <c r="K58" s="4"/>
+      <c r="L58" s="102"/>
+      <c r="M58" s="102"/>
+      <c r="N58" s="49"/>
+    </row>
+    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B59" s="59"/>
+      <c r="C59" s="63"/>
+      <c r="D59" s="64"/>
+      <c r="E59" s="69"/>
+      <c r="F59" s="69"/>
+      <c r="G59" s="69"/>
+      <c r="H59" s="70"/>
+      <c r="I59" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="J58" s="55"/>
-      <c r="K58" s="4"/>
-      <c r="L58" s="103"/>
-      <c r="M58" s="50"/>
-    </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B59" s="60"/>
-      <c r="C59" s="64"/>
-      <c r="D59" s="65"/>
-      <c r="E59" s="70"/>
-      <c r="F59" s="70"/>
-      <c r="G59" s="70"/>
-      <c r="H59" s="71"/>
-      <c r="I59" s="74" t="s">
+      <c r="J59" s="54"/>
+      <c r="K59" s="4"/>
+      <c r="L59" s="102"/>
+      <c r="M59" s="102"/>
+      <c r="N59" s="49"/>
+    </row>
+    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B60" s="59"/>
+      <c r="C60" s="63"/>
+      <c r="D60" s="64"/>
+      <c r="E60" s="69"/>
+      <c r="F60" s="69"/>
+      <c r="G60" s="69"/>
+      <c r="H60" s="70"/>
+      <c r="I60" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="J59" s="55"/>
-      <c r="K59" s="4"/>
-      <c r="L59" s="103"/>
-      <c r="M59" s="50"/>
-    </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B60" s="61"/>
-      <c r="C60" s="64"/>
-      <c r="D60" s="65"/>
-      <c r="E60" s="70"/>
-      <c r="F60" s="70"/>
-      <c r="G60" s="70"/>
-      <c r="H60" s="71"/>
-      <c r="I60" s="74" t="s">
+      <c r="J60" s="54"/>
+      <c r="K60" s="4"/>
+      <c r="L60" s="102"/>
+      <c r="M60" s="102"/>
+      <c r="N60" s="49"/>
+    </row>
+    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B61" s="60"/>
+      <c r="C61" s="63"/>
+      <c r="D61" s="64"/>
+      <c r="E61" s="69"/>
+      <c r="F61" s="69"/>
+      <c r="G61" s="69"/>
+      <c r="H61" s="70"/>
+      <c r="I61" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="J60" s="55"/>
-      <c r="K60" s="4"/>
-      <c r="L60" s="103"/>
-      <c r="M60" s="50"/>
-    </row>
-    <row r="61" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B61" s="59">
-        <f>B56+1</f>
-        <v>23</v>
-      </c>
-      <c r="C61" s="62"/>
-      <c r="D61" s="63"/>
-      <c r="E61" s="63"/>
-      <c r="F61" s="68" t="s">
+      <c r="J61" s="54"/>
+      <c r="K61" s="4"/>
+      <c r="L61" s="102"/>
+      <c r="M61" s="102"/>
+      <c r="N61" s="49"/>
+    </row>
+    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B62" s="58">
+        <f>B57+1</f>
+        <v>37</v>
+      </c>
+      <c r="C62" s="61"/>
+      <c r="D62" s="62"/>
+      <c r="E62" s="62"/>
+      <c r="F62" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="G61" s="68"/>
-      <c r="H61" s="69"/>
-      <c r="I61" s="55" t="s">
+      <c r="G62" s="67"/>
+      <c r="H62" s="68"/>
+      <c r="I62" s="54" t="s">
         <v>45</v>
-      </c>
-      <c r="J61" s="56"/>
-      <c r="K61" s="4"/>
-      <c r="L61" s="103"/>
-      <c r="M61" s="50"/>
-    </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B62" s="60"/>
-      <c r="C62" s="64"/>
-      <c r="D62" s="65"/>
-      <c r="E62" s="65"/>
-      <c r="F62" s="70"/>
-      <c r="G62" s="70"/>
-      <c r="H62" s="71"/>
-      <c r="I62" s="74" t="s">
-        <v>46</v>
       </c>
       <c r="J62" s="55"/>
       <c r="K62" s="4"/>
-      <c r="L62" s="103"/>
-      <c r="M62" s="50"/>
-    </row>
-    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B63" s="60"/>
-      <c r="C63" s="64"/>
-      <c r="D63" s="65"/>
-      <c r="E63" s="65"/>
-      <c r="F63" s="70"/>
-      <c r="G63" s="70"/>
-      <c r="H63" s="71"/>
-      <c r="I63" s="74" t="s">
+      <c r="L62" s="102"/>
+      <c r="M62" s="102"/>
+      <c r="N62" s="49"/>
+    </row>
+    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B63" s="59"/>
+      <c r="C63" s="63"/>
+      <c r="D63" s="64"/>
+      <c r="E63" s="64"/>
+      <c r="F63" s="69"/>
+      <c r="G63" s="69"/>
+      <c r="H63" s="70"/>
+      <c r="I63" s="73" t="s">
+        <v>46</v>
+      </c>
+      <c r="J63" s="54"/>
+      <c r="K63" s="4"/>
+      <c r="L63" s="102"/>
+      <c r="M63" s="102"/>
+      <c r="N63" s="49"/>
+    </row>
+    <row r="64" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B64" s="59"/>
+      <c r="C64" s="63"/>
+      <c r="D64" s="64"/>
+      <c r="E64" s="64"/>
+      <c r="F64" s="69"/>
+      <c r="G64" s="69"/>
+      <c r="H64" s="70"/>
+      <c r="I64" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="J63" s="55"/>
-      <c r="K63" s="4"/>
-      <c r="L63" s="103"/>
-      <c r="M63" s="50"/>
-    </row>
-    <row r="64" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B64" s="61"/>
-      <c r="C64" s="66"/>
-      <c r="D64" s="67"/>
-      <c r="E64" s="67"/>
-      <c r="F64" s="72"/>
-      <c r="G64" s="72"/>
-      <c r="H64" s="73"/>
-      <c r="I64" s="74" t="s">
+      <c r="J64" s="54"/>
+      <c r="K64" s="4"/>
+      <c r="L64" s="102"/>
+      <c r="M64" s="102"/>
+      <c r="N64" s="49"/>
+    </row>
+    <row r="65" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B65" s="60"/>
+      <c r="C65" s="65"/>
+      <c r="D65" s="66"/>
+      <c r="E65" s="66"/>
+      <c r="F65" s="71"/>
+      <c r="G65" s="71"/>
+      <c r="H65" s="72"/>
+      <c r="I65" s="73" t="s">
         <v>58</v>
       </c>
-      <c r="J64" s="55"/>
-      <c r="K64" s="10"/>
-      <c r="L64" s="88"/>
-      <c r="M64" s="50" t="s">
+      <c r="J65" s="54"/>
+      <c r="K65" s="10"/>
+      <c r="L65" s="87"/>
+      <c r="M65" s="87"/>
+      <c r="N65" s="49" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B65" s="22">
-        <f>B61+1</f>
-        <v>24</v>
-      </c>
-      <c r="C65" s="5"/>
-      <c r="D65" s="9"/>
-      <c r="E65" s="9"/>
-      <c r="F65" s="9"/>
-      <c r="G65" s="53" t="s">
+    <row r="66" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B66" s="22">
+        <f>B62+1</f>
+        <v>38</v>
+      </c>
+      <c r="C66" s="5"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="H65" s="54"/>
-      <c r="I65" s="55" t="s">
+      <c r="H66" s="53"/>
+      <c r="I66" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="J65" s="56"/>
-      <c r="K65" s="4"/>
-      <c r="L65" s="103"/>
-      <c r="M65" s="50"/>
-    </row>
-    <row r="66" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B66" s="22">
-        <f t="shared" ref="B66:B76" si="2">B65+1</f>
-        <v>25</v>
-      </c>
-      <c r="C66" s="57"/>
-      <c r="D66" s="58"/>
-      <c r="E66" s="58"/>
-      <c r="F66" s="58"/>
-      <c r="G66" s="53" t="s">
+      <c r="J66" s="55"/>
+      <c r="K66" s="4"/>
+      <c r="L66" s="102"/>
+      <c r="M66" s="102"/>
+      <c r="N66" s="49"/>
+    </row>
+    <row r="67" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B67" s="22">
+        <f t="shared" ref="B67:B77" si="2">B66+1</f>
+        <v>39</v>
+      </c>
+      <c r="C67" s="56"/>
+      <c r="D67" s="57"/>
+      <c r="E67" s="57"/>
+      <c r="F67" s="57"/>
+      <c r="G67" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="H66" s="54"/>
-      <c r="I66" s="51"/>
-      <c r="J66" s="52"/>
-      <c r="K66" s="4"/>
-      <c r="L66" s="103"/>
-      <c r="M66" s="50"/>
-    </row>
-    <row r="67" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B67" s="22">
-        <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-      <c r="C67" s="5"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="9"/>
-      <c r="F67" s="9"/>
-      <c r="G67" s="9"/>
-      <c r="H67" s="6"/>
-      <c r="I67" s="51"/>
-      <c r="J67" s="52"/>
+      <c r="H67" s="53"/>
+      <c r="I67" s="50"/>
+      <c r="J67" s="51"/>
       <c r="K67" s="4"/>
-      <c r="L67" s="103"/>
-      <c r="M67" s="50"/>
-    </row>
-    <row r="68" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L67" s="102"/>
+      <c r="M67" s="102"/>
+      <c r="N67" s="49"/>
+    </row>
+    <row r="68" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B68" s="22">
         <f t="shared" si="2"/>
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="9"/>
@@ -2545,16 +2746,17 @@
       <c r="F68" s="9"/>
       <c r="G68" s="9"/>
       <c r="H68" s="6"/>
-      <c r="I68" s="51"/>
-      <c r="J68" s="52"/>
+      <c r="I68" s="50"/>
+      <c r="J68" s="51"/>
       <c r="K68" s="4"/>
-      <c r="L68" s="103"/>
-      <c r="M68" s="50"/>
-    </row>
-    <row r="69" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L68" s="102"/>
+      <c r="M68" s="102"/>
+      <c r="N68" s="49"/>
+    </row>
+    <row r="69" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B69" s="22">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="9"/>
@@ -2562,16 +2764,17 @@
       <c r="F69" s="9"/>
       <c r="G69" s="9"/>
       <c r="H69" s="6"/>
-      <c r="I69" s="51"/>
-      <c r="J69" s="52"/>
+      <c r="I69" s="50"/>
+      <c r="J69" s="51"/>
       <c r="K69" s="4"/>
-      <c r="L69" s="103"/>
-      <c r="M69" s="50"/>
-    </row>
-    <row r="70" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L69" s="102"/>
+      <c r="M69" s="102"/>
+      <c r="N69" s="49"/>
+    </row>
+    <row r="70" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B70" s="22">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="9"/>
@@ -2579,16 +2782,17 @@
       <c r="F70" s="9"/>
       <c r="G70" s="9"/>
       <c r="H70" s="6"/>
-      <c r="I70" s="51"/>
-      <c r="J70" s="52"/>
+      <c r="I70" s="50"/>
+      <c r="J70" s="51"/>
       <c r="K70" s="4"/>
-      <c r="L70" s="103"/>
-      <c r="M70" s="50"/>
-    </row>
-    <row r="71" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L70" s="102"/>
+      <c r="M70" s="102"/>
+      <c r="N70" s="49"/>
+    </row>
+    <row r="71" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B71" s="22">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C71" s="5"/>
       <c r="D71" s="9"/>
@@ -2596,16 +2800,17 @@
       <c r="F71" s="9"/>
       <c r="G71" s="9"/>
       <c r="H71" s="6"/>
-      <c r="I71" s="51"/>
-      <c r="J71" s="52"/>
+      <c r="I71" s="50"/>
+      <c r="J71" s="51"/>
       <c r="K71" s="4"/>
-      <c r="L71" s="103"/>
-      <c r="M71" s="50"/>
-    </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L71" s="102"/>
+      <c r="M71" s="102"/>
+      <c r="N71" s="49"/>
+    </row>
+    <row r="72" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B72" s="22">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="9"/>
@@ -2613,16 +2818,17 @@
       <c r="F72" s="9"/>
       <c r="G72" s="9"/>
       <c r="H72" s="6"/>
-      <c r="I72" s="51"/>
-      <c r="J72" s="52"/>
+      <c r="I72" s="50"/>
+      <c r="J72" s="51"/>
       <c r="K72" s="4"/>
-      <c r="L72" s="103"/>
-      <c r="M72" s="50"/>
-    </row>
-    <row r="73" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L72" s="102"/>
+      <c r="M72" s="102"/>
+      <c r="N72" s="49"/>
+    </row>
+    <row r="73" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B73" s="22">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C73" s="5"/>
       <c r="D73" s="9"/>
@@ -2630,16 +2836,17 @@
       <c r="F73" s="9"/>
       <c r="G73" s="9"/>
       <c r="H73" s="6"/>
-      <c r="I73" s="51"/>
-      <c r="J73" s="52"/>
+      <c r="I73" s="50"/>
+      <c r="J73" s="51"/>
       <c r="K73" s="4"/>
-      <c r="L73" s="103"/>
-      <c r="M73" s="50"/>
-    </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L73" s="102"/>
+      <c r="M73" s="102"/>
+      <c r="N73" s="49"/>
+    </row>
+    <row r="74" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B74" s="22">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="9"/>
@@ -2647,16 +2854,17 @@
       <c r="F74" s="9"/>
       <c r="G74" s="9"/>
       <c r="H74" s="6"/>
-      <c r="I74" s="51"/>
-      <c r="J74" s="52"/>
+      <c r="I74" s="50"/>
+      <c r="J74" s="51"/>
       <c r="K74" s="4"/>
-      <c r="L74" s="103"/>
-      <c r="M74" s="50"/>
-    </row>
-    <row r="75" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L74" s="102"/>
+      <c r="M74" s="102"/>
+      <c r="N74" s="49"/>
+    </row>
+    <row r="75" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B75" s="22">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="C75" s="5"/>
       <c r="D75" s="9"/>
@@ -2664,16 +2872,17 @@
       <c r="F75" s="9"/>
       <c r="G75" s="9"/>
       <c r="H75" s="6"/>
-      <c r="I75" s="51"/>
-      <c r="J75" s="52"/>
+      <c r="I75" s="50"/>
+      <c r="J75" s="51"/>
       <c r="K75" s="4"/>
-      <c r="L75" s="103"/>
-      <c r="M75" s="50"/>
-    </row>
-    <row r="76" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L75" s="102"/>
+      <c r="M75" s="102"/>
+      <c r="N75" s="49"/>
+    </row>
+    <row r="76" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B76" s="22">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="9"/>
@@ -2681,117 +2890,135 @@
       <c r="F76" s="9"/>
       <c r="G76" s="9"/>
       <c r="H76" s="6"/>
-      <c r="I76" s="51"/>
-      <c r="J76" s="52"/>
+      <c r="I76" s="50"/>
+      <c r="J76" s="51"/>
       <c r="K76" s="4"/>
-      <c r="L76" s="103"/>
-      <c r="M76" s="50"/>
+      <c r="L76" s="102"/>
+      <c r="M76" s="102"/>
+      <c r="N76" s="49"/>
+    </row>
+    <row r="77" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B77" s="22">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="C77" s="5"/>
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="9"/>
+      <c r="G77" s="9"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="50"/>
+      <c r="J77" s="51"/>
+      <c r="K77" s="4"/>
+      <c r="L77" s="102"/>
+      <c r="M77" s="102"/>
+      <c r="N77" s="49"/>
     </row>
   </sheetData>
-  <mergeCells count="103">
+  <mergeCells count="102">
     <mergeCell ref="B4:E4"/>
+    <mergeCell ref="M10:M13"/>
+    <mergeCell ref="B17:N17"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I16:J16"/>
-    <mergeCell ref="M10:M13"/>
+    <mergeCell ref="N10:N13"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="I74:J74"/>
     <mergeCell ref="I75:J75"/>
     <mergeCell ref="I76:J76"/>
+    <mergeCell ref="I77:J77"/>
     <mergeCell ref="C7:H7"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="D8:H8"/>
     <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I68:J68"/>
+    <mergeCell ref="I22:J22"/>
     <mergeCell ref="I69:J69"/>
     <mergeCell ref="I70:J70"/>
     <mergeCell ref="I71:J71"/>
     <mergeCell ref="I72:J72"/>
     <mergeCell ref="I73:J73"/>
-    <mergeCell ref="G65:H65"/>
-    <mergeCell ref="I65:J65"/>
-    <mergeCell ref="C66:F66"/>
+    <mergeCell ref="I74:J74"/>
     <mergeCell ref="G66:H66"/>
     <mergeCell ref="I66:J66"/>
+    <mergeCell ref="C67:F67"/>
+    <mergeCell ref="G67:H67"/>
     <mergeCell ref="I67:J67"/>
-    <mergeCell ref="B61:B64"/>
-    <mergeCell ref="C61:E64"/>
-    <mergeCell ref="F61:H64"/>
-    <mergeCell ref="I61:J61"/>
+    <mergeCell ref="I68:J68"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="C62:E65"/>
+    <mergeCell ref="F62:H65"/>
     <mergeCell ref="I62:J62"/>
     <mergeCell ref="I63:J63"/>
     <mergeCell ref="I64:J64"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="B56:B60"/>
-    <mergeCell ref="C56:D60"/>
-    <mergeCell ref="E56:H60"/>
+    <mergeCell ref="I65:J65"/>
+    <mergeCell ref="F56:H56"/>
     <mergeCell ref="I56:J56"/>
+    <mergeCell ref="B57:B61"/>
+    <mergeCell ref="C57:D61"/>
+    <mergeCell ref="E57:H61"/>
     <mergeCell ref="I57:J57"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="I59:J59"/>
     <mergeCell ref="I60:J60"/>
-    <mergeCell ref="B51:B54"/>
-    <mergeCell ref="C51:D54"/>
-    <mergeCell ref="E51:H54"/>
-    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="I61:J61"/>
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="C52:D55"/>
+    <mergeCell ref="E52:H55"/>
     <mergeCell ref="I52:J52"/>
     <mergeCell ref="I53:J53"/>
     <mergeCell ref="I54:J54"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:H49"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="D49:H50"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="D51:H51"/>
+    <mergeCell ref="I51:N51"/>
+    <mergeCell ref="B43:B47"/>
+    <mergeCell ref="C43:E47"/>
+    <mergeCell ref="F43:H47"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="I44:N44"/>
+    <mergeCell ref="C48:H48"/>
     <mergeCell ref="I48:J48"/>
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="D50:H50"/>
-    <mergeCell ref="I50:M50"/>
-    <mergeCell ref="B42:B46"/>
-    <mergeCell ref="C42:E46"/>
-    <mergeCell ref="F42:H46"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:E42"/>
+    <mergeCell ref="F41:H42"/>
+    <mergeCell ref="I41:J41"/>
     <mergeCell ref="I42:J42"/>
-    <mergeCell ref="I43:M43"/>
-    <mergeCell ref="C47:H47"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:H37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:E39"/>
+    <mergeCell ref="F38:H39"/>
+    <mergeCell ref="I38:J38"/>
     <mergeCell ref="I39:J39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:E41"/>
-    <mergeCell ref="F40:H41"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:H36"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:E38"/>
-    <mergeCell ref="F37:H38"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="E31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="C32:E36"/>
+    <mergeCell ref="F32:H36"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:N33"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:H27"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="D28:H30"/>
+    <mergeCell ref="I28:J28"/>
     <mergeCell ref="I29:J29"/>
-    <mergeCell ref="E30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="B31:B35"/>
-    <mergeCell ref="C31:E35"/>
-    <mergeCell ref="F31:H35"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="I32:M32"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:H26"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="C24:H25"/>
+    <mergeCell ref="I24:J24"/>
     <mergeCell ref="I25:J25"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="D27:H29"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="C23:H24"/>
     <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="D21:H21"/>
+    <mergeCell ref="D22:H22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2857,18 +3084,18 @@
       <c r="B5" s="11">
         <v>1</v>
       </c>
-      <c r="C5" s="84" t="s">
+      <c r="C5" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="74" t="s">
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="55"/>
+      <c r="J5" s="54"/>
       <c r="K5" s="4" t="s">
         <v>6</v>
       </c>
@@ -2879,14 +3106,14 @@
         <f>B5+1</f>
         <v>2</v>
       </c>
-      <c r="C6" s="84" t="s">
+      <c r="C6" s="83" t="s">
         <v>86</v>
       </c>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="54"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="53"/>
       <c r="I6" s="23"/>
       <c r="J6" s="24"/>
       <c r="K6" s="10" t="s">
@@ -2895,22 +3122,22 @@
       <c r="L6" s="4"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="59">
+      <c r="B7" s="58">
         <f>B6+1</f>
         <v>3</v>
       </c>
-      <c r="C7" s="76" t="s">
+      <c r="C7" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="68"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="68"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="74" t="s">
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="55"/>
+      <c r="J7" s="54"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="N7" s="20" t="s">
@@ -2918,17 +3145,17 @@
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="61"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="73"/>
-      <c r="I8" s="74" t="s">
+      <c r="B8" s="60"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="J8" s="55"/>
+      <c r="J8" s="54"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="N8" s="4" t="s">
@@ -2936,22 +3163,22 @@
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="59">
+      <c r="B9" s="58">
         <f>B7+1</f>
         <v>4</v>
       </c>
-      <c r="C9" s="62"/>
-      <c r="D9" s="68" t="s">
+      <c r="C9" s="61"/>
+      <c r="D9" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="68"/>
-      <c r="F9" s="68"/>
-      <c r="G9" s="68"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="74" t="s">
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="55"/>
+      <c r="J9" s="54"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="N9" s="10" t="s">
@@ -2959,67 +3186,67 @@
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="61"/>
-      <c r="C10" s="66"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="72"/>
-      <c r="G10" s="72"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="74" t="s">
+      <c r="B10" s="60"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="72"/>
+      <c r="I10" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="J10" s="55"/>
+      <c r="J10" s="54"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="59">
+      <c r="B11" s="58">
         <f>B9+1</f>
         <v>5</v>
       </c>
-      <c r="C11" s="62"/>
-      <c r="D11" s="68" t="s">
+      <c r="C11" s="61"/>
+      <c r="D11" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="68"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="68"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="74" t="s">
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="55"/>
+      <c r="J11" s="54"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="60"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="70"/>
-      <c r="G12" s="70"/>
-      <c r="H12" s="71"/>
-      <c r="I12" s="74" t="s">
+      <c r="B12" s="59"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="70"/>
+      <c r="I12" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="J12" s="55"/>
+      <c r="J12" s="54"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="61"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="73"/>
-      <c r="I13" s="74" t="s">
+      <c r="B13" s="60"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="71"/>
+      <c r="H13" s="72"/>
+      <c r="I13" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="J13" s="55"/>
+      <c r="J13" s="54"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
     </row>
@@ -3030,62 +3257,62 @@
       </c>
       <c r="C14" s="26"/>
       <c r="D14" s="25"/>
-      <c r="E14" s="53" t="s">
+      <c r="E14" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="74" t="s">
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="73" t="s">
         <v>57</v>
       </c>
-      <c r="J14" s="55"/>
+      <c r="J14" s="54"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="59">
+      <c r="B15" s="58">
         <f>B14+1</f>
         <v>7</v>
       </c>
-      <c r="C15" s="62"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="68" t="s">
+      <c r="C15" s="61"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="68"/>
-      <c r="H15" s="69"/>
-      <c r="I15" s="74" t="s">
+      <c r="G15" s="67"/>
+      <c r="H15" s="68"/>
+      <c r="I15" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="J15" s="55"/>
+      <c r="J15" s="54"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="60"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="70"/>
-      <c r="G16" s="70"/>
-      <c r="H16" s="71"/>
-      <c r="I16" s="74" t="s">
+      <c r="B16" s="59"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="J16" s="79"/>
-      <c r="K16" s="79"/>
-      <c r="L16" s="79"/>
+      <c r="J16" s="78"/>
+      <c r="K16" s="78"/>
+      <c r="L16" s="78"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="60"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="70"/>
-      <c r="G17" s="70"/>
-      <c r="H17" s="71"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="69"/>
+      <c r="H17" s="70"/>
       <c r="I17" s="7"/>
       <c r="J17" s="8" t="s">
         <v>32</v>
@@ -3094,13 +3321,13 @@
       <c r="L17" s="4"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="60"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="65"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="70"/>
-      <c r="G18" s="70"/>
-      <c r="H18" s="71"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="63"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="70"/>
       <c r="I18" s="7"/>
       <c r="J18" s="8" t="s">
         <v>34</v>
@@ -3109,13 +3336,13 @@
       <c r="L18" s="4"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="61"/>
-      <c r="C19" s="66"/>
-      <c r="D19" s="67"/>
-      <c r="E19" s="67"/>
-      <c r="F19" s="72"/>
-      <c r="G19" s="72"/>
-      <c r="H19" s="73"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="72"/>
       <c r="I19" s="7"/>
       <c r="J19" s="8" t="s">
         <v>35</v>
@@ -3130,53 +3357,53 @@
         <f>B15+1</f>
         <v>8</v>
       </c>
-      <c r="C20" s="57"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="53" t="s">
+      <c r="C20" s="56"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="54"/>
-      <c r="I20" s="74" t="s">
+      <c r="F20" s="52"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="J20" s="55"/>
+      <c r="J20" s="54"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="59">
+      <c r="B21" s="58">
         <f>B20+1</f>
         <v>9</v>
       </c>
-      <c r="C21" s="62"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="68" t="s">
+      <c r="C21" s="61"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="68"/>
-      <c r="H21" s="69"/>
-      <c r="I21" s="74" t="s">
+      <c r="G21" s="67"/>
+      <c r="H21" s="68"/>
+      <c r="I21" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="J21" s="55"/>
+      <c r="J21" s="54"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="61"/>
-      <c r="C22" s="66"/>
-      <c r="D22" s="67"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="72"/>
-      <c r="H22" s="73"/>
-      <c r="I22" s="74" t="s">
+      <c r="B22" s="60"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="72"/>
+      <c r="I22" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="J22" s="55"/>
+      <c r="J22" s="54"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
     </row>
@@ -3188,96 +3415,96 @@
       <c r="C23" s="5"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
-      <c r="F23" s="53" t="s">
+      <c r="F23" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="G23" s="53"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="74" t="s">
+      <c r="G23" s="52"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="J23" s="55"/>
+      <c r="J23" s="54"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="59">
+      <c r="B24" s="58">
         <f t="shared" ref="B24:B40" si="0">B23+1</f>
         <v>11</v>
       </c>
-      <c r="C24" s="62"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="63"/>
-      <c r="F24" s="68" t="s">
+      <c r="C24" s="61"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="G24" s="68"/>
-      <c r="H24" s="69"/>
-      <c r="I24" s="82" t="s">
+      <c r="G24" s="67"/>
+      <c r="H24" s="68"/>
+      <c r="I24" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="J24" s="83"/>
+      <c r="J24" s="82"/>
       <c r="K24" s="18"/>
       <c r="L24" s="18"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="61"/>
-      <c r="C25" s="66"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="67"/>
-      <c r="F25" s="72"/>
-      <c r="G25" s="72"/>
-      <c r="H25" s="73"/>
-      <c r="I25" s="74" t="s">
+      <c r="B25" s="60"/>
+      <c r="C25" s="65"/>
+      <c r="D25" s="66"/>
+      <c r="E25" s="66"/>
+      <c r="F25" s="71"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="J25" s="55"/>
+      <c r="J25" s="54"/>
       <c r="K25" s="18"/>
       <c r="L25" s="18"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="59">
+      <c r="B26" s="58">
         <f>B24+1</f>
         <v>12</v>
       </c>
-      <c r="C26" s="76"/>
-      <c r="D26" s="68"/>
-      <c r="E26" s="68"/>
-      <c r="F26" s="68" t="s">
+      <c r="C26" s="75"/>
+      <c r="D26" s="67"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="G26" s="68"/>
-      <c r="H26" s="69"/>
-      <c r="I26" s="74" t="s">
+      <c r="G26" s="67"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="J26" s="55"/>
+      <c r="J26" s="54"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="60"/>
-      <c r="C27" s="77"/>
-      <c r="D27" s="70"/>
-      <c r="E27" s="70"/>
-      <c r="F27" s="70"/>
-      <c r="G27" s="70"/>
-      <c r="H27" s="71"/>
-      <c r="I27" s="74" t="s">
+      <c r="B27" s="59"/>
+      <c r="C27" s="76"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="69"/>
+      <c r="G27" s="69"/>
+      <c r="H27" s="70"/>
+      <c r="I27" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="J27" s="79"/>
-      <c r="K27" s="79"/>
-      <c r="L27" s="79"/>
+      <c r="J27" s="78"/>
+      <c r="K27" s="78"/>
+      <c r="L27" s="78"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="60"/>
-      <c r="C28" s="77"/>
-      <c r="D28" s="70"/>
-      <c r="E28" s="70"/>
-      <c r="F28" s="70"/>
-      <c r="G28" s="70"/>
-      <c r="H28" s="71"/>
+      <c r="B28" s="59"/>
+      <c r="C28" s="76"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="69"/>
+      <c r="G28" s="69"/>
+      <c r="H28" s="70"/>
       <c r="I28" s="7"/>
       <c r="J28" s="8" t="s">
         <v>32</v>
@@ -3286,13 +3513,13 @@
       <c r="L28" s="4"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="60"/>
-      <c r="C29" s="77"/>
-      <c r="D29" s="70"/>
-      <c r="E29" s="70"/>
-      <c r="F29" s="70"/>
-      <c r="G29" s="70"/>
-      <c r="H29" s="71"/>
+      <c r="B29" s="59"/>
+      <c r="C29" s="76"/>
+      <c r="D29" s="69"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="69"/>
+      <c r="G29" s="69"/>
+      <c r="H29" s="70"/>
       <c r="I29" s="7"/>
       <c r="J29" s="8" t="s">
         <v>34</v>
@@ -3301,13 +3528,13 @@
       <c r="L29" s="4"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B30" s="61"/>
-      <c r="C30" s="78"/>
-      <c r="D30" s="72"/>
-      <c r="E30" s="72"/>
-      <c r="F30" s="72"/>
-      <c r="G30" s="72"/>
-      <c r="H30" s="73"/>
+      <c r="B30" s="60"/>
+      <c r="C30" s="77"/>
+      <c r="D30" s="71"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="72"/>
       <c r="I30" s="7"/>
       <c r="J30" s="8" t="s">
         <v>35</v>
@@ -3322,53 +3549,53 @@
         <f>B26+1</f>
         <v>13</v>
       </c>
-      <c r="C31" s="78" t="s">
+      <c r="C31" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="72"/>
-      <c r="E31" s="72"/>
-      <c r="F31" s="72"/>
-      <c r="G31" s="72"/>
-      <c r="H31" s="54"/>
-      <c r="I31" s="80" t="s">
+      <c r="D31" s="71"/>
+      <c r="E31" s="71"/>
+      <c r="F31" s="71"/>
+      <c r="G31" s="71"/>
+      <c r="H31" s="53"/>
+      <c r="I31" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="J31" s="81"/>
+      <c r="J31" s="80"/>
       <c r="K31" s="19"/>
       <c r="L31" s="19"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="59">
+      <c r="B32" s="58">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C32" s="62"/>
-      <c r="D32" s="68" t="s">
+      <c r="C32" s="61"/>
+      <c r="D32" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="E32" s="68"/>
-      <c r="F32" s="68"/>
-      <c r="G32" s="68"/>
-      <c r="H32" s="69"/>
-      <c r="I32" s="74" t="s">
+      <c r="E32" s="67"/>
+      <c r="F32" s="67"/>
+      <c r="G32" s="67"/>
+      <c r="H32" s="68"/>
+      <c r="I32" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="J32" s="55"/>
+      <c r="J32" s="54"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B33" s="61"/>
-      <c r="C33" s="66"/>
-      <c r="D33" s="72"/>
-      <c r="E33" s="72"/>
-      <c r="F33" s="72"/>
-      <c r="G33" s="72"/>
-      <c r="H33" s="73"/>
-      <c r="I33" s="74" t="s">
+      <c r="B33" s="60"/>
+      <c r="C33" s="65"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="71"/>
+      <c r="H33" s="72"/>
+      <c r="I33" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="J33" s="55"/>
+      <c r="J33" s="54"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
     </row>
@@ -3378,82 +3605,82 @@
         <v>15</v>
       </c>
       <c r="C34" s="5"/>
-      <c r="D34" s="53" t="s">
+      <c r="D34" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="53"/>
-      <c r="F34" s="53"/>
-      <c r="G34" s="53"/>
-      <c r="H34" s="54"/>
-      <c r="I34" s="51"/>
-      <c r="J34" s="75"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="75"/>
+      <c r="E34" s="52"/>
+      <c r="F34" s="52"/>
+      <c r="G34" s="52"/>
+      <c r="H34" s="53"/>
+      <c r="I34" s="50"/>
+      <c r="J34" s="74"/>
+      <c r="K34" s="74"/>
+      <c r="L34" s="74"/>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B35" s="59">
+      <c r="B35" s="58">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C35" s="62"/>
-      <c r="D35" s="63"/>
-      <c r="E35" s="68" t="s">
+      <c r="C35" s="61"/>
+      <c r="D35" s="62"/>
+      <c r="E35" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="F35" s="68"/>
-      <c r="G35" s="68"/>
-      <c r="H35" s="69"/>
-      <c r="I35" s="74" t="s">
+      <c r="F35" s="67"/>
+      <c r="G35" s="67"/>
+      <c r="H35" s="68"/>
+      <c r="I35" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="J35" s="55"/>
+      <c r="J35" s="54"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B36" s="60"/>
-      <c r="C36" s="64"/>
-      <c r="D36" s="65"/>
-      <c r="E36" s="70"/>
-      <c r="F36" s="70"/>
-      <c r="G36" s="70"/>
-      <c r="H36" s="71"/>
-      <c r="I36" s="74" t="s">
+      <c r="B36" s="59"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="64"/>
+      <c r="E36" s="69"/>
+      <c r="F36" s="69"/>
+      <c r="G36" s="69"/>
+      <c r="H36" s="70"/>
+      <c r="I36" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="J36" s="55"/>
+      <c r="J36" s="54"/>
       <c r="K36" s="20"/>
       <c r="L36" s="21" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B37" s="60"/>
-      <c r="C37" s="64"/>
-      <c r="D37" s="65"/>
-      <c r="E37" s="70"/>
-      <c r="F37" s="70"/>
-      <c r="G37" s="70"/>
-      <c r="H37" s="71"/>
-      <c r="I37" s="74" t="s">
+      <c r="B37" s="59"/>
+      <c r="C37" s="63"/>
+      <c r="D37" s="64"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="69"/>
+      <c r="G37" s="69"/>
+      <c r="H37" s="70"/>
+      <c r="I37" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="J37" s="55"/>
+      <c r="J37" s="54"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B38" s="61"/>
-      <c r="C38" s="66"/>
-      <c r="D38" s="67"/>
-      <c r="E38" s="72"/>
-      <c r="F38" s="72"/>
-      <c r="G38" s="72"/>
-      <c r="H38" s="73"/>
-      <c r="I38" s="74" t="s">
+      <c r="B38" s="60"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="66"/>
+      <c r="E38" s="71"/>
+      <c r="F38" s="71"/>
+      <c r="G38" s="71"/>
+      <c r="H38" s="72"/>
+      <c r="I38" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="J38" s="55"/>
+      <c r="J38" s="54"/>
       <c r="K38" s="20"/>
       <c r="L38" s="21" t="s">
         <v>29</v>
@@ -3467,160 +3694,160 @@
       <c r="C39" s="5"/>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
-      <c r="F39" s="53" t="s">
+      <c r="F39" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="G39" s="53"/>
-      <c r="H39" s="54"/>
-      <c r="I39" s="74" t="s">
+      <c r="G39" s="52"/>
+      <c r="H39" s="53"/>
+      <c r="I39" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="J39" s="55"/>
+      <c r="J39" s="54"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B40" s="59">
+      <c r="B40" s="58">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C40" s="62"/>
-      <c r="D40" s="63"/>
-      <c r="E40" s="68" t="s">
+      <c r="C40" s="61"/>
+      <c r="D40" s="62"/>
+      <c r="E40" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="F40" s="68"/>
-      <c r="G40" s="68"/>
-      <c r="H40" s="69"/>
-      <c r="I40" s="74" t="s">
+      <c r="F40" s="67"/>
+      <c r="G40" s="67"/>
+      <c r="H40" s="68"/>
+      <c r="I40" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="J40" s="55"/>
+      <c r="J40" s="54"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B41" s="60"/>
-      <c r="C41" s="64"/>
-      <c r="D41" s="65"/>
-      <c r="E41" s="70"/>
-      <c r="F41" s="70"/>
-      <c r="G41" s="70"/>
-      <c r="H41" s="71"/>
-      <c r="I41" s="74" t="s">
+      <c r="B41" s="59"/>
+      <c r="C41" s="63"/>
+      <c r="D41" s="64"/>
+      <c r="E41" s="69"/>
+      <c r="F41" s="69"/>
+      <c r="G41" s="69"/>
+      <c r="H41" s="70"/>
+      <c r="I41" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="J41" s="55"/>
+      <c r="J41" s="54"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B42" s="60"/>
-      <c r="C42" s="64"/>
-      <c r="D42" s="65"/>
-      <c r="E42" s="70"/>
-      <c r="F42" s="70"/>
-      <c r="G42" s="70"/>
-      <c r="H42" s="71"/>
-      <c r="I42" s="74" t="s">
+      <c r="B42" s="59"/>
+      <c r="C42" s="63"/>
+      <c r="D42" s="64"/>
+      <c r="E42" s="69"/>
+      <c r="F42" s="69"/>
+      <c r="G42" s="69"/>
+      <c r="H42" s="70"/>
+      <c r="I42" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="J42" s="55"/>
+      <c r="J42" s="54"/>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B43" s="60"/>
-      <c r="C43" s="64"/>
-      <c r="D43" s="65"/>
-      <c r="E43" s="70"/>
-      <c r="F43" s="70"/>
-      <c r="G43" s="70"/>
-      <c r="H43" s="71"/>
-      <c r="I43" s="74" t="s">
+      <c r="B43" s="59"/>
+      <c r="C43" s="63"/>
+      <c r="D43" s="64"/>
+      <c r="E43" s="69"/>
+      <c r="F43" s="69"/>
+      <c r="G43" s="69"/>
+      <c r="H43" s="70"/>
+      <c r="I43" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="J43" s="55"/>
+      <c r="J43" s="54"/>
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B44" s="61"/>
-      <c r="C44" s="64"/>
-      <c r="D44" s="65"/>
-      <c r="E44" s="70"/>
-      <c r="F44" s="70"/>
-      <c r="G44" s="70"/>
-      <c r="H44" s="71"/>
-      <c r="I44" s="74" t="s">
+      <c r="B44" s="60"/>
+      <c r="C44" s="63"/>
+      <c r="D44" s="64"/>
+      <c r="E44" s="69"/>
+      <c r="F44" s="69"/>
+      <c r="G44" s="69"/>
+      <c r="H44" s="70"/>
+      <c r="I44" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="J44" s="55"/>
+      <c r="J44" s="54"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B45" s="59">
+      <c r="B45" s="58">
         <f>B40+1</f>
         <v>19</v>
       </c>
-      <c r="C45" s="62"/>
-      <c r="D45" s="63"/>
-      <c r="E45" s="63"/>
-      <c r="F45" s="68" t="s">
+      <c r="C45" s="61"/>
+      <c r="D45" s="62"/>
+      <c r="E45" s="62"/>
+      <c r="F45" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="G45" s="68"/>
-      <c r="H45" s="69"/>
-      <c r="I45" s="55" t="s">
+      <c r="G45" s="67"/>
+      <c r="H45" s="68"/>
+      <c r="I45" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="J45" s="56"/>
+      <c r="J45" s="55"/>
       <c r="K45" s="4"/>
       <c r="L45" s="4"/>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B46" s="60"/>
-      <c r="C46" s="64"/>
-      <c r="D46" s="65"/>
-      <c r="E46" s="65"/>
-      <c r="F46" s="70"/>
-      <c r="G46" s="70"/>
-      <c r="H46" s="71"/>
-      <c r="I46" s="74" t="s">
+      <c r="B46" s="59"/>
+      <c r="C46" s="63"/>
+      <c r="D46" s="64"/>
+      <c r="E46" s="64"/>
+      <c r="F46" s="69"/>
+      <c r="G46" s="69"/>
+      <c r="H46" s="70"/>
+      <c r="I46" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="J46" s="55"/>
+      <c r="J46" s="54"/>
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B47" s="60"/>
-      <c r="C47" s="64"/>
-      <c r="D47" s="65"/>
-      <c r="E47" s="65"/>
-      <c r="F47" s="70"/>
-      <c r="G47" s="70"/>
-      <c r="H47" s="71"/>
-      <c r="I47" s="74" t="s">
+      <c r="B47" s="59"/>
+      <c r="C47" s="63"/>
+      <c r="D47" s="64"/>
+      <c r="E47" s="64"/>
+      <c r="F47" s="69"/>
+      <c r="G47" s="69"/>
+      <c r="H47" s="70"/>
+      <c r="I47" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="J47" s="55"/>
+      <c r="J47" s="54"/>
       <c r="K47" s="4"/>
       <c r="L47" s="4"/>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B48" s="61"/>
-      <c r="C48" s="66"/>
-      <c r="D48" s="67"/>
-      <c r="E48" s="67"/>
-      <c r="F48" s="72"/>
-      <c r="G48" s="72"/>
-      <c r="H48" s="73"/>
-      <c r="I48" s="74" t="s">
+      <c r="B48" s="60"/>
+      <c r="C48" s="65"/>
+      <c r="D48" s="66"/>
+      <c r="E48" s="66"/>
+      <c r="F48" s="71"/>
+      <c r="G48" s="71"/>
+      <c r="H48" s="72"/>
+      <c r="I48" s="73" t="s">
         <v>58</v>
       </c>
-      <c r="J48" s="55"/>
+      <c r="J48" s="54"/>
       <c r="K48" s="10"/>
       <c r="L48" s="4" t="s">
         <v>59</v>
@@ -3635,14 +3862,14 @@
       <c r="D49" s="9"/>
       <c r="E49" s="9"/>
       <c r="F49" s="9"/>
-      <c r="G49" s="53" t="s">
+      <c r="G49" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="H49" s="54"/>
-      <c r="I49" s="55" t="s">
+      <c r="H49" s="53"/>
+      <c r="I49" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="J49" s="56"/>
+      <c r="J49" s="55"/>
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
     </row>
@@ -3651,16 +3878,16 @@
         <f t="shared" ref="B50:B60" si="1">B49+1</f>
         <v>21</v>
       </c>
-      <c r="C50" s="57"/>
-      <c r="D50" s="58"/>
-      <c r="E50" s="58"/>
-      <c r="F50" s="58"/>
-      <c r="G50" s="53" t="s">
+      <c r="C50" s="56"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="57"/>
+      <c r="F50" s="57"/>
+      <c r="G50" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="H50" s="54"/>
-      <c r="I50" s="51"/>
-      <c r="J50" s="52"/>
+      <c r="H50" s="53"/>
+      <c r="I50" s="50"/>
+      <c r="J50" s="51"/>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
     </row>
@@ -3675,8 +3902,8 @@
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
       <c r="H51" s="6"/>
-      <c r="I51" s="51"/>
-      <c r="J51" s="52"/>
+      <c r="I51" s="50"/>
+      <c r="J51" s="51"/>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
     </row>
@@ -3691,8 +3918,8 @@
       <c r="F52" s="9"/>
       <c r="G52" s="9"/>
       <c r="H52" s="6"/>
-      <c r="I52" s="51"/>
-      <c r="J52" s="52"/>
+      <c r="I52" s="50"/>
+      <c r="J52" s="51"/>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
     </row>
@@ -3707,8 +3934,8 @@
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
       <c r="H53" s="6"/>
-      <c r="I53" s="51"/>
-      <c r="J53" s="52"/>
+      <c r="I53" s="50"/>
+      <c r="J53" s="51"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
     </row>
@@ -3723,8 +3950,8 @@
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
       <c r="H54" s="6"/>
-      <c r="I54" s="51"/>
-      <c r="J54" s="52"/>
+      <c r="I54" s="50"/>
+      <c r="J54" s="51"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
     </row>
@@ -3739,8 +3966,8 @@
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
       <c r="H55" s="6"/>
-      <c r="I55" s="51"/>
-      <c r="J55" s="52"/>
+      <c r="I55" s="50"/>
+      <c r="J55" s="51"/>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
     </row>
@@ -3755,8 +3982,8 @@
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
       <c r="H56" s="6"/>
-      <c r="I56" s="51"/>
-      <c r="J56" s="52"/>
+      <c r="I56" s="50"/>
+      <c r="J56" s="51"/>
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
     </row>
@@ -3771,8 +3998,8 @@
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
       <c r="H57" s="6"/>
-      <c r="I57" s="51"/>
-      <c r="J57" s="52"/>
+      <c r="I57" s="50"/>
+      <c r="J57" s="51"/>
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
     </row>
@@ -3787,8 +4014,8 @@
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
       <c r="H58" s="6"/>
-      <c r="I58" s="51"/>
-      <c r="J58" s="52"/>
+      <c r="I58" s="50"/>
+      <c r="J58" s="51"/>
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
     </row>
@@ -3803,8 +4030,8 @@
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
       <c r="H59" s="6"/>
-      <c r="I59" s="51"/>
-      <c r="J59" s="52"/>
+      <c r="I59" s="50"/>
+      <c r="J59" s="51"/>
       <c r="K59" s="4"/>
       <c r="L59" s="4"/>
     </row>
@@ -3819,8 +4046,8 @@
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
       <c r="H60" s="6"/>
-      <c r="I60" s="51"/>
-      <c r="J60" s="52"/>
+      <c r="I60" s="50"/>
+      <c r="J60" s="51"/>
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
     </row>

</xml_diff>

<commit_message>
#6 - SQL errors cause server to crash
</commit_message>
<xml_diff>
--- a/documents/Testing Schedule.xlsx
+++ b/documents/Testing Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Node\Timelog\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF11C611-A5C1-40D3-86F1-87ACF8DD75E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7931E56-4955-4B58-83D8-B772A10EA8A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{9AAAF6DA-95E7-49F0-B7DD-46373E33B9E7}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="123">
   <si>
     <t>RMPC Timelog Testing Schedule</t>
   </si>
@@ -381,9 +381,6 @@
     <t>No error message transition</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>N - Failed</t>
   </si>
   <si>
@@ -393,22 +390,22 @@
     <t>Y - Pass / Fixed</t>
   </si>
   <si>
-    <t>Temporarily disabled until payments imposed</t>
-  </si>
-  <si>
     <t>Issue #</t>
   </si>
   <si>
     <t>#1</t>
   </si>
   <si>
-    <t>#2</t>
-  </si>
-  <si>
     <t>#3</t>
   </si>
   <si>
     <t>SHOWSTOPPER</t>
+  </si>
+  <si>
+    <t>Temporarily disabled pending end of Beta Promotion</t>
+  </si>
+  <si>
+    <t>#2 - #3</t>
   </si>
 </sst>
 </file>
@@ -967,18 +964,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1003,9 +994,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1050,6 +1038,15 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1374,7 +1371,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P27" sqref="P27"/>
+      <selection pane="bottomLeft" activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1386,48 +1383,48 @@
     <col min="9" max="9" width="11.42578125" style="2" customWidth="1"/>
     <col min="10" max="10" width="29.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="11.28515625" style="101" customWidth="1"/>
-    <col min="14" max="14" width="42.7109375" style="89" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="11.28515625" style="99" customWidth="1"/>
+    <col min="14" max="14" width="49.140625" style="89" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="99" t="s">
-        <v>117</v>
-      </c>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="P2" s="96"/>
+      <c r="B2" s="97" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="P2" s="94"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="118" t="s">
-        <v>116</v>
-      </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="116"/>
-      <c r="F3" s="117"/>
+      <c r="B3" s="115" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="113"/>
+      <c r="F3" s="114"/>
       <c r="H3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I3" s="1"/>
       <c r="L3" s="2"/>
-      <c r="N3" s="101"/>
+      <c r="N3" s="99"/>
       <c r="O3" s="89"/>
-      <c r="Q3" s="97"/>
+      <c r="Q3" s="95"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="100" t="s">
-        <v>115</v>
-      </c>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="100"/>
+      <c r="B4" s="98" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="P4" s="98"/>
+      <c r="P4" s="96"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
@@ -1452,7 +1449,7 @@
         <v>110</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="N6" s="17" t="s">
         <v>106</v>
@@ -1473,8 +1470,8 @@
       <c r="I7" s="73"/>
       <c r="J7" s="54"/>
       <c r="K7" s="4"/>
-      <c r="L7" s="102"/>
-      <c r="M7" s="102"/>
+      <c r="L7" s="100"/>
+      <c r="M7" s="100"/>
       <c r="N7" s="49"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
@@ -1519,8 +1516,8 @@
       <c r="I9" s="45"/>
       <c r="J9" s="46"/>
       <c r="K9" s="4"/>
-      <c r="L9" s="102"/>
-      <c r="M9" s="102"/>
+      <c r="L9" s="100"/>
+      <c r="M9" s="100"/>
       <c r="N9" s="49"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
@@ -1543,13 +1540,13 @@
       <c r="K10" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="L10" s="114" t="s">
+      <c r="L10" s="111" t="s">
         <v>70</v>
       </c>
-      <c r="M10" s="111" t="s">
-        <v>122</v>
-      </c>
-      <c r="N10" s="90" t="s">
+      <c r="M10" s="108" t="s">
+        <v>119</v>
+      </c>
+      <c r="N10" s="116" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1573,11 +1570,11 @@
       <c r="K11" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="L11" s="114" t="s">
+      <c r="L11" s="111" t="s">
         <v>70</v>
       </c>
-      <c r="M11" s="112"/>
-      <c r="N11" s="91"/>
+      <c r="M11" s="109"/>
+      <c r="N11" s="117"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="11">
@@ -1599,11 +1596,11 @@
       <c r="K12" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="L12" s="114" t="s">
+      <c r="L12" s="111" t="s">
         <v>70</v>
       </c>
-      <c r="M12" s="112"/>
-      <c r="N12" s="91"/>
+      <c r="M12" s="109"/>
+      <c r="N12" s="117"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="11">
@@ -1625,11 +1622,11 @@
       <c r="K13" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="L13" s="114" t="s">
+      <c r="L13" s="111" t="s">
         <v>70</v>
       </c>
-      <c r="M13" s="113"/>
-      <c r="N13" s="92"/>
+      <c r="M13" s="110"/>
+      <c r="N13" s="117"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" s="11">
@@ -1651,13 +1648,13 @@
       <c r="K14" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="L14" s="103" t="s">
-        <v>114</v>
-      </c>
-      <c r="M14" s="103" t="s">
-        <v>121</v>
-      </c>
-      <c r="N14" s="49"/>
+      <c r="L14" s="111" t="s">
+        <v>70</v>
+      </c>
+      <c r="M14" s="111" t="s">
+        <v>122</v>
+      </c>
+      <c r="N14" s="117"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" s="11">
@@ -1679,15 +1676,13 @@
       <c r="K15" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="L15" s="114" t="s">
+      <c r="L15" s="111" t="s">
         <v>70</v>
       </c>
-      <c r="M15" s="114" t="s">
-        <v>122</v>
-      </c>
-      <c r="N15" s="49" t="s">
-        <v>113</v>
-      </c>
+      <c r="M15" s="111" t="s">
+        <v>119</v>
+      </c>
+      <c r="N15" s="118"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="11">
@@ -1713,28 +1708,28 @@
         <v>70</v>
       </c>
       <c r="M16" s="88" t="s">
+        <v>118</v>
+      </c>
+      <c r="N16" s="49" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="105" t="s">
         <v>120</v>
       </c>
-      <c r="N16" s="49" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="108" t="s">
-        <v>123</v>
-      </c>
-      <c r="C17" s="109"/>
-      <c r="D17" s="109"/>
-      <c r="E17" s="109"/>
-      <c r="F17" s="109"/>
-      <c r="G17" s="109"/>
-      <c r="H17" s="109"/>
-      <c r="I17" s="109"/>
-      <c r="J17" s="109"/>
-      <c r="K17" s="109"/>
-      <c r="L17" s="109"/>
-      <c r="M17" s="109"/>
-      <c r="N17" s="110"/>
+      <c r="C17" s="106"/>
+      <c r="D17" s="106"/>
+      <c r="E17" s="106"/>
+      <c r="F17" s="106"/>
+      <c r="G17" s="106"/>
+      <c r="H17" s="106"/>
+      <c r="I17" s="106"/>
+      <c r="J17" s="106"/>
+      <c r="K17" s="106"/>
+      <c r="L17" s="106"/>
+      <c r="M17" s="106"/>
+      <c r="N17" s="107"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="11">
@@ -1752,8 +1747,8 @@
       <c r="I18" s="45"/>
       <c r="J18" s="46"/>
       <c r="K18" s="4"/>
-      <c r="L18" s="102"/>
-      <c r="M18" s="102"/>
+      <c r="L18" s="100"/>
+      <c r="M18" s="100"/>
       <c r="N18" s="49"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
@@ -1776,8 +1771,8 @@
       <c r="K19" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="L19" s="102"/>
-      <c r="M19" s="102"/>
+      <c r="L19" s="100"/>
+      <c r="M19" s="100"/>
       <c r="N19" s="49"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
@@ -1794,8 +1789,8 @@
       <c r="I20" s="45"/>
       <c r="J20" s="46"/>
       <c r="K20" s="4"/>
-      <c r="L20" s="102"/>
-      <c r="M20" s="102"/>
+      <c r="L20" s="100"/>
+      <c r="M20" s="100"/>
       <c r="N20" s="49"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
@@ -1814,8 +1809,8 @@
       <c r="I21" s="73"/>
       <c r="J21" s="54"/>
       <c r="K21" s="4"/>
-      <c r="L21" s="102"/>
-      <c r="M21" s="102"/>
+      <c r="L21" s="100"/>
+      <c r="M21" s="100"/>
       <c r="N21" s="49"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
@@ -1836,8 +1831,8 @@
       </c>
       <c r="J22" s="54"/>
       <c r="K22" s="4"/>
-      <c r="L22" s="102"/>
-      <c r="M22" s="102"/>
+      <c r="L22" s="100"/>
+      <c r="M22" s="100"/>
       <c r="N22" s="49"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
@@ -1858,8 +1853,8 @@
       </c>
       <c r="J23" s="54"/>
       <c r="K23" s="4"/>
-      <c r="L23" s="102"/>
-      <c r="M23" s="102"/>
+      <c r="L23" s="100"/>
+      <c r="M23" s="100"/>
       <c r="N23" s="49"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
@@ -1880,8 +1875,8 @@
       </c>
       <c r="J24" s="54"/>
       <c r="K24" s="4"/>
-      <c r="L24" s="102"/>
-      <c r="M24" s="102"/>
+      <c r="L24" s="100"/>
+      <c r="M24" s="100"/>
       <c r="N24" s="49"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
@@ -1900,8 +1895,8 @@
       </c>
       <c r="J25" s="54"/>
       <c r="K25" s="4"/>
-      <c r="L25" s="102"/>
-      <c r="M25" s="102"/>
+      <c r="L25" s="100"/>
+      <c r="M25" s="100"/>
       <c r="N25" s="49"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
@@ -1922,8 +1917,8 @@
       </c>
       <c r="J26" s="54"/>
       <c r="K26" s="4"/>
-      <c r="L26" s="102"/>
-      <c r="M26" s="102"/>
+      <c r="L26" s="100"/>
+      <c r="M26" s="100"/>
       <c r="N26" s="49"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
@@ -1942,8 +1937,8 @@
       </c>
       <c r="J27" s="54"/>
       <c r="K27" s="4"/>
-      <c r="L27" s="102"/>
-      <c r="M27" s="102"/>
+      <c r="L27" s="100"/>
+      <c r="M27" s="100"/>
       <c r="N27" s="49"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
@@ -1964,8 +1959,8 @@
       </c>
       <c r="J28" s="54"/>
       <c r="K28" s="4"/>
-      <c r="L28" s="102"/>
-      <c r="M28" s="102"/>
+      <c r="L28" s="100"/>
+      <c r="M28" s="100"/>
       <c r="N28" s="49"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
@@ -1984,8 +1979,8 @@
       </c>
       <c r="J29" s="54"/>
       <c r="K29" s="4"/>
-      <c r="L29" s="102"/>
-      <c r="M29" s="102"/>
+      <c r="L29" s="100"/>
+      <c r="M29" s="100"/>
       <c r="N29" s="49"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
@@ -2004,8 +1999,8 @@
       </c>
       <c r="J30" s="54"/>
       <c r="K30" s="4"/>
-      <c r="L30" s="102"/>
-      <c r="M30" s="102"/>
+      <c r="L30" s="100"/>
+      <c r="M30" s="100"/>
       <c r="N30" s="49"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
@@ -2026,8 +2021,8 @@
       </c>
       <c r="J31" s="54"/>
       <c r="K31" s="4"/>
-      <c r="L31" s="102"/>
-      <c r="M31" s="102"/>
+      <c r="L31" s="100"/>
+      <c r="M31" s="100"/>
       <c r="N31" s="49"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
@@ -2048,8 +2043,8 @@
       </c>
       <c r="J32" s="55"/>
       <c r="K32" s="4"/>
-      <c r="L32" s="102"/>
-      <c r="M32" s="102"/>
+      <c r="L32" s="100"/>
+      <c r="M32" s="100"/>
       <c r="N32" s="49"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
@@ -2088,8 +2083,8 @@
         <v>32</v>
       </c>
       <c r="K34" s="4"/>
-      <c r="L34" s="102"/>
-      <c r="M34" s="102"/>
+      <c r="L34" s="100"/>
+      <c r="M34" s="100"/>
       <c r="N34" s="49"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
@@ -2103,13 +2098,13 @@
       <c r="F35" s="69"/>
       <c r="G35" s="69"/>
       <c r="H35" s="69"/>
-      <c r="I35" s="107"/>
+      <c r="I35" s="104"/>
       <c r="J35" s="8" t="s">
         <v>34</v>
       </c>
       <c r="K35" s="4"/>
-      <c r="L35" s="102"/>
-      <c r="M35" s="102"/>
+      <c r="L35" s="100"/>
+      <c r="M35" s="100"/>
       <c r="N35" s="49"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
@@ -2123,7 +2118,7 @@
       <c r="F36" s="71"/>
       <c r="G36" s="71"/>
       <c r="H36" s="72"/>
-      <c r="I36" s="107"/>
+      <c r="I36" s="104"/>
       <c r="J36" s="8" t="s">
         <v>35</v>
       </c>
@@ -2152,8 +2147,8 @@
       </c>
       <c r="J37" s="54"/>
       <c r="K37" s="4"/>
-      <c r="L37" s="102"/>
-      <c r="M37" s="102"/>
+      <c r="L37" s="100"/>
+      <c r="M37" s="100"/>
       <c r="N37" s="49"/>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
@@ -2174,8 +2169,8 @@
       </c>
       <c r="J38" s="54"/>
       <c r="K38" s="4"/>
-      <c r="L38" s="102"/>
-      <c r="M38" s="102"/>
+      <c r="L38" s="100"/>
+      <c r="M38" s="100"/>
       <c r="N38" s="49"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
@@ -2191,8 +2186,8 @@
       </c>
       <c r="J39" s="54"/>
       <c r="K39" s="4"/>
-      <c r="L39" s="102"/>
-      <c r="M39" s="102"/>
+      <c r="L39" s="100"/>
+      <c r="M39" s="100"/>
       <c r="N39" s="49"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
@@ -2213,8 +2208,8 @@
       </c>
       <c r="J40" s="8"/>
       <c r="K40" s="4"/>
-      <c r="L40" s="102"/>
-      <c r="M40" s="102"/>
+      <c r="L40" s="100"/>
+      <c r="M40" s="100"/>
       <c r="N40" s="49"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.25">
@@ -2235,9 +2230,9 @@
       </c>
       <c r="J41" s="82"/>
       <c r="K41" s="18"/>
-      <c r="L41" s="104"/>
-      <c r="M41" s="104"/>
-      <c r="N41" s="93"/>
+      <c r="L41" s="101"/>
+      <c r="M41" s="101"/>
+      <c r="N41" s="91"/>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B42" s="60"/>
@@ -2252,9 +2247,9 @@
       </c>
       <c r="J42" s="54"/>
       <c r="K42" s="18"/>
-      <c r="L42" s="104"/>
-      <c r="M42" s="104"/>
-      <c r="N42" s="93"/>
+      <c r="L42" s="101"/>
+      <c r="M42" s="101"/>
+      <c r="N42" s="91"/>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B43" s="58">
@@ -2274,8 +2269,8 @@
       </c>
       <c r="J43" s="54"/>
       <c r="K43" s="4"/>
-      <c r="L43" s="102"/>
-      <c r="M43" s="102"/>
+      <c r="L43" s="100"/>
+      <c r="M43" s="100"/>
       <c r="N43" s="49"/>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.25">
@@ -2308,8 +2303,8 @@
         <v>32</v>
       </c>
       <c r="K45" s="8"/>
-      <c r="L45" s="105"/>
-      <c r="M45" s="105"/>
+      <c r="L45" s="102"/>
+      <c r="M45" s="102"/>
       <c r="N45" s="49"/>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.25">
@@ -2325,8 +2320,8 @@
         <v>34</v>
       </c>
       <c r="K46" s="4"/>
-      <c r="L46" s="102"/>
-      <c r="M46" s="102"/>
+      <c r="L46" s="100"/>
+      <c r="M46" s="100"/>
       <c r="N46" s="49"/>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.25">
@@ -2366,9 +2361,9 @@
       </c>
       <c r="J48" s="80"/>
       <c r="K48" s="19"/>
-      <c r="L48" s="106"/>
-      <c r="M48" s="106"/>
-      <c r="N48" s="94"/>
+      <c r="L48" s="103"/>
+      <c r="M48" s="103"/>
+      <c r="N48" s="92"/>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B49" s="58">
@@ -2388,8 +2383,8 @@
       </c>
       <c r="J49" s="54"/>
       <c r="K49" s="4"/>
-      <c r="L49" s="102"/>
-      <c r="M49" s="102"/>
+      <c r="L49" s="100"/>
+      <c r="M49" s="100"/>
       <c r="N49" s="49"/>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.25">
@@ -2405,8 +2400,8 @@
       </c>
       <c r="J50" s="54"/>
       <c r="K50" s="4"/>
-      <c r="L50" s="102"/>
-      <c r="M50" s="102"/>
+      <c r="L50" s="100"/>
+      <c r="M50" s="100"/>
       <c r="N50" s="49"/>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.25">
@@ -2447,8 +2442,8 @@
       </c>
       <c r="J52" s="54"/>
       <c r="K52" s="4"/>
-      <c r="L52" s="102"/>
-      <c r="M52" s="102"/>
+      <c r="L52" s="100"/>
+      <c r="M52" s="100"/>
       <c r="N52" s="49"/>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.25">
@@ -2466,7 +2461,7 @@
       <c r="K53" s="20"/>
       <c r="L53" s="88"/>
       <c r="M53" s="88"/>
-      <c r="N53" s="95" t="s">
+      <c r="N53" s="93" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2483,8 +2478,8 @@
       </c>
       <c r="J54" s="54"/>
       <c r="K54" s="4"/>
-      <c r="L54" s="102"/>
-      <c r="M54" s="102"/>
+      <c r="L54" s="100"/>
+      <c r="M54" s="100"/>
       <c r="N54" s="49"/>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.25">
@@ -2502,7 +2497,7 @@
       <c r="K55" s="20"/>
       <c r="L55" s="88"/>
       <c r="M55" s="88"/>
-      <c r="N55" s="95" t="s">
+      <c r="N55" s="93" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2524,8 +2519,8 @@
       </c>
       <c r="J56" s="54"/>
       <c r="K56" s="4"/>
-      <c r="L56" s="102"/>
-      <c r="M56" s="102"/>
+      <c r="L56" s="100"/>
+      <c r="M56" s="100"/>
       <c r="N56" s="49"/>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.25">
@@ -2546,8 +2541,8 @@
       </c>
       <c r="J57" s="54"/>
       <c r="K57" s="4"/>
-      <c r="L57" s="102"/>
-      <c r="M57" s="102"/>
+      <c r="L57" s="100"/>
+      <c r="M57" s="100"/>
       <c r="N57" s="49"/>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.25">
@@ -2563,8 +2558,8 @@
       </c>
       <c r="J58" s="54"/>
       <c r="K58" s="4"/>
-      <c r="L58" s="102"/>
-      <c r="M58" s="102"/>
+      <c r="L58" s="100"/>
+      <c r="M58" s="100"/>
       <c r="N58" s="49"/>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.25">
@@ -2580,8 +2575,8 @@
       </c>
       <c r="J59" s="54"/>
       <c r="K59" s="4"/>
-      <c r="L59" s="102"/>
-      <c r="M59" s="102"/>
+      <c r="L59" s="100"/>
+      <c r="M59" s="100"/>
       <c r="N59" s="49"/>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.25">
@@ -2597,8 +2592,8 @@
       </c>
       <c r="J60" s="54"/>
       <c r="K60" s="4"/>
-      <c r="L60" s="102"/>
-      <c r="M60" s="102"/>
+      <c r="L60" s="100"/>
+      <c r="M60" s="100"/>
       <c r="N60" s="49"/>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.25">
@@ -2614,8 +2609,8 @@
       </c>
       <c r="J61" s="54"/>
       <c r="K61" s="4"/>
-      <c r="L61" s="102"/>
-      <c r="M61" s="102"/>
+      <c r="L61" s="100"/>
+      <c r="M61" s="100"/>
       <c r="N61" s="49"/>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.25">
@@ -2636,8 +2631,8 @@
       </c>
       <c r="J62" s="55"/>
       <c r="K62" s="4"/>
-      <c r="L62" s="102"/>
-      <c r="M62" s="102"/>
+      <c r="L62" s="100"/>
+      <c r="M62" s="100"/>
       <c r="N62" s="49"/>
     </row>
     <row r="63" spans="2:14" x14ac:dyDescent="0.25">
@@ -2653,8 +2648,8 @@
       </c>
       <c r="J63" s="54"/>
       <c r="K63" s="4"/>
-      <c r="L63" s="102"/>
-      <c r="M63" s="102"/>
+      <c r="L63" s="100"/>
+      <c r="M63" s="100"/>
       <c r="N63" s="49"/>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.25">
@@ -2670,8 +2665,8 @@
       </c>
       <c r="J64" s="54"/>
       <c r="K64" s="4"/>
-      <c r="L64" s="102"/>
-      <c r="M64" s="102"/>
+      <c r="L64" s="100"/>
+      <c r="M64" s="100"/>
       <c r="N64" s="49"/>
     </row>
     <row r="65" spans="2:14" x14ac:dyDescent="0.25">
@@ -2711,8 +2706,8 @@
       </c>
       <c r="J66" s="55"/>
       <c r="K66" s="4"/>
-      <c r="L66" s="102"/>
-      <c r="M66" s="102"/>
+      <c r="L66" s="100"/>
+      <c r="M66" s="100"/>
       <c r="N66" s="49"/>
     </row>
     <row r="67" spans="2:14" x14ac:dyDescent="0.25">
@@ -2731,8 +2726,8 @@
       <c r="I67" s="50"/>
       <c r="J67" s="51"/>
       <c r="K67" s="4"/>
-      <c r="L67" s="102"/>
-      <c r="M67" s="102"/>
+      <c r="L67" s="100"/>
+      <c r="M67" s="100"/>
       <c r="N67" s="49"/>
     </row>
     <row r="68" spans="2:14" x14ac:dyDescent="0.25">
@@ -2749,8 +2744,8 @@
       <c r="I68" s="50"/>
       <c r="J68" s="51"/>
       <c r="K68" s="4"/>
-      <c r="L68" s="102"/>
-      <c r="M68" s="102"/>
+      <c r="L68" s="100"/>
+      <c r="M68" s="100"/>
       <c r="N68" s="49"/>
     </row>
     <row r="69" spans="2:14" x14ac:dyDescent="0.25">
@@ -2767,8 +2762,8 @@
       <c r="I69" s="50"/>
       <c r="J69" s="51"/>
       <c r="K69" s="4"/>
-      <c r="L69" s="102"/>
-      <c r="M69" s="102"/>
+      <c r="L69" s="100"/>
+      <c r="M69" s="100"/>
       <c r="N69" s="49"/>
     </row>
     <row r="70" spans="2:14" x14ac:dyDescent="0.25">
@@ -2785,8 +2780,8 @@
       <c r="I70" s="50"/>
       <c r="J70" s="51"/>
       <c r="K70" s="4"/>
-      <c r="L70" s="102"/>
-      <c r="M70" s="102"/>
+      <c r="L70" s="100"/>
+      <c r="M70" s="100"/>
       <c r="N70" s="49"/>
     </row>
     <row r="71" spans="2:14" x14ac:dyDescent="0.25">
@@ -2803,8 +2798,8 @@
       <c r="I71" s="50"/>
       <c r="J71" s="51"/>
       <c r="K71" s="4"/>
-      <c r="L71" s="102"/>
-      <c r="M71" s="102"/>
+      <c r="L71" s="100"/>
+      <c r="M71" s="100"/>
       <c r="N71" s="49"/>
     </row>
     <row r="72" spans="2:14" x14ac:dyDescent="0.25">
@@ -2821,8 +2816,8 @@
       <c r="I72" s="50"/>
       <c r="J72" s="51"/>
       <c r="K72" s="4"/>
-      <c r="L72" s="102"/>
-      <c r="M72" s="102"/>
+      <c r="L72" s="100"/>
+      <c r="M72" s="100"/>
       <c r="N72" s="49"/>
     </row>
     <row r="73" spans="2:14" x14ac:dyDescent="0.25">
@@ -2839,8 +2834,8 @@
       <c r="I73" s="50"/>
       <c r="J73" s="51"/>
       <c r="K73" s="4"/>
-      <c r="L73" s="102"/>
-      <c r="M73" s="102"/>
+      <c r="L73" s="100"/>
+      <c r="M73" s="100"/>
       <c r="N73" s="49"/>
     </row>
     <row r="74" spans="2:14" x14ac:dyDescent="0.25">
@@ -2857,8 +2852,8 @@
       <c r="I74" s="50"/>
       <c r="J74" s="51"/>
       <c r="K74" s="4"/>
-      <c r="L74" s="102"/>
-      <c r="M74" s="102"/>
+      <c r="L74" s="100"/>
+      <c r="M74" s="100"/>
       <c r="N74" s="49"/>
     </row>
     <row r="75" spans="2:14" x14ac:dyDescent="0.25">
@@ -2875,8 +2870,8 @@
       <c r="I75" s="50"/>
       <c r="J75" s="51"/>
       <c r="K75" s="4"/>
-      <c r="L75" s="102"/>
-      <c r="M75" s="102"/>
+      <c r="L75" s="100"/>
+      <c r="M75" s="100"/>
       <c r="N75" s="49"/>
     </row>
     <row r="76" spans="2:14" x14ac:dyDescent="0.25">
@@ -2893,8 +2888,8 @@
       <c r="I76" s="50"/>
       <c r="J76" s="51"/>
       <c r="K76" s="4"/>
-      <c r="L76" s="102"/>
-      <c r="M76" s="102"/>
+      <c r="L76" s="100"/>
+      <c r="M76" s="100"/>
       <c r="N76" s="49"/>
     </row>
     <row r="77" spans="2:14" x14ac:dyDescent="0.25">
@@ -2911,8 +2906,8 @@
       <c r="I77" s="50"/>
       <c r="J77" s="51"/>
       <c r="K77" s="4"/>
-      <c r="L77" s="102"/>
-      <c r="M77" s="102"/>
+      <c r="L77" s="100"/>
+      <c r="M77" s="100"/>
       <c r="N77" s="49"/>
     </row>
   </sheetData>
@@ -2920,9 +2915,9 @@
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="M10:M13"/>
     <mergeCell ref="B17:N17"/>
+    <mergeCell ref="N10:N15"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I16:J16"/>
-    <mergeCell ref="N10:N13"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="I75:J75"/>

</xml_diff>

<commit_message>
#7 Server error on Sign Up is not shown to the user\ + Default credentials for test sign up
</commit_message>
<xml_diff>
--- a/documents/Testing Schedule.xlsx
+++ b/documents/Testing Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Node\Timelog\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7931E56-4955-4B58-83D8-B772A10EA8A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D72B6C7-4FB3-4940-B43E-34F244B4D5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{9AAAF6DA-95E7-49F0-B7DD-46373E33B9E7}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="125">
   <si>
     <t>RMPC Timelog Testing Schedule</t>
   </si>
@@ -354,33 +354,24 @@
     <t>Sign Up page</t>
   </si>
   <si>
-    <t>Action</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>Click link</t>
-  </si>
-  <si>
     <t>Navigate</t>
   </si>
   <si>
-    <t>Submit</t>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
     <t>Home page</t>
   </si>
   <si>
-    <t>Load</t>
-  </si>
-  <si>
     <t>No error message transition</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>N - Failed</t>
   </si>
   <si>
@@ -396,23 +387,38 @@
     <t>#1</t>
   </si>
   <si>
+    <t>#2</t>
+  </si>
+  <si>
     <t>#3</t>
   </si>
   <si>
-    <t>SHOWSTOPPER</t>
-  </si>
-  <si>
     <t>Temporarily disabled pending end of Beta Promotion</t>
   </si>
   <si>
-    <t>#2 - #3</t>
+    <t>Database entries</t>
+  </si>
+  <si>
+    <t>Create</t>
+  </si>
+  <si>
+    <t>Accounts table</t>
+  </si>
+  <si>
+    <t>Script error</t>
+  </si>
+  <si>
+    <t>#5</t>
+  </si>
+  <si>
+    <t>#6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -463,21 +469,13 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="0" tint="-4.9989318521683403E-2"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFEA8B00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -511,12 +509,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -702,7 +694,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -820,99 +812,87 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -961,15 +941,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -994,59 +965,26 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1371,7 +1309,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R26" sqref="R26"/>
+      <selection pane="bottomLeft" activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1380,51 +1318,51 @@
     <col min="2" max="2" width="5.7109375" style="3" customWidth="1"/>
     <col min="3" max="7" width="10.7109375" style="2" customWidth="1"/>
     <col min="8" max="8" width="35.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="29.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="11.28515625" style="99" customWidth="1"/>
-    <col min="14" max="14" width="49.140625" style="89" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="62.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="3" customWidth="1"/>
+    <col min="11" max="12" width="9.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="49.140625" style="92" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="49.140625" style="85" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="97" t="s">
-        <v>116</v>
-      </c>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="P2" s="94"/>
+      <c r="B2" s="90" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="P2" s="87"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="115" t="s">
-        <v>115</v>
-      </c>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="113"/>
-      <c r="F3" s="114"/>
+      <c r="B3" s="97" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="96"/>
       <c r="H3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I3" s="1"/>
-      <c r="L3" s="2"/>
-      <c r="N3" s="99"/>
-      <c r="O3" s="89"/>
-      <c r="Q3" s="95"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="92"/>
+      <c r="O3" s="85"/>
+      <c r="Q3" s="88"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="98" t="s">
-        <v>114</v>
-      </c>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
+      <c r="B4" s="91" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="P4" s="96"/>
+      <c r="P4" s="89"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
@@ -1438,41 +1376,39 @@
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
       <c r="H6" s="15"/>
-      <c r="I6" s="84" t="s">
+      <c r="I6" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="K6" s="80" t="s">
+        <v>114</v>
+      </c>
+      <c r="L6" s="81"/>
+      <c r="M6" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="J6" s="85"/>
-      <c r="K6" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="L6" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="M6" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="N6" s="17" t="s">
-        <v>106</v>
-      </c>
+      <c r="N6" s="2"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="11">
         <v>1</v>
       </c>
-      <c r="C7" s="83" t="s">
+      <c r="C7" s="79" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="73"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="100"/>
-      <c r="M7" s="100"/>
-      <c r="N7" s="49"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="93"/>
+      <c r="K7" s="93"/>
+      <c r="L7" s="93"/>
+      <c r="M7" s="45"/>
+      <c r="N7" s="2"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="11">
@@ -1480,29 +1416,27 @@
         <v>2</v>
       </c>
       <c r="C8" s="41"/>
-      <c r="D8" s="52" t="s">
+      <c r="D8" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="73" t="s">
-        <v>107</v>
-      </c>
-      <c r="J8" s="54"/>
-      <c r="K8" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="L8" s="88" t="s">
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="J8" s="84" t="s">
         <v>70</v>
       </c>
-      <c r="M8" s="88"/>
-      <c r="N8" s="49"/>
+      <c r="K8" s="84"/>
+      <c r="L8" s="84"/>
+      <c r="M8" s="45"/>
+      <c r="N8" s="2"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="11">
-        <f t="shared" ref="B9:B36" si="0">B8+1</f>
+        <f t="shared" ref="B9:B72" si="0">B8+1</f>
         <v>3</v>
       </c>
       <c r="C9" s="41"/>
@@ -1512,13 +1446,13 @@
       <c r="E9" s="42"/>
       <c r="F9" s="42"/>
       <c r="G9" s="42"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="46"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="100"/>
-      <c r="M9" s="100"/>
-      <c r="N9" s="49"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="93"/>
+      <c r="K9" s="93"/>
+      <c r="L9" s="93"/>
+      <c r="M9" s="45"/>
+      <c r="N9" s="2"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" s="11">
@@ -1532,23 +1466,21 @@
       </c>
       <c r="F10" s="42"/>
       <c r="G10" s="42"/>
-      <c r="H10" s="43"/>
+      <c r="H10" s="42"/>
       <c r="I10" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="J10" s="98" t="s">
+        <v>70</v>
+      </c>
+      <c r="K10" s="99" t="s">
+        <v>117</v>
+      </c>
+      <c r="L10" s="98"/>
+      <c r="M10" s="100" t="s">
         <v>109</v>
       </c>
-      <c r="J10" s="46"/>
-      <c r="K10" s="45" t="s">
-        <v>95</v>
-      </c>
-      <c r="L10" s="111" t="s">
-        <v>70</v>
-      </c>
-      <c r="M10" s="108" t="s">
-        <v>119</v>
-      </c>
-      <c r="N10" s="116" t="s">
-        <v>113</v>
-      </c>
+      <c r="N10" s="2"/>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" s="11">
@@ -1562,19 +1494,17 @@
       </c>
       <c r="F11" s="42"/>
       <c r="G11" s="42"/>
-      <c r="H11" s="43"/>
+      <c r="H11" s="42"/>
       <c r="I11" s="45" t="s">
-        <v>109</v>
-      </c>
-      <c r="J11" s="46"/>
-      <c r="K11" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="L11" s="111" t="s">
+      <c r="J11" s="98" t="s">
         <v>70</v>
       </c>
-      <c r="M11" s="109"/>
-      <c r="N11" s="117"/>
+      <c r="K11" s="99"/>
+      <c r="L11" s="98"/>
+      <c r="M11" s="100"/>
+      <c r="N11" s="2"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="11">
@@ -1588,19 +1518,17 @@
       </c>
       <c r="F12" s="42"/>
       <c r="G12" s="42"/>
-      <c r="H12" s="43"/>
+      <c r="H12" s="42"/>
       <c r="I12" s="45" t="s">
-        <v>109</v>
-      </c>
-      <c r="J12" s="46"/>
-      <c r="K12" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="L12" s="111" t="s">
+      <c r="J12" s="98" t="s">
         <v>70</v>
       </c>
-      <c r="M12" s="109"/>
-      <c r="N12" s="117"/>
+      <c r="K12" s="99"/>
+      <c r="L12" s="98"/>
+      <c r="M12" s="100"/>
+      <c r="N12" s="2"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="11">
@@ -1614,19 +1542,17 @@
       </c>
       <c r="F13" s="42"/>
       <c r="G13" s="42"/>
-      <c r="H13" s="43"/>
+      <c r="H13" s="42"/>
       <c r="I13" s="45" t="s">
-        <v>109</v>
-      </c>
-      <c r="J13" s="46"/>
-      <c r="K13" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="L13" s="111" t="s">
+      <c r="J13" s="98" t="s">
         <v>70</v>
       </c>
-      <c r="M13" s="110"/>
-      <c r="N13" s="117"/>
+      <c r="K13" s="99"/>
+      <c r="L13" s="98"/>
+      <c r="M13" s="100"/>
+      <c r="N13" s="2"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" s="11">
@@ -1640,21 +1566,21 @@
       </c>
       <c r="F14" s="42"/>
       <c r="G14" s="42"/>
-      <c r="H14" s="43"/>
+      <c r="H14" s="42"/>
       <c r="I14" s="45" t="s">
-        <v>109</v>
-      </c>
-      <c r="J14" s="46"/>
-      <c r="K14" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="L14" s="111" t="s">
+      <c r="J14" s="98" t="s">
         <v>70</v>
       </c>
-      <c r="M14" s="111" t="s">
-        <v>122</v>
-      </c>
-      <c r="N14" s="117"/>
+      <c r="K14" s="84" t="s">
+        <v>116</v>
+      </c>
+      <c r="L14" s="98" t="s">
+        <v>117</v>
+      </c>
+      <c r="M14" s="100"/>
+      <c r="N14" s="2"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" s="11">
@@ -1668,21 +1594,19 @@
       </c>
       <c r="F15" s="42"/>
       <c r="G15" s="42"/>
-      <c r="H15" s="43"/>
+      <c r="H15" s="42"/>
       <c r="I15" s="45" t="s">
-        <v>109</v>
-      </c>
-      <c r="J15" s="46"/>
-      <c r="K15" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="L15" s="111" t="s">
+      <c r="J15" s="98" t="s">
         <v>70</v>
       </c>
-      <c r="M15" s="111" t="s">
-        <v>119</v>
-      </c>
-      <c r="N15" s="118"/>
+      <c r="K15" s="98" t="s">
+        <v>117</v>
+      </c>
+      <c r="L15" s="98"/>
+      <c r="M15" s="100"/>
+      <c r="N15" s="2"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="11">
@@ -1696,149 +1620,160 @@
       </c>
       <c r="F16" s="42"/>
       <c r="G16" s="42"/>
-      <c r="H16" s="43"/>
-      <c r="I16" s="73" t="s">
-        <v>112</v>
-      </c>
-      <c r="J16" s="54"/>
-      <c r="K16" s="45" t="s">
+      <c r="H16" s="42"/>
+      <c r="I16" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="L16" s="88" t="s">
+      <c r="J16" s="84" t="s">
         <v>70</v>
       </c>
-      <c r="M16" s="88" t="s">
+      <c r="K16" s="84" t="s">
+        <v>115</v>
+      </c>
+      <c r="L16" s="84"/>
+      <c r="M16" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="N16" s="49" t="s">
-        <v>121</v>
-      </c>
+      <c r="N16" s="2"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="105" t="s">
-        <v>120</v>
-      </c>
-      <c r="C17" s="106"/>
-      <c r="D17" s="106"/>
-      <c r="E17" s="106"/>
-      <c r="F17" s="106"/>
-      <c r="G17" s="106"/>
-      <c r="H17" s="106"/>
-      <c r="I17" s="106"/>
-      <c r="J17" s="106"/>
-      <c r="K17" s="106"/>
-      <c r="L17" s="106"/>
-      <c r="M17" s="106"/>
-      <c r="N17" s="107"/>
+      <c r="B17" s="11">
+        <f>B16+1</f>
+        <v>11</v>
+      </c>
+      <c r="C17" s="41"/>
+      <c r="D17" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="93"/>
+      <c r="K17" s="93"/>
+      <c r="L17" s="93"/>
+      <c r="M17" s="45"/>
+      <c r="N17" s="2"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="11">
-        <f>B16+1</f>
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
       <c r="C18" s="41"/>
-      <c r="D18" s="42" t="s">
-        <v>103</v>
-      </c>
-      <c r="E18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42" t="s">
+        <v>108</v>
+      </c>
       <c r="F18" s="42"/>
       <c r="G18" s="42"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="45"/>
-      <c r="J18" s="46"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="100"/>
-      <c r="M18" s="100"/>
-      <c r="N18" s="49"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="J18" s="83" t="s">
+        <v>110</v>
+      </c>
+      <c r="K18" s="84" t="s">
+        <v>123</v>
+      </c>
+      <c r="L18" s="83" t="s">
+        <v>124</v>
+      </c>
+      <c r="M18" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="N18" s="2"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="11">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C19" s="41"/>
       <c r="D19" s="42"/>
       <c r="E19" s="42" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="F19" s="42"/>
       <c r="G19" s="42"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="45" t="s">
-        <v>109</v>
-      </c>
-      <c r="J19" s="46"/>
-      <c r="K19" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="L19" s="100"/>
-      <c r="M19" s="100"/>
-      <c r="N19" s="49"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="93"/>
+      <c r="K19" s="93"/>
+      <c r="L19" s="93"/>
+      <c r="M19" s="45"/>
+      <c r="N19" s="2"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="11">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C20" s="41"/>
       <c r="D20" s="42"/>
       <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
+      <c r="F20" s="42" t="s">
+        <v>121</v>
+      </c>
       <c r="G20" s="42"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="46"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="100"/>
-      <c r="M20" s="100"/>
-      <c r="N20" s="49"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="J20" s="93"/>
+      <c r="K20" s="93"/>
+      <c r="L20" s="93"/>
+      <c r="M20" s="45"/>
+      <c r="N20" s="2"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="11">
         <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="C21" s="83" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="79" t="s">
         <v>90</v>
       </c>
-      <c r="D21" s="52"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="73"/>
-      <c r="J21" s="54"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="82"/>
       <c r="K21" s="4"/>
-      <c r="L21" s="100"/>
-      <c r="M21" s="100"/>
-      <c r="N21" s="49"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="93"/>
+      <c r="N21" s="2"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="11">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C22" s="5"/>
-      <c r="D22" s="52" t="s">
+      <c r="D22" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="E22" s="52"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="73" t="s">
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="J22" s="54"/>
+      <c r="J22" s="82"/>
       <c r="K22" s="4"/>
-      <c r="L22" s="100"/>
-      <c r="M22" s="100"/>
-      <c r="N22" s="49"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="93"/>
+      <c r="N22" s="2"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="11">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="9" t="s">
@@ -1847,1172 +1782,1162 @@
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="73" t="s">
+      <c r="H23" s="9"/>
+      <c r="I23" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J23" s="54"/>
+      <c r="J23" s="82"/>
       <c r="K23" s="4"/>
-      <c r="L23" s="100"/>
-      <c r="M23" s="100"/>
-      <c r="N23" s="49"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="93"/>
+      <c r="N23" s="2"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="11">
         <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="C24" s="75" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="67"/>
-      <c r="E24" s="67"/>
-      <c r="F24" s="67"/>
-      <c r="G24" s="67"/>
-      <c r="H24" s="68"/>
-      <c r="I24" s="73" t="s">
+      <c r="D24" s="63"/>
+      <c r="E24" s="63"/>
+      <c r="F24" s="63"/>
+      <c r="G24" s="63"/>
+      <c r="H24" s="63"/>
+      <c r="I24" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J24" s="54"/>
+      <c r="J24" s="82"/>
       <c r="K24" s="4"/>
-      <c r="L24" s="100"/>
-      <c r="M24" s="100"/>
-      <c r="N24" s="49"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="93"/>
+      <c r="N24" s="2"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="11">
         <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="C25" s="77"/>
-      <c r="D25" s="71"/>
-      <c r="E25" s="71"/>
-      <c r="F25" s="71"/>
-      <c r="G25" s="71"/>
-      <c r="H25" s="72"/>
-      <c r="I25" s="73" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="73"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="67"/>
+      <c r="H25" s="67"/>
+      <c r="I25" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J25" s="54"/>
+      <c r="J25" s="82"/>
       <c r="K25" s="4"/>
-      <c r="L25" s="100"/>
-      <c r="M25" s="100"/>
-      <c r="N25" s="49"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="93"/>
+      <c r="N25" s="2"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="11">
         <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="C26" s="61"/>
-      <c r="D26" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="57"/>
+      <c r="D26" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="67"/>
-      <c r="F26" s="67"/>
-      <c r="G26" s="67"/>
-      <c r="H26" s="68"/>
-      <c r="I26" s="73" t="s">
+      <c r="E26" s="63"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="63"/>
+      <c r="H26" s="63"/>
+      <c r="I26" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J26" s="54"/>
+      <c r="J26" s="82"/>
       <c r="K26" s="4"/>
-      <c r="L26" s="100"/>
-      <c r="M26" s="100"/>
-      <c r="N26" s="49"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="93"/>
+      <c r="N26" s="2"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="11">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="C27" s="65"/>
-      <c r="D27" s="71"/>
-      <c r="E27" s="71"/>
-      <c r="F27" s="71"/>
-      <c r="G27" s="71"/>
-      <c r="H27" s="72"/>
-      <c r="I27" s="73" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="61"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="67"/>
+      <c r="G27" s="67"/>
+      <c r="H27" s="67"/>
+      <c r="I27" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="J27" s="54"/>
+      <c r="J27" s="82"/>
       <c r="K27" s="4"/>
-      <c r="L27" s="100"/>
-      <c r="M27" s="100"/>
-      <c r="N27" s="49"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="93"/>
+      <c r="N27" s="2"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="11">
         <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="C28" s="61"/>
-      <c r="D28" s="67" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="57"/>
+      <c r="D28" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="67"/>
-      <c r="F28" s="67"/>
-      <c r="G28" s="67"/>
-      <c r="H28" s="68"/>
-      <c r="I28" s="73" t="s">
+      <c r="E28" s="63"/>
+      <c r="F28" s="63"/>
+      <c r="G28" s="63"/>
+      <c r="H28" s="63"/>
+      <c r="I28" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J28" s="54"/>
+      <c r="J28" s="82"/>
       <c r="K28" s="4"/>
-      <c r="L28" s="100"/>
-      <c r="M28" s="100"/>
-      <c r="N28" s="49"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="93"/>
+      <c r="N28" s="2"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="11">
         <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="C29" s="63"/>
-      <c r="D29" s="69"/>
-      <c r="E29" s="69"/>
-      <c r="F29" s="69"/>
-      <c r="G29" s="69"/>
-      <c r="H29" s="70"/>
-      <c r="I29" s="73" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="59"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="65"/>
+      <c r="F29" s="65"/>
+      <c r="G29" s="65"/>
+      <c r="H29" s="65"/>
+      <c r="I29" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="J29" s="54"/>
+      <c r="J29" s="82"/>
       <c r="K29" s="4"/>
-      <c r="L29" s="100"/>
-      <c r="M29" s="100"/>
-      <c r="N29" s="49"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="93"/>
+      <c r="N29" s="2"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="11">
         <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="C30" s="65"/>
-      <c r="D30" s="71"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="72"/>
-      <c r="I30" s="73" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="61"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="67"/>
+      <c r="H30" s="67"/>
+      <c r="I30" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="J30" s="54"/>
+      <c r="J30" s="82"/>
       <c r="K30" s="4"/>
-      <c r="L30" s="100"/>
-      <c r="M30" s="100"/>
-      <c r="N30" s="49"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="93"/>
+      <c r="N30" s="2"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" s="11">
         <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="C31" s="48"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="44"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="F31" s="52"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="53"/>
-      <c r="I31" s="73" t="s">
+      <c r="F31" s="48"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="J31" s="54"/>
+      <c r="J31" s="82"/>
       <c r="K31" s="4"/>
-      <c r="L31" s="100"/>
-      <c r="M31" s="100"/>
-      <c r="N31" s="49"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="93"/>
+      <c r="N31" s="2"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" s="11">
         <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="C32" s="61"/>
-      <c r="D32" s="62"/>
-      <c r="E32" s="62"/>
-      <c r="F32" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="57"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="58"/>
+      <c r="F32" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="G32" s="67"/>
-      <c r="H32" s="68"/>
-      <c r="I32" s="55" t="s">
+      <c r="G32" s="63"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J32" s="55"/>
+      <c r="J32" s="82"/>
       <c r="K32" s="4"/>
-      <c r="L32" s="100"/>
-      <c r="M32" s="100"/>
-      <c r="N32" s="49"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="93"/>
+      <c r="N32" s="2"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="11">
         <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="C33" s="63"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
-      <c r="F33" s="69"/>
-      <c r="G33" s="69"/>
-      <c r="H33" s="70"/>
-      <c r="I33" s="90" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="59"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="65"/>
+      <c r="G33" s="65"/>
+      <c r="H33" s="65"/>
+      <c r="I33" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J33" s="55"/>
-      <c r="K33" s="55"/>
-      <c r="L33" s="86"/>
-      <c r="M33" s="86"/>
-      <c r="N33" s="55"/>
+      <c r="J33" s="82"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="2"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" s="11">
         <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="C34" s="63"/>
-      <c r="D34" s="64"/>
-      <c r="E34" s="64"/>
-      <c r="F34" s="69"/>
-      <c r="G34" s="69"/>
-      <c r="H34" s="69"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="59"/>
+      <c r="D34" s="60"/>
+      <c r="E34" s="60"/>
+      <c r="F34" s="65"/>
+      <c r="G34" s="65"/>
+      <c r="H34" s="65"/>
+      <c r="I34" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="K34" s="4"/>
-      <c r="L34" s="100"/>
-      <c r="M34" s="100"/>
-      <c r="N34" s="49"/>
+      <c r="J34" s="82"/>
+      <c r="K34" s="93"/>
+      <c r="L34" s="93"/>
+      <c r="M34" s="45"/>
+      <c r="N34" s="2"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="11">
         <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="C35" s="63"/>
-      <c r="D35" s="64"/>
-      <c r="E35" s="64"/>
-      <c r="F35" s="69"/>
-      <c r="G35" s="69"/>
-      <c r="H35" s="69"/>
-      <c r="I35" s="104"/>
-      <c r="J35" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="59"/>
+      <c r="D35" s="60"/>
+      <c r="E35" s="60"/>
+      <c r="F35" s="65"/>
+      <c r="G35" s="65"/>
+      <c r="H35" s="65"/>
+      <c r="I35" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="K35" s="4"/>
-      <c r="L35" s="100"/>
-      <c r="M35" s="100"/>
-      <c r="N35" s="49"/>
+      <c r="J35" s="82"/>
+      <c r="K35" s="93"/>
+      <c r="L35" s="93"/>
+      <c r="M35" s="45"/>
+      <c r="N35" s="2"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" s="11">
         <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="C36" s="65"/>
-      <c r="D36" s="66"/>
-      <c r="E36" s="66"/>
-      <c r="F36" s="71"/>
-      <c r="G36" s="71"/>
-      <c r="H36" s="72"/>
-      <c r="I36" s="104"/>
-      <c r="J36" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="61"/>
+      <c r="D36" s="62"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="67"/>
+      <c r="G36" s="67"/>
+      <c r="H36" s="67"/>
+      <c r="I36" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K36" s="10"/>
-      <c r="L36" s="87"/>
-      <c r="M36" s="87"/>
-      <c r="N36" s="49" t="s">
+      <c r="J36" s="83"/>
+      <c r="K36" s="83"/>
+      <c r="L36" s="83"/>
+      <c r="M36" s="45" t="s">
         <v>36</v>
       </c>
+      <c r="N36" s="2"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B37" s="44">
-        <f>B32+1</f>
-        <v>26</v>
-      </c>
-      <c r="C37" s="56"/>
-      <c r="D37" s="57"/>
-      <c r="E37" s="52" t="s">
+      <c r="B37" s="11">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="C37" s="52"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="F37" s="52"/>
-      <c r="G37" s="52"/>
-      <c r="H37" s="53"/>
-      <c r="I37" s="73" t="s">
+      <c r="F37" s="48"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="48"/>
+      <c r="I37" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J37" s="54"/>
+      <c r="J37" s="82"/>
       <c r="K37" s="4"/>
-      <c r="L37" s="100"/>
-      <c r="M37" s="100"/>
-      <c r="N37" s="49"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="93"/>
+      <c r="N37" s="2"/>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B38" s="58">
-        <f>B37+1</f>
-        <v>27</v>
-      </c>
-      <c r="C38" s="61"/>
-      <c r="D38" s="62"/>
-      <c r="E38" s="62"/>
-      <c r="F38" s="67" t="s">
+      <c r="B38" s="11">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="C38" s="57"/>
+      <c r="D38" s="58"/>
+      <c r="E38" s="58"/>
+      <c r="F38" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="G38" s="67"/>
-      <c r="H38" s="68"/>
-      <c r="I38" s="73" t="s">
+      <c r="G38" s="63"/>
+      <c r="H38" s="63"/>
+      <c r="I38" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="J38" s="54"/>
+      <c r="J38" s="82"/>
       <c r="K38" s="4"/>
-      <c r="L38" s="100"/>
-      <c r="M38" s="100"/>
-      <c r="N38" s="49"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="93"/>
+      <c r="N38" s="2"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B39" s="60"/>
-      <c r="C39" s="65"/>
-      <c r="D39" s="66"/>
-      <c r="E39" s="66"/>
-      <c r="F39" s="71"/>
-      <c r="G39" s="71"/>
-      <c r="H39" s="72"/>
-      <c r="I39" s="73" t="s">
+      <c r="B39" s="11">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="C39" s="61"/>
+      <c r="D39" s="62"/>
+      <c r="E39" s="62"/>
+      <c r="F39" s="67"/>
+      <c r="G39" s="67"/>
+      <c r="H39" s="67"/>
+      <c r="I39" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J39" s="54"/>
+      <c r="J39" s="82"/>
       <c r="K39" s="4"/>
-      <c r="L39" s="100"/>
-      <c r="M39" s="100"/>
-      <c r="N39" s="49"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="93"/>
+      <c r="N39" s="2"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B40" s="44">
-        <f>B38+1</f>
-        <v>28</v>
+      <c r="B40" s="11">
+        <f t="shared" si="0"/>
+        <v>34</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
-      <c r="F40" s="52" t="s">
+      <c r="F40" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="G40" s="52"/>
-      <c r="H40" s="53"/>
-      <c r="I40" s="7" t="s">
+      <c r="G40" s="48"/>
+      <c r="H40" s="48"/>
+      <c r="I40" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J40" s="8"/>
+      <c r="J40" s="82"/>
       <c r="K40" s="4"/>
-      <c r="L40" s="100"/>
-      <c r="M40" s="100"/>
-      <c r="N40" s="49"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="93"/>
+      <c r="N40" s="2"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B41" s="58">
-        <f t="shared" ref="B41:B57" si="1">B40+1</f>
-        <v>29</v>
-      </c>
-      <c r="C41" s="61"/>
-      <c r="D41" s="62"/>
-      <c r="E41" s="62"/>
-      <c r="F41" s="67" t="s">
+      <c r="B41" s="11">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="C41" s="57"/>
+      <c r="D41" s="58"/>
+      <c r="E41" s="58"/>
+      <c r="F41" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="G41" s="67"/>
-      <c r="H41" s="68"/>
-      <c r="I41" s="81" t="s">
+      <c r="G41" s="63"/>
+      <c r="H41" s="63"/>
+      <c r="I41" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J41" s="82"/>
-      <c r="K41" s="18"/>
-      <c r="L41" s="101"/>
-      <c r="M41" s="101"/>
-      <c r="N41" s="91"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="93"/>
+      <c r="N41" s="2"/>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B42" s="60"/>
-      <c r="C42" s="65"/>
-      <c r="D42" s="66"/>
-      <c r="E42" s="66"/>
-      <c r="F42" s="71"/>
-      <c r="G42" s="71"/>
-      <c r="H42" s="72"/>
-      <c r="I42" s="73" t="s">
+      <c r="B42" s="11">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="C42" s="61"/>
+      <c r="D42" s="62"/>
+      <c r="E42" s="62"/>
+      <c r="F42" s="67"/>
+      <c r="G42" s="67"/>
+      <c r="H42" s="67"/>
+      <c r="I42" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J42" s="54"/>
-      <c r="K42" s="18"/>
-      <c r="L42" s="101"/>
-      <c r="M42" s="101"/>
-      <c r="N42" s="91"/>
+      <c r="J42" s="82"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="93"/>
+      <c r="N42" s="2"/>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B43" s="58">
-        <f>B41+1</f>
-        <v>30</v>
-      </c>
-      <c r="C43" s="75"/>
-      <c r="D43" s="67"/>
-      <c r="E43" s="67"/>
-      <c r="F43" s="67" t="s">
+      <c r="B43" s="11">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="C43" s="71"/>
+      <c r="D43" s="63"/>
+      <c r="E43" s="63"/>
+      <c r="F43" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="G43" s="67"/>
-      <c r="H43" s="68"/>
-      <c r="I43" s="73" t="s">
+      <c r="G43" s="63"/>
+      <c r="H43" s="63"/>
+      <c r="I43" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J43" s="54"/>
+      <c r="J43" s="82"/>
       <c r="K43" s="4"/>
-      <c r="L43" s="100"/>
-      <c r="M43" s="100"/>
-      <c r="N43" s="49"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="93"/>
+      <c r="N43" s="2"/>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B44" s="59"/>
-      <c r="C44" s="76"/>
-      <c r="D44" s="69"/>
-      <c r="E44" s="69"/>
-      <c r="F44" s="69"/>
-      <c r="G44" s="69"/>
-      <c r="H44" s="70"/>
-      <c r="I44" s="73" t="s">
+      <c r="B44" s="11">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="C44" s="72"/>
+      <c r="D44" s="65"/>
+      <c r="E44" s="65"/>
+      <c r="F44" s="65"/>
+      <c r="G44" s="65"/>
+      <c r="H44" s="65"/>
+      <c r="I44" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J44" s="78"/>
-      <c r="K44" s="78"/>
-      <c r="L44" s="74"/>
-      <c r="M44" s="74"/>
-      <c r="N44" s="78"/>
+      <c r="J44" s="82"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="2"/>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B45" s="59"/>
-      <c r="C45" s="76"/>
-      <c r="D45" s="69"/>
-      <c r="E45" s="69"/>
-      <c r="F45" s="69"/>
-      <c r="G45" s="69"/>
-      <c r="H45" s="70"/>
-      <c r="I45" s="7"/>
-      <c r="J45" s="8" t="s">
+      <c r="B45" s="11">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="C45" s="72"/>
+      <c r="D45" s="65"/>
+      <c r="E45" s="65"/>
+      <c r="F45" s="65"/>
+      <c r="G45" s="65"/>
+      <c r="H45" s="65"/>
+      <c r="I45" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="K45" s="8"/>
-      <c r="L45" s="102"/>
-      <c r="M45" s="102"/>
-      <c r="N45" s="49"/>
+      <c r="J45" s="82"/>
+      <c r="K45" s="93"/>
+      <c r="L45" s="93"/>
+      <c r="M45" s="45"/>
+      <c r="N45" s="2"/>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B46" s="59"/>
-      <c r="C46" s="76"/>
-      <c r="D46" s="69"/>
-      <c r="E46" s="69"/>
-      <c r="F46" s="69"/>
-      <c r="G46" s="69"/>
-      <c r="H46" s="70"/>
-      <c r="I46" s="7"/>
-      <c r="J46" s="8" t="s">
+      <c r="B46" s="11">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="C46" s="72"/>
+      <c r="D46" s="65"/>
+      <c r="E46" s="65"/>
+      <c r="F46" s="65"/>
+      <c r="G46" s="65"/>
+      <c r="H46" s="65"/>
+      <c r="I46" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="K46" s="4"/>
-      <c r="L46" s="100"/>
-      <c r="M46" s="100"/>
-      <c r="N46" s="49"/>
+      <c r="J46" s="82"/>
+      <c r="K46" s="93"/>
+      <c r="L46" s="93"/>
+      <c r="M46" s="45"/>
+      <c r="N46" s="2"/>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B47" s="60"/>
-      <c r="C47" s="77"/>
-      <c r="D47" s="71"/>
-      <c r="E47" s="71"/>
-      <c r="F47" s="71"/>
-      <c r="G47" s="71"/>
-      <c r="H47" s="72"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="8" t="s">
+      <c r="B47" s="11">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="C47" s="73"/>
+      <c r="D47" s="67"/>
+      <c r="E47" s="67"/>
+      <c r="F47" s="67"/>
+      <c r="G47" s="67"/>
+      <c r="H47" s="67"/>
+      <c r="I47" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K47" s="10"/>
-      <c r="L47" s="87"/>
-      <c r="M47" s="87"/>
-      <c r="N47" s="49" t="s">
+      <c r="J47" s="83"/>
+      <c r="K47" s="83"/>
+      <c r="L47" s="83"/>
+      <c r="M47" s="45" t="s">
         <v>36</v>
       </c>
+      <c r="N47" s="2"/>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B48" s="11">
-        <f>B43+1</f>
-        <v>31</v>
-      </c>
-      <c r="C48" s="77" t="s">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="C48" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="D48" s="71"/>
-      <c r="E48" s="71"/>
-      <c r="F48" s="71"/>
-      <c r="G48" s="71"/>
-      <c r="H48" s="53"/>
-      <c r="I48" s="79" t="s">
+      <c r="D48" s="67"/>
+      <c r="E48" s="67"/>
+      <c r="F48" s="67"/>
+      <c r="G48" s="67"/>
+      <c r="H48" s="48"/>
+      <c r="I48" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J48" s="80"/>
-      <c r="K48" s="19"/>
-      <c r="L48" s="103"/>
-      <c r="M48" s="103"/>
-      <c r="N48" s="92"/>
+      <c r="J48" s="82"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="93"/>
+      <c r="N48" s="2"/>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B49" s="58">
-        <f t="shared" si="1"/>
-        <v>32</v>
-      </c>
-      <c r="C49" s="61"/>
-      <c r="D49" s="67" t="s">
+      <c r="B49" s="11">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="C49" s="57"/>
+      <c r="D49" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="E49" s="67"/>
-      <c r="F49" s="67"/>
-      <c r="G49" s="67"/>
-      <c r="H49" s="68"/>
-      <c r="I49" s="73" t="s">
+      <c r="E49" s="63"/>
+      <c r="F49" s="63"/>
+      <c r="G49" s="63"/>
+      <c r="H49" s="63"/>
+      <c r="I49" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J49" s="54"/>
+      <c r="J49" s="82"/>
       <c r="K49" s="4"/>
-      <c r="L49" s="100"/>
-      <c r="M49" s="100"/>
-      <c r="N49" s="49"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="93"/>
+      <c r="N49" s="2"/>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B50" s="60"/>
-      <c r="C50" s="65"/>
-      <c r="D50" s="71"/>
-      <c r="E50" s="71"/>
-      <c r="F50" s="71"/>
-      <c r="G50" s="71"/>
-      <c r="H50" s="72"/>
-      <c r="I50" s="73" t="s">
+      <c r="B50" s="11">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="C50" s="61"/>
+      <c r="D50" s="67"/>
+      <c r="E50" s="67"/>
+      <c r="F50" s="67"/>
+      <c r="G50" s="67"/>
+      <c r="H50" s="67"/>
+      <c r="I50" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J50" s="54"/>
+      <c r="J50" s="82"/>
       <c r="K50" s="4"/>
-      <c r="L50" s="100"/>
-      <c r="M50" s="100"/>
-      <c r="N50" s="49"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="93"/>
+      <c r="N50" s="2"/>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B51" s="11">
-        <f>B49+1</f>
-        <v>33</v>
+        <f t="shared" si="0"/>
+        <v>45</v>
       </c>
       <c r="C51" s="5"/>
-      <c r="D51" s="52" t="s">
+      <c r="D51" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E51" s="52"/>
-      <c r="F51" s="52"/>
-      <c r="G51" s="52"/>
-      <c r="H51" s="53"/>
-      <c r="I51" s="50"/>
-      <c r="J51" s="74"/>
-      <c r="K51" s="74"/>
-      <c r="L51" s="74"/>
-      <c r="M51" s="74"/>
-      <c r="N51" s="74"/>
+      <c r="E51" s="48"/>
+      <c r="F51" s="48"/>
+      <c r="G51" s="48"/>
+      <c r="H51" s="48"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="82"/>
+      <c r="K51" s="4"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="4"/>
+      <c r="N51" s="2"/>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B52" s="58">
-        <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="C52" s="61"/>
-      <c r="D52" s="62"/>
-      <c r="E52" s="67" t="s">
+      <c r="B52" s="11">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="C52" s="57"/>
+      <c r="D52" s="58"/>
+      <c r="E52" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="F52" s="67"/>
-      <c r="G52" s="67"/>
-      <c r="H52" s="68"/>
-      <c r="I52" s="73" t="s">
+      <c r="F52" s="63"/>
+      <c r="G52" s="63"/>
+      <c r="H52" s="63"/>
+      <c r="I52" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J52" s="54"/>
+      <c r="J52" s="82"/>
       <c r="K52" s="4"/>
-      <c r="L52" s="100"/>
-      <c r="M52" s="100"/>
-      <c r="N52" s="49"/>
+      <c r="L52" s="4"/>
+      <c r="M52" s="93"/>
+      <c r="N52" s="2"/>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B53" s="59"/>
-      <c r="C53" s="63"/>
-      <c r="D53" s="64"/>
-      <c r="E53" s="69"/>
-      <c r="F53" s="69"/>
-      <c r="G53" s="69"/>
-      <c r="H53" s="70"/>
-      <c r="I53" s="73" t="s">
+      <c r="B53" s="11">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="C53" s="59"/>
+      <c r="D53" s="60"/>
+      <c r="E53" s="65"/>
+      <c r="F53" s="65"/>
+      <c r="G53" s="65"/>
+      <c r="H53" s="65"/>
+      <c r="I53" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J53" s="54"/>
+      <c r="J53" s="82"/>
       <c r="K53" s="20"/>
-      <c r="L53" s="88"/>
-      <c r="M53" s="88"/>
-      <c r="N53" s="93" t="s">
+      <c r="L53" s="20"/>
+      <c r="M53" s="86" t="s">
         <v>28</v>
       </c>
+      <c r="N53" s="2"/>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B54" s="59"/>
-      <c r="C54" s="63"/>
-      <c r="D54" s="64"/>
-      <c r="E54" s="69"/>
-      <c r="F54" s="69"/>
-      <c r="G54" s="69"/>
-      <c r="H54" s="70"/>
-      <c r="I54" s="73" t="s">
+      <c r="B54" s="11">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="C54" s="59"/>
+      <c r="D54" s="60"/>
+      <c r="E54" s="65"/>
+      <c r="F54" s="65"/>
+      <c r="G54" s="65"/>
+      <c r="H54" s="65"/>
+      <c r="I54" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J54" s="54"/>
+      <c r="J54" s="82"/>
       <c r="K54" s="4"/>
-      <c r="L54" s="100"/>
-      <c r="M54" s="100"/>
-      <c r="N54" s="49"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="45"/>
+      <c r="N54" s="2"/>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B55" s="60"/>
-      <c r="C55" s="65"/>
-      <c r="D55" s="66"/>
-      <c r="E55" s="71"/>
-      <c r="F55" s="71"/>
-      <c r="G55" s="71"/>
-      <c r="H55" s="72"/>
-      <c r="I55" s="73" t="s">
+      <c r="B55" s="11">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="C55" s="61"/>
+      <c r="D55" s="62"/>
+      <c r="E55" s="67"/>
+      <c r="F55" s="67"/>
+      <c r="G55" s="67"/>
+      <c r="H55" s="67"/>
+      <c r="I55" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="J55" s="54"/>
+      <c r="J55" s="82"/>
       <c r="K55" s="20"/>
-      <c r="L55" s="88"/>
-      <c r="M55" s="88"/>
-      <c r="N55" s="93" t="s">
+      <c r="L55" s="20"/>
+      <c r="M55" s="86" t="s">
         <v>29</v>
       </c>
+      <c r="N55" s="2"/>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B56" s="11">
-        <f>B52+1</f>
-        <v>35</v>
+        <f t="shared" si="0"/>
+        <v>50</v>
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="9"/>
       <c r="E56" s="9"/>
-      <c r="F56" s="52" t="s">
+      <c r="F56" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="G56" s="52"/>
-      <c r="H56" s="53"/>
-      <c r="I56" s="73" t="s">
+      <c r="G56" s="48"/>
+      <c r="H56" s="48"/>
+      <c r="I56" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J56" s="54"/>
+      <c r="J56" s="82"/>
       <c r="K56" s="4"/>
-      <c r="L56" s="100"/>
-      <c r="M56" s="100"/>
-      <c r="N56" s="49"/>
+      <c r="L56" s="4"/>
+      <c r="M56" s="93"/>
+      <c r="N56" s="2"/>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B57" s="58">
-        <f t="shared" si="1"/>
-        <v>36</v>
-      </c>
-      <c r="C57" s="61"/>
-      <c r="D57" s="62"/>
-      <c r="E57" s="67" t="s">
+      <c r="B57" s="11">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="C57" s="57"/>
+      <c r="D57" s="58"/>
+      <c r="E57" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="F57" s="67"/>
-      <c r="G57" s="67"/>
-      <c r="H57" s="68"/>
-      <c r="I57" s="73" t="s">
+      <c r="F57" s="63"/>
+      <c r="G57" s="63"/>
+      <c r="H57" s="63"/>
+      <c r="I57" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J57" s="54"/>
+      <c r="J57" s="82"/>
       <c r="K57" s="4"/>
-      <c r="L57" s="100"/>
-      <c r="M57" s="100"/>
-      <c r="N57" s="49"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="93"/>
+      <c r="N57" s="2"/>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B58" s="59"/>
-      <c r="C58" s="63"/>
-      <c r="D58" s="64"/>
-      <c r="E58" s="69"/>
-      <c r="F58" s="69"/>
-      <c r="G58" s="69"/>
-      <c r="H58" s="70"/>
-      <c r="I58" s="73" t="s">
+      <c r="B58" s="11">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="C58" s="59"/>
+      <c r="D58" s="60"/>
+      <c r="E58" s="65"/>
+      <c r="F58" s="65"/>
+      <c r="G58" s="65"/>
+      <c r="H58" s="65"/>
+      <c r="I58" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J58" s="54"/>
+      <c r="J58" s="82"/>
       <c r="K58" s="4"/>
-      <c r="L58" s="100"/>
-      <c r="M58" s="100"/>
-      <c r="N58" s="49"/>
+      <c r="L58" s="4"/>
+      <c r="M58" s="93"/>
+      <c r="N58" s="2"/>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B59" s="59"/>
-      <c r="C59" s="63"/>
-      <c r="D59" s="64"/>
-      <c r="E59" s="69"/>
-      <c r="F59" s="69"/>
-      <c r="G59" s="69"/>
-      <c r="H59" s="70"/>
-      <c r="I59" s="73" t="s">
+      <c r="B59" s="11">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="C59" s="59"/>
+      <c r="D59" s="60"/>
+      <c r="E59" s="65"/>
+      <c r="F59" s="65"/>
+      <c r="G59" s="65"/>
+      <c r="H59" s="65"/>
+      <c r="I59" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="J59" s="54"/>
+      <c r="J59" s="82"/>
       <c r="K59" s="4"/>
-      <c r="L59" s="100"/>
-      <c r="M59" s="100"/>
-      <c r="N59" s="49"/>
+      <c r="L59" s="4"/>
+      <c r="M59" s="93"/>
+      <c r="N59" s="2"/>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B60" s="59"/>
-      <c r="C60" s="63"/>
-      <c r="D60" s="64"/>
-      <c r="E60" s="69"/>
-      <c r="F60" s="69"/>
-      <c r="G60" s="69"/>
-      <c r="H60" s="70"/>
-      <c r="I60" s="73" t="s">
+      <c r="B60" s="11">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="C60" s="59"/>
+      <c r="D60" s="60"/>
+      <c r="E60" s="65"/>
+      <c r="F60" s="65"/>
+      <c r="G60" s="65"/>
+      <c r="H60" s="65"/>
+      <c r="I60" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J60" s="54"/>
+      <c r="J60" s="82"/>
       <c r="K60" s="4"/>
-      <c r="L60" s="100"/>
-      <c r="M60" s="100"/>
-      <c r="N60" s="49"/>
+      <c r="L60" s="4"/>
+      <c r="M60" s="93"/>
+      <c r="N60" s="2"/>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B61" s="60"/>
-      <c r="C61" s="63"/>
-      <c r="D61" s="64"/>
-      <c r="E61" s="69"/>
-      <c r="F61" s="69"/>
-      <c r="G61" s="69"/>
-      <c r="H61" s="70"/>
-      <c r="I61" s="73" t="s">
+      <c r="B61" s="11">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="C61" s="59"/>
+      <c r="D61" s="60"/>
+      <c r="E61" s="65"/>
+      <c r="F61" s="65"/>
+      <c r="G61" s="65"/>
+      <c r="H61" s="65"/>
+      <c r="I61" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="J61" s="54"/>
+      <c r="J61" s="82"/>
       <c r="K61" s="4"/>
-      <c r="L61" s="100"/>
-      <c r="M61" s="100"/>
-      <c r="N61" s="49"/>
+      <c r="L61" s="4"/>
+      <c r="M61" s="93"/>
+      <c r="N61" s="2"/>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B62" s="58">
-        <f>B57+1</f>
-        <v>37</v>
-      </c>
-      <c r="C62" s="61"/>
-      <c r="D62" s="62"/>
-      <c r="E62" s="62"/>
-      <c r="F62" s="67" t="s">
+      <c r="B62" s="11">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="C62" s="57"/>
+      <c r="D62" s="58"/>
+      <c r="E62" s="58"/>
+      <c r="F62" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="G62" s="67"/>
-      <c r="H62" s="68"/>
-      <c r="I62" s="54" t="s">
+      <c r="G62" s="63"/>
+      <c r="H62" s="63"/>
+      <c r="I62" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="J62" s="55"/>
+      <c r="J62" s="82"/>
       <c r="K62" s="4"/>
-      <c r="L62" s="100"/>
-      <c r="M62" s="100"/>
-      <c r="N62" s="49"/>
+      <c r="L62" s="4"/>
+      <c r="M62" s="93"/>
+      <c r="N62" s="2"/>
     </row>
     <row r="63" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B63" s="59"/>
-      <c r="C63" s="63"/>
-      <c r="D63" s="64"/>
-      <c r="E63" s="64"/>
-      <c r="F63" s="69"/>
-      <c r="G63" s="69"/>
-      <c r="H63" s="70"/>
-      <c r="I63" s="73" t="s">
+      <c r="B63" s="11">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="C63" s="59"/>
+      <c r="D63" s="60"/>
+      <c r="E63" s="60"/>
+      <c r="F63" s="65"/>
+      <c r="G63" s="65"/>
+      <c r="H63" s="65"/>
+      <c r="I63" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="J63" s="54"/>
+      <c r="J63" s="82"/>
       <c r="K63" s="4"/>
-      <c r="L63" s="100"/>
-      <c r="M63" s="100"/>
-      <c r="N63" s="49"/>
+      <c r="L63" s="4"/>
+      <c r="M63" s="93"/>
+      <c r="N63" s="2"/>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B64" s="59"/>
-      <c r="C64" s="63"/>
-      <c r="D64" s="64"/>
-      <c r="E64" s="64"/>
-      <c r="F64" s="69"/>
-      <c r="G64" s="69"/>
-      <c r="H64" s="70"/>
-      <c r="I64" s="73" t="s">
+      <c r="B64" s="11">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="C64" s="59"/>
+      <c r="D64" s="60"/>
+      <c r="E64" s="60"/>
+      <c r="F64" s="65"/>
+      <c r="G64" s="65"/>
+      <c r="H64" s="65"/>
+      <c r="I64" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J64" s="54"/>
+      <c r="J64" s="82"/>
       <c r="K64" s="4"/>
-      <c r="L64" s="100"/>
-      <c r="M64" s="100"/>
-      <c r="N64" s="49"/>
+      <c r="L64" s="4"/>
+      <c r="M64" s="93"/>
+      <c r="N64" s="2"/>
     </row>
     <row r="65" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B65" s="60"/>
-      <c r="C65" s="65"/>
-      <c r="D65" s="66"/>
-      <c r="E65" s="66"/>
-      <c r="F65" s="71"/>
-      <c r="G65" s="71"/>
-      <c r="H65" s="72"/>
-      <c r="I65" s="73" t="s">
+      <c r="B65" s="11">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="C65" s="61"/>
+      <c r="D65" s="62"/>
+      <c r="E65" s="62"/>
+      <c r="F65" s="67"/>
+      <c r="G65" s="67"/>
+      <c r="H65" s="67"/>
+      <c r="I65" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="J65" s="54"/>
+      <c r="J65" s="82"/>
       <c r="K65" s="10"/>
-      <c r="L65" s="87"/>
-      <c r="M65" s="87"/>
-      <c r="N65" s="49" t="s">
+      <c r="L65" s="10"/>
+      <c r="M65" s="45" t="s">
         <v>59</v>
       </c>
+      <c r="N65" s="2"/>
     </row>
     <row r="66" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B66" s="22">
-        <f>B62+1</f>
-        <v>38</v>
+      <c r="B66" s="11">
+        <f t="shared" si="0"/>
+        <v>60</v>
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="9"/>
       <c r="E66" s="9"/>
       <c r="F66" s="9"/>
-      <c r="G66" s="52" t="s">
+      <c r="G66" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="H66" s="53"/>
-      <c r="I66" s="54" t="s">
+      <c r="H66" s="48"/>
+      <c r="I66" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="J66" s="55"/>
+      <c r="J66" s="82"/>
       <c r="K66" s="4"/>
-      <c r="L66" s="100"/>
-      <c r="M66" s="100"/>
-      <c r="N66" s="49"/>
+      <c r="L66" s="4"/>
+      <c r="M66" s="93"/>
+      <c r="N66" s="2"/>
     </row>
     <row r="67" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B67" s="22">
-        <f t="shared" ref="B67:B77" si="2">B66+1</f>
-        <v>39</v>
-      </c>
-      <c r="C67" s="56"/>
-      <c r="D67" s="57"/>
-      <c r="E67" s="57"/>
-      <c r="F67" s="57"/>
-      <c r="G67" s="52" t="s">
+      <c r="B67" s="11">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="C67" s="52"/>
+      <c r="D67" s="53"/>
+      <c r="E67" s="53"/>
+      <c r="F67" s="53"/>
+      <c r="G67" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="H67" s="53"/>
-      <c r="I67" s="50"/>
-      <c r="J67" s="51"/>
+      <c r="H67" s="48"/>
+      <c r="I67" s="4"/>
+      <c r="J67" s="82"/>
       <c r="K67" s="4"/>
-      <c r="L67" s="100"/>
-      <c r="M67" s="100"/>
-      <c r="N67" s="49"/>
+      <c r="L67" s="4"/>
+      <c r="M67" s="93"/>
+      <c r="N67" s="2"/>
     </row>
     <row r="68" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B68" s="22">
-        <f t="shared" si="2"/>
-        <v>40</v>
+      <c r="B68" s="11">
+        <f t="shared" si="0"/>
+        <v>62</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="9"/>
       <c r="E68" s="9"/>
       <c r="F68" s="9"/>
       <c r="G68" s="9"/>
-      <c r="H68" s="6"/>
-      <c r="I68" s="50"/>
-      <c r="J68" s="51"/>
+      <c r="H68" s="9"/>
+      <c r="I68" s="4"/>
+      <c r="J68" s="82"/>
       <c r="K68" s="4"/>
-      <c r="L68" s="100"/>
-      <c r="M68" s="100"/>
-      <c r="N68" s="49"/>
+      <c r="L68" s="4"/>
+      <c r="M68" s="93"/>
+      <c r="N68" s="2"/>
     </row>
     <row r="69" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B69" s="22">
-        <f t="shared" si="2"/>
-        <v>41</v>
+      <c r="B69" s="11">
+        <f t="shared" si="0"/>
+        <v>63</v>
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="9"/>
       <c r="E69" s="9"/>
       <c r="F69" s="9"/>
       <c r="G69" s="9"/>
-      <c r="H69" s="6"/>
-      <c r="I69" s="50"/>
-      <c r="J69" s="51"/>
+      <c r="H69" s="9"/>
+      <c r="I69" s="4"/>
+      <c r="J69" s="82"/>
       <c r="K69" s="4"/>
-      <c r="L69" s="100"/>
-      <c r="M69" s="100"/>
-      <c r="N69" s="49"/>
+      <c r="L69" s="4"/>
+      <c r="M69" s="93"/>
+      <c r="N69" s="2"/>
     </row>
     <row r="70" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B70" s="22">
-        <f t="shared" si="2"/>
-        <v>42</v>
+      <c r="B70" s="11">
+        <f t="shared" si="0"/>
+        <v>64</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="9"/>
       <c r="E70" s="9"/>
       <c r="F70" s="9"/>
       <c r="G70" s="9"/>
-      <c r="H70" s="6"/>
-      <c r="I70" s="50"/>
-      <c r="J70" s="51"/>
+      <c r="H70" s="9"/>
+      <c r="I70" s="4"/>
+      <c r="J70" s="82"/>
       <c r="K70" s="4"/>
-      <c r="L70" s="100"/>
-      <c r="M70" s="100"/>
-      <c r="N70" s="49"/>
+      <c r="L70" s="4"/>
+      <c r="M70" s="93"/>
+      <c r="N70" s="2"/>
     </row>
     <row r="71" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B71" s="22">
-        <f t="shared" si="2"/>
-        <v>43</v>
+      <c r="B71" s="11">
+        <f t="shared" si="0"/>
+        <v>65</v>
       </c>
       <c r="C71" s="5"/>
       <c r="D71" s="9"/>
       <c r="E71" s="9"/>
       <c r="F71" s="9"/>
       <c r="G71" s="9"/>
-      <c r="H71" s="6"/>
-      <c r="I71" s="50"/>
-      <c r="J71" s="51"/>
+      <c r="H71" s="9"/>
+      <c r="I71" s="4"/>
+      <c r="J71" s="82"/>
       <c r="K71" s="4"/>
-      <c r="L71" s="100"/>
-      <c r="M71" s="100"/>
-      <c r="N71" s="49"/>
+      <c r="L71" s="4"/>
+      <c r="M71" s="93"/>
+      <c r="N71" s="2"/>
     </row>
     <row r="72" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B72" s="22">
-        <f t="shared" si="2"/>
-        <v>44</v>
+      <c r="B72" s="11">
+        <f t="shared" si="0"/>
+        <v>66</v>
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="9"/>
       <c r="E72" s="9"/>
       <c r="F72" s="9"/>
       <c r="G72" s="9"/>
-      <c r="H72" s="6"/>
-      <c r="I72" s="50"/>
-      <c r="J72" s="51"/>
+      <c r="H72" s="9"/>
+      <c r="I72" s="4"/>
+      <c r="J72" s="82"/>
       <c r="K72" s="4"/>
-      <c r="L72" s="100"/>
-      <c r="M72" s="100"/>
-      <c r="N72" s="49"/>
+      <c r="L72" s="4"/>
+      <c r="M72" s="93"/>
+      <c r="N72" s="2"/>
     </row>
     <row r="73" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B73" s="22">
-        <f t="shared" si="2"/>
-        <v>45</v>
+      <c r="B73" s="11">
+        <f t="shared" ref="B73:B77" si="1">B72+1</f>
+        <v>67</v>
       </c>
       <c r="C73" s="5"/>
       <c r="D73" s="9"/>
       <c r="E73" s="9"/>
       <c r="F73" s="9"/>
       <c r="G73" s="9"/>
-      <c r="H73" s="6"/>
-      <c r="I73" s="50"/>
-      <c r="J73" s="51"/>
+      <c r="H73" s="9"/>
+      <c r="I73" s="4"/>
+      <c r="J73" s="82"/>
       <c r="K73" s="4"/>
-      <c r="L73" s="100"/>
-      <c r="M73" s="100"/>
-      <c r="N73" s="49"/>
+      <c r="L73" s="4"/>
+      <c r="M73" s="93"/>
+      <c r="N73" s="2"/>
     </row>
     <row r="74" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B74" s="22">
-        <f t="shared" si="2"/>
-        <v>46</v>
+      <c r="B74" s="11">
+        <f t="shared" si="1"/>
+        <v>68</v>
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="9"/>
       <c r="E74" s="9"/>
       <c r="F74" s="9"/>
       <c r="G74" s="9"/>
-      <c r="H74" s="6"/>
-      <c r="I74" s="50"/>
-      <c r="J74" s="51"/>
+      <c r="H74" s="9"/>
+      <c r="I74" s="4"/>
+      <c r="J74" s="82"/>
       <c r="K74" s="4"/>
-      <c r="L74" s="100"/>
-      <c r="M74" s="100"/>
-      <c r="N74" s="49"/>
+      <c r="L74" s="4"/>
+      <c r="M74" s="93"/>
+      <c r="N74" s="2"/>
     </row>
     <row r="75" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B75" s="22">
-        <f t="shared" si="2"/>
-        <v>47</v>
+      <c r="B75" s="11">
+        <f t="shared" si="1"/>
+        <v>69</v>
       </c>
       <c r="C75" s="5"/>
       <c r="D75" s="9"/>
       <c r="E75" s="9"/>
       <c r="F75" s="9"/>
       <c r="G75" s="9"/>
-      <c r="H75" s="6"/>
-      <c r="I75" s="50"/>
-      <c r="J75" s="51"/>
+      <c r="H75" s="9"/>
+      <c r="I75" s="4"/>
+      <c r="J75" s="82"/>
       <c r="K75" s="4"/>
-      <c r="L75" s="100"/>
-      <c r="M75" s="100"/>
-      <c r="N75" s="49"/>
+      <c r="L75" s="4"/>
+      <c r="M75" s="93"/>
+      <c r="N75" s="2"/>
     </row>
     <row r="76" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B76" s="22">
-        <f t="shared" si="2"/>
-        <v>48</v>
+      <c r="B76" s="11">
+        <f t="shared" si="1"/>
+        <v>70</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="9"/>
       <c r="E76" s="9"/>
       <c r="F76" s="9"/>
       <c r="G76" s="9"/>
-      <c r="H76" s="6"/>
-      <c r="I76" s="50"/>
-      <c r="J76" s="51"/>
+      <c r="H76" s="9"/>
+      <c r="I76" s="4"/>
+      <c r="J76" s="82"/>
       <c r="K76" s="4"/>
-      <c r="L76" s="100"/>
-      <c r="M76" s="100"/>
-      <c r="N76" s="49"/>
+      <c r="L76" s="4"/>
+      <c r="M76" s="93"/>
+      <c r="N76" s="2"/>
     </row>
     <row r="77" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B77" s="22">
-        <f t="shared" si="2"/>
-        <v>49</v>
+      <c r="B77" s="11">
+        <f t="shared" si="1"/>
+        <v>71</v>
       </c>
       <c r="C77" s="5"/>
       <c r="D77" s="9"/>
       <c r="E77" s="9"/>
       <c r="F77" s="9"/>
       <c r="G77" s="9"/>
-      <c r="H77" s="6"/>
-      <c r="I77" s="50"/>
-      <c r="J77" s="51"/>
+      <c r="H77" s="9"/>
+      <c r="I77" s="4"/>
+      <c r="J77" s="82"/>
       <c r="K77" s="4"/>
-      <c r="L77" s="100"/>
-      <c r="M77" s="100"/>
-      <c r="N77" s="49"/>
+      <c r="L77" s="4"/>
+      <c r="M77" s="93"/>
+      <c r="N77" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="102">
+  <mergeCells count="41">
     <mergeCell ref="B4:E4"/>
-    <mergeCell ref="M10:M13"/>
-    <mergeCell ref="B17:N17"/>
-    <mergeCell ref="N10:N15"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K10:K13"/>
+    <mergeCell ref="M10:M15"/>
+    <mergeCell ref="K6:L6"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="I76:J76"/>
-    <mergeCell ref="I77:J77"/>
     <mergeCell ref="C7:H7"/>
-    <mergeCell ref="I7:J7"/>
     <mergeCell ref="D8:H8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I69:J69"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="I71:J71"/>
-    <mergeCell ref="I72:J72"/>
-    <mergeCell ref="I73:J73"/>
-    <mergeCell ref="I74:J74"/>
     <mergeCell ref="G66:H66"/>
-    <mergeCell ref="I66:J66"/>
     <mergeCell ref="C67:F67"/>
     <mergeCell ref="G67:H67"/>
-    <mergeCell ref="I67:J67"/>
-    <mergeCell ref="I68:J68"/>
-    <mergeCell ref="B62:B65"/>
     <mergeCell ref="C62:E65"/>
     <mergeCell ref="F62:H65"/>
-    <mergeCell ref="I62:J62"/>
-    <mergeCell ref="I63:J63"/>
-    <mergeCell ref="I64:J64"/>
-    <mergeCell ref="I65:J65"/>
     <mergeCell ref="F56:H56"/>
-    <mergeCell ref="I56:J56"/>
-    <mergeCell ref="B57:B61"/>
     <mergeCell ref="C57:D61"/>
     <mergeCell ref="E57:H61"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="I60:J60"/>
-    <mergeCell ref="I61:J61"/>
-    <mergeCell ref="B52:B55"/>
     <mergeCell ref="C52:D55"/>
     <mergeCell ref="E52:H55"/>
-    <mergeCell ref="I52:J52"/>
-    <mergeCell ref="I53:J53"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="B49:B50"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="D49:H50"/>
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="I50:J50"/>
     <mergeCell ref="D51:H51"/>
-    <mergeCell ref="I51:N51"/>
-    <mergeCell ref="B43:B47"/>
     <mergeCell ref="C43:E47"/>
     <mergeCell ref="F43:H47"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="I44:N44"/>
     <mergeCell ref="C48:H48"/>
-    <mergeCell ref="I48:J48"/>
     <mergeCell ref="F40:H40"/>
-    <mergeCell ref="B41:B42"/>
     <mergeCell ref="C41:E42"/>
     <mergeCell ref="F41:H42"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="I42:J42"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="E37:H37"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="B38:B39"/>
     <mergeCell ref="C38:E39"/>
     <mergeCell ref="F38:H39"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="I30:J30"/>
     <mergeCell ref="E31:H31"/>
-    <mergeCell ref="I31:J31"/>
     <mergeCell ref="C32:E36"/>
     <mergeCell ref="F32:H36"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:N33"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="D26:H27"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I27:J27"/>
     <mergeCell ref="C28:C30"/>
     <mergeCell ref="D28:H30"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="I29:J29"/>
     <mergeCell ref="C21:H21"/>
-    <mergeCell ref="I21:J21"/>
     <mergeCell ref="C24:H25"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="I23:J23"/>
     <mergeCell ref="D22:H22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3079,18 +3004,18 @@
       <c r="B5" s="11">
         <v>1</v>
       </c>
-      <c r="C5" s="83" t="s">
+      <c r="C5" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="73" t="s">
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="54"/>
+      <c r="J5" s="50"/>
       <c r="K5" s="4" t="s">
         <v>6</v>
       </c>
@@ -3101,14 +3026,14 @@
         <f>B5+1</f>
         <v>2</v>
       </c>
-      <c r="C6" s="83" t="s">
+      <c r="C6" s="79" t="s">
         <v>86</v>
       </c>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="53"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="49"/>
       <c r="I6" s="23"/>
       <c r="J6" s="24"/>
       <c r="K6" s="10" t="s">
@@ -3117,22 +3042,22 @@
       <c r="L6" s="4"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="58">
+      <c r="B7" s="54">
         <f>B6+1</f>
         <v>3</v>
       </c>
-      <c r="C7" s="75" t="s">
+      <c r="C7" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="68"/>
-      <c r="I7" s="73" t="s">
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="54"/>
+      <c r="J7" s="50"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="N7" s="20" t="s">
@@ -3140,17 +3065,17 @@
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="60"/>
-      <c r="C8" s="77"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="71"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="73" t="s">
+      <c r="B8" s="56"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="J8" s="54"/>
+      <c r="J8" s="50"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="N8" s="4" t="s">
@@ -3158,22 +3083,22 @@
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="58">
+      <c r="B9" s="54">
         <f>B7+1</f>
         <v>4</v>
       </c>
-      <c r="C9" s="61"/>
-      <c r="D9" s="67" t="s">
+      <c r="C9" s="57"/>
+      <c r="D9" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="68"/>
-      <c r="I9" s="73" t="s">
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="54"/>
+      <c r="J9" s="50"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="N9" s="10" t="s">
@@ -3181,67 +3106,67 @@
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="60"/>
-      <c r="C10" s="65"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="71"/>
-      <c r="H10" s="72"/>
-      <c r="I10" s="73" t="s">
+      <c r="B10" s="56"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="67"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="J10" s="54"/>
+      <c r="J10" s="50"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="58">
+      <c r="B11" s="54">
         <f>B9+1</f>
         <v>5</v>
       </c>
-      <c r="C11" s="61"/>
-      <c r="D11" s="67" t="s">
+      <c r="C11" s="57"/>
+      <c r="D11" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="68"/>
-      <c r="I11" s="73" t="s">
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="54"/>
+      <c r="J11" s="50"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="59"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="69"/>
-      <c r="H12" s="70"/>
-      <c r="I12" s="73" t="s">
+      <c r="B12" s="55"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="66"/>
+      <c r="I12" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="J12" s="54"/>
+      <c r="J12" s="50"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="60"/>
-      <c r="C13" s="65"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="71"/>
-      <c r="H13" s="72"/>
-      <c r="I13" s="73" t="s">
+      <c r="B13" s="56"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="J13" s="54"/>
+      <c r="J13" s="50"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
     </row>
@@ -3252,62 +3177,62 @@
       </c>
       <c r="C14" s="26"/>
       <c r="D14" s="25"/>
-      <c r="E14" s="52" t="s">
+      <c r="E14" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="73" t="s">
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="J14" s="54"/>
+      <c r="J14" s="50"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="58">
+      <c r="B15" s="54">
         <f>B14+1</f>
         <v>7</v>
       </c>
-      <c r="C15" s="61"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="67" t="s">
+      <c r="C15" s="57"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="67"/>
-      <c r="H15" s="68"/>
-      <c r="I15" s="73" t="s">
+      <c r="G15" s="63"/>
+      <c r="H15" s="64"/>
+      <c r="I15" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="J15" s="54"/>
+      <c r="J15" s="50"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="59"/>
-      <c r="C16" s="63"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="69"/>
-      <c r="G16" s="69"/>
-      <c r="H16" s="70"/>
-      <c r="I16" s="73" t="s">
+      <c r="B16" s="55"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="66"/>
+      <c r="I16" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="J16" s="78"/>
-      <c r="K16" s="78"/>
-      <c r="L16" s="78"/>
+      <c r="J16" s="74"/>
+      <c r="K16" s="74"/>
+      <c r="L16" s="74"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="59"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="69"/>
-      <c r="H17" s="70"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="66"/>
       <c r="I17" s="7"/>
       <c r="J17" s="8" t="s">
         <v>32</v>
@@ -3316,13 +3241,13 @@
       <c r="L17" s="4"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="59"/>
-      <c r="C18" s="63"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="69"/>
-      <c r="G18" s="69"/>
-      <c r="H18" s="70"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="66"/>
       <c r="I18" s="7"/>
       <c r="J18" s="8" t="s">
         <v>34</v>
@@ -3331,13 +3256,13 @@
       <c r="L18" s="4"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="60"/>
-      <c r="C19" s="65"/>
-      <c r="D19" s="66"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="71"/>
-      <c r="H19" s="72"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="68"/>
       <c r="I19" s="7"/>
       <c r="J19" s="8" t="s">
         <v>35</v>
@@ -3352,53 +3277,53 @@
         <f>B15+1</f>
         <v>8</v>
       </c>
-      <c r="C20" s="56"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="52" t="s">
+      <c r="C20" s="52"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="52"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="73" t="s">
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="J20" s="54"/>
+      <c r="J20" s="50"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="58">
+      <c r="B21" s="54">
         <f>B20+1</f>
         <v>9</v>
       </c>
-      <c r="C21" s="61"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="67" t="s">
+      <c r="C21" s="57"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="67"/>
-      <c r="H21" s="68"/>
-      <c r="I21" s="73" t="s">
+      <c r="G21" s="63"/>
+      <c r="H21" s="64"/>
+      <c r="I21" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="J21" s="54"/>
+      <c r="J21" s="50"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="60"/>
-      <c r="C22" s="65"/>
-      <c r="D22" s="66"/>
-      <c r="E22" s="66"/>
-      <c r="F22" s="71"/>
-      <c r="G22" s="71"/>
-      <c r="H22" s="72"/>
-      <c r="I22" s="73" t="s">
+      <c r="B22" s="56"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="68"/>
+      <c r="I22" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J22" s="54"/>
+      <c r="J22" s="50"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
     </row>
@@ -3410,96 +3335,96 @@
       <c r="C23" s="5"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
-      <c r="F23" s="52" t="s">
+      <c r="F23" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="G23" s="52"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="73" t="s">
+      <c r="G23" s="48"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="J23" s="54"/>
+      <c r="J23" s="50"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="58">
+      <c r="B24" s="54">
         <f t="shared" ref="B24:B40" si="0">B23+1</f>
         <v>11</v>
       </c>
-      <c r="C24" s="61"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="67" t="s">
+      <c r="C24" s="57"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="G24" s="67"/>
-      <c r="H24" s="68"/>
-      <c r="I24" s="81" t="s">
+      <c r="G24" s="63"/>
+      <c r="H24" s="64"/>
+      <c r="I24" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="J24" s="82"/>
+      <c r="J24" s="78"/>
       <c r="K24" s="18"/>
       <c r="L24" s="18"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="60"/>
-      <c r="C25" s="65"/>
-      <c r="D25" s="66"/>
-      <c r="E25" s="66"/>
-      <c r="F25" s="71"/>
-      <c r="G25" s="71"/>
-      <c r="H25" s="72"/>
-      <c r="I25" s="73" t="s">
+      <c r="B25" s="56"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="67"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="J25" s="54"/>
+      <c r="J25" s="50"/>
       <c r="K25" s="18"/>
       <c r="L25" s="18"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="58">
+      <c r="B26" s="54">
         <f>B24+1</f>
         <v>12</v>
       </c>
-      <c r="C26" s="75"/>
-      <c r="D26" s="67"/>
-      <c r="E26" s="67"/>
-      <c r="F26" s="67" t="s">
+      <c r="C26" s="71"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="G26" s="67"/>
-      <c r="H26" s="68"/>
-      <c r="I26" s="73" t="s">
+      <c r="G26" s="63"/>
+      <c r="H26" s="64"/>
+      <c r="I26" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="J26" s="54"/>
+      <c r="J26" s="50"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="59"/>
-      <c r="C27" s="76"/>
-      <c r="D27" s="69"/>
-      <c r="E27" s="69"/>
-      <c r="F27" s="69"/>
-      <c r="G27" s="69"/>
-      <c r="H27" s="70"/>
-      <c r="I27" s="73" t="s">
+      <c r="B27" s="55"/>
+      <c r="C27" s="72"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="66"/>
+      <c r="I27" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="J27" s="78"/>
-      <c r="K27" s="78"/>
-      <c r="L27" s="78"/>
+      <c r="J27" s="74"/>
+      <c r="K27" s="74"/>
+      <c r="L27" s="74"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="59"/>
-      <c r="C28" s="76"/>
-      <c r="D28" s="69"/>
-      <c r="E28" s="69"/>
-      <c r="F28" s="69"/>
-      <c r="G28" s="69"/>
-      <c r="H28" s="70"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="72"/>
+      <c r="D28" s="65"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="66"/>
       <c r="I28" s="7"/>
       <c r="J28" s="8" t="s">
         <v>32</v>
@@ -3508,13 +3433,13 @@
       <c r="L28" s="4"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="59"/>
-      <c r="C29" s="76"/>
-      <c r="D29" s="69"/>
-      <c r="E29" s="69"/>
-      <c r="F29" s="69"/>
-      <c r="G29" s="69"/>
-      <c r="H29" s="70"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="72"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="65"/>
+      <c r="F29" s="65"/>
+      <c r="G29" s="65"/>
+      <c r="H29" s="66"/>
       <c r="I29" s="7"/>
       <c r="J29" s="8" t="s">
         <v>34</v>
@@ -3523,13 +3448,13 @@
       <c r="L29" s="4"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B30" s="60"/>
-      <c r="C30" s="77"/>
-      <c r="D30" s="71"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="72"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="73"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="67"/>
+      <c r="H30" s="68"/>
       <c r="I30" s="7"/>
       <c r="J30" s="8" t="s">
         <v>35</v>
@@ -3544,53 +3469,53 @@
         <f>B26+1</f>
         <v>13</v>
       </c>
-      <c r="C31" s="77" t="s">
+      <c r="C31" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="71"/>
-      <c r="E31" s="71"/>
-      <c r="F31" s="71"/>
-      <c r="G31" s="71"/>
-      <c r="H31" s="53"/>
-      <c r="I31" s="79" t="s">
+      <c r="D31" s="67"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="67"/>
+      <c r="G31" s="67"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="J31" s="80"/>
+      <c r="J31" s="76"/>
       <c r="K31" s="19"/>
       <c r="L31" s="19"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="58">
+      <c r="B32" s="54">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C32" s="61"/>
-      <c r="D32" s="67" t="s">
+      <c r="C32" s="57"/>
+      <c r="D32" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="E32" s="67"/>
-      <c r="F32" s="67"/>
-      <c r="G32" s="67"/>
-      <c r="H32" s="68"/>
-      <c r="I32" s="73" t="s">
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="64"/>
+      <c r="I32" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="J32" s="54"/>
+      <c r="J32" s="50"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B33" s="60"/>
-      <c r="C33" s="65"/>
-      <c r="D33" s="71"/>
-      <c r="E33" s="71"/>
-      <c r="F33" s="71"/>
-      <c r="G33" s="71"/>
-      <c r="H33" s="72"/>
-      <c r="I33" s="73" t="s">
+      <c r="B33" s="56"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="67"/>
+      <c r="E33" s="67"/>
+      <c r="F33" s="67"/>
+      <c r="G33" s="67"/>
+      <c r="H33" s="68"/>
+      <c r="I33" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="J33" s="54"/>
+      <c r="J33" s="50"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
     </row>
@@ -3600,82 +3525,82 @@
         <v>15</v>
       </c>
       <c r="C34" s="5"/>
-      <c r="D34" s="52" t="s">
+      <c r="D34" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="52"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="52"/>
-      <c r="H34" s="53"/>
-      <c r="I34" s="50"/>
-      <c r="J34" s="74"/>
-      <c r="K34" s="74"/>
-      <c r="L34" s="74"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="46"/>
+      <c r="J34" s="70"/>
+      <c r="K34" s="70"/>
+      <c r="L34" s="70"/>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B35" s="58">
+      <c r="B35" s="54">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C35" s="61"/>
-      <c r="D35" s="62"/>
-      <c r="E35" s="67" t="s">
+      <c r="C35" s="57"/>
+      <c r="D35" s="58"/>
+      <c r="E35" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="F35" s="67"/>
-      <c r="G35" s="67"/>
-      <c r="H35" s="68"/>
-      <c r="I35" s="73" t="s">
+      <c r="F35" s="63"/>
+      <c r="G35" s="63"/>
+      <c r="H35" s="64"/>
+      <c r="I35" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="J35" s="54"/>
+      <c r="J35" s="50"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B36" s="59"/>
-      <c r="C36" s="63"/>
-      <c r="D36" s="64"/>
-      <c r="E36" s="69"/>
-      <c r="F36" s="69"/>
-      <c r="G36" s="69"/>
-      <c r="H36" s="70"/>
-      <c r="I36" s="73" t="s">
+      <c r="B36" s="55"/>
+      <c r="C36" s="59"/>
+      <c r="D36" s="60"/>
+      <c r="E36" s="65"/>
+      <c r="F36" s="65"/>
+      <c r="G36" s="65"/>
+      <c r="H36" s="66"/>
+      <c r="I36" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="J36" s="54"/>
+      <c r="J36" s="50"/>
       <c r="K36" s="20"/>
       <c r="L36" s="21" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B37" s="59"/>
-      <c r="C37" s="63"/>
-      <c r="D37" s="64"/>
-      <c r="E37" s="69"/>
-      <c r="F37" s="69"/>
-      <c r="G37" s="69"/>
-      <c r="H37" s="70"/>
-      <c r="I37" s="73" t="s">
+      <c r="B37" s="55"/>
+      <c r="C37" s="59"/>
+      <c r="D37" s="60"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
+      <c r="G37" s="65"/>
+      <c r="H37" s="66"/>
+      <c r="I37" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="J37" s="54"/>
+      <c r="J37" s="50"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B38" s="60"/>
-      <c r="C38" s="65"/>
-      <c r="D38" s="66"/>
-      <c r="E38" s="71"/>
-      <c r="F38" s="71"/>
-      <c r="G38" s="71"/>
-      <c r="H38" s="72"/>
-      <c r="I38" s="73" t="s">
+      <c r="B38" s="56"/>
+      <c r="C38" s="61"/>
+      <c r="D38" s="62"/>
+      <c r="E38" s="67"/>
+      <c r="F38" s="67"/>
+      <c r="G38" s="67"/>
+      <c r="H38" s="68"/>
+      <c r="I38" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="J38" s="54"/>
+      <c r="J38" s="50"/>
       <c r="K38" s="20"/>
       <c r="L38" s="21" t="s">
         <v>29</v>
@@ -3689,160 +3614,160 @@
       <c r="C39" s="5"/>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
-      <c r="F39" s="52" t="s">
+      <c r="F39" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="G39" s="52"/>
-      <c r="H39" s="53"/>
-      <c r="I39" s="73" t="s">
+      <c r="G39" s="48"/>
+      <c r="H39" s="49"/>
+      <c r="I39" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="J39" s="54"/>
+      <c r="J39" s="50"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B40" s="58">
+      <c r="B40" s="54">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C40" s="61"/>
-      <c r="D40" s="62"/>
-      <c r="E40" s="67" t="s">
+      <c r="C40" s="57"/>
+      <c r="D40" s="58"/>
+      <c r="E40" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="F40" s="67"/>
-      <c r="G40" s="67"/>
-      <c r="H40" s="68"/>
-      <c r="I40" s="73" t="s">
+      <c r="F40" s="63"/>
+      <c r="G40" s="63"/>
+      <c r="H40" s="64"/>
+      <c r="I40" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="J40" s="54"/>
+      <c r="J40" s="50"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B41" s="59"/>
-      <c r="C41" s="63"/>
-      <c r="D41" s="64"/>
-      <c r="E41" s="69"/>
-      <c r="F41" s="69"/>
-      <c r="G41" s="69"/>
-      <c r="H41" s="70"/>
-      <c r="I41" s="73" t="s">
+      <c r="B41" s="55"/>
+      <c r="C41" s="59"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="65"/>
+      <c r="F41" s="65"/>
+      <c r="G41" s="65"/>
+      <c r="H41" s="66"/>
+      <c r="I41" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="J41" s="54"/>
+      <c r="J41" s="50"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B42" s="59"/>
-      <c r="C42" s="63"/>
-      <c r="D42" s="64"/>
-      <c r="E42" s="69"/>
-      <c r="F42" s="69"/>
-      <c r="G42" s="69"/>
-      <c r="H42" s="70"/>
-      <c r="I42" s="73" t="s">
+      <c r="B42" s="55"/>
+      <c r="C42" s="59"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="65"/>
+      <c r="F42" s="65"/>
+      <c r="G42" s="65"/>
+      <c r="H42" s="66"/>
+      <c r="I42" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="J42" s="54"/>
+      <c r="J42" s="50"/>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B43" s="59"/>
-      <c r="C43" s="63"/>
-      <c r="D43" s="64"/>
-      <c r="E43" s="69"/>
-      <c r="F43" s="69"/>
-      <c r="G43" s="69"/>
-      <c r="H43" s="70"/>
-      <c r="I43" s="73" t="s">
+      <c r="B43" s="55"/>
+      <c r="C43" s="59"/>
+      <c r="D43" s="60"/>
+      <c r="E43" s="65"/>
+      <c r="F43" s="65"/>
+      <c r="G43" s="65"/>
+      <c r="H43" s="66"/>
+      <c r="I43" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="J43" s="54"/>
+      <c r="J43" s="50"/>
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B44" s="60"/>
-      <c r="C44" s="63"/>
-      <c r="D44" s="64"/>
-      <c r="E44" s="69"/>
-      <c r="F44" s="69"/>
-      <c r="G44" s="69"/>
-      <c r="H44" s="70"/>
-      <c r="I44" s="73" t="s">
+      <c r="B44" s="56"/>
+      <c r="C44" s="59"/>
+      <c r="D44" s="60"/>
+      <c r="E44" s="65"/>
+      <c r="F44" s="65"/>
+      <c r="G44" s="65"/>
+      <c r="H44" s="66"/>
+      <c r="I44" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="J44" s="54"/>
+      <c r="J44" s="50"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B45" s="58">
+      <c r="B45" s="54">
         <f>B40+1</f>
         <v>19</v>
       </c>
-      <c r="C45" s="61"/>
-      <c r="D45" s="62"/>
-      <c r="E45" s="62"/>
-      <c r="F45" s="67" t="s">
+      <c r="C45" s="57"/>
+      <c r="D45" s="58"/>
+      <c r="E45" s="58"/>
+      <c r="F45" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="G45" s="67"/>
-      <c r="H45" s="68"/>
-      <c r="I45" s="54" t="s">
+      <c r="G45" s="63"/>
+      <c r="H45" s="64"/>
+      <c r="I45" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="J45" s="55"/>
+      <c r="J45" s="51"/>
       <c r="K45" s="4"/>
       <c r="L45" s="4"/>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B46" s="59"/>
-      <c r="C46" s="63"/>
-      <c r="D46" s="64"/>
-      <c r="E46" s="64"/>
-      <c r="F46" s="69"/>
-      <c r="G46" s="69"/>
-      <c r="H46" s="70"/>
-      <c r="I46" s="73" t="s">
+      <c r="B46" s="55"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="60"/>
+      <c r="E46" s="60"/>
+      <c r="F46" s="65"/>
+      <c r="G46" s="65"/>
+      <c r="H46" s="66"/>
+      <c r="I46" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="J46" s="54"/>
+      <c r="J46" s="50"/>
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B47" s="59"/>
-      <c r="C47" s="63"/>
-      <c r="D47" s="64"/>
-      <c r="E47" s="64"/>
-      <c r="F47" s="69"/>
-      <c r="G47" s="69"/>
-      <c r="H47" s="70"/>
-      <c r="I47" s="73" t="s">
+      <c r="B47" s="55"/>
+      <c r="C47" s="59"/>
+      <c r="D47" s="60"/>
+      <c r="E47" s="60"/>
+      <c r="F47" s="65"/>
+      <c r="G47" s="65"/>
+      <c r="H47" s="66"/>
+      <c r="I47" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="J47" s="54"/>
+      <c r="J47" s="50"/>
       <c r="K47" s="4"/>
       <c r="L47" s="4"/>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B48" s="60"/>
-      <c r="C48" s="65"/>
-      <c r="D48" s="66"/>
-      <c r="E48" s="66"/>
-      <c r="F48" s="71"/>
-      <c r="G48" s="71"/>
-      <c r="H48" s="72"/>
-      <c r="I48" s="73" t="s">
+      <c r="B48" s="56"/>
+      <c r="C48" s="61"/>
+      <c r="D48" s="62"/>
+      <c r="E48" s="62"/>
+      <c r="F48" s="67"/>
+      <c r="G48" s="67"/>
+      <c r="H48" s="68"/>
+      <c r="I48" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="J48" s="54"/>
+      <c r="J48" s="50"/>
       <c r="K48" s="10"/>
       <c r="L48" s="4" t="s">
         <v>59</v>
@@ -3857,14 +3782,14 @@
       <c r="D49" s="9"/>
       <c r="E49" s="9"/>
       <c r="F49" s="9"/>
-      <c r="G49" s="52" t="s">
+      <c r="G49" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="H49" s="53"/>
-      <c r="I49" s="54" t="s">
+      <c r="H49" s="49"/>
+      <c r="I49" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="J49" s="55"/>
+      <c r="J49" s="51"/>
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
     </row>
@@ -3873,16 +3798,16 @@
         <f t="shared" ref="B50:B60" si="1">B49+1</f>
         <v>21</v>
       </c>
-      <c r="C50" s="56"/>
-      <c r="D50" s="57"/>
-      <c r="E50" s="57"/>
-      <c r="F50" s="57"/>
-      <c r="G50" s="52" t="s">
+      <c r="C50" s="52"/>
+      <c r="D50" s="53"/>
+      <c r="E50" s="53"/>
+      <c r="F50" s="53"/>
+      <c r="G50" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="H50" s="53"/>
-      <c r="I50" s="50"/>
-      <c r="J50" s="51"/>
+      <c r="H50" s="49"/>
+      <c r="I50" s="46"/>
+      <c r="J50" s="47"/>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
     </row>
@@ -3897,8 +3822,8 @@
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
       <c r="H51" s="6"/>
-      <c r="I51" s="50"/>
-      <c r="J51" s="51"/>
+      <c r="I51" s="46"/>
+      <c r="J51" s="47"/>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
     </row>
@@ -3913,8 +3838,8 @@
       <c r="F52" s="9"/>
       <c r="G52" s="9"/>
       <c r="H52" s="6"/>
-      <c r="I52" s="50"/>
-      <c r="J52" s="51"/>
+      <c r="I52" s="46"/>
+      <c r="J52" s="47"/>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
     </row>
@@ -3929,8 +3854,8 @@
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
       <c r="H53" s="6"/>
-      <c r="I53" s="50"/>
-      <c r="J53" s="51"/>
+      <c r="I53" s="46"/>
+      <c r="J53" s="47"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
     </row>
@@ -3945,8 +3870,8 @@
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
       <c r="H54" s="6"/>
-      <c r="I54" s="50"/>
-      <c r="J54" s="51"/>
+      <c r="I54" s="46"/>
+      <c r="J54" s="47"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
     </row>
@@ -3961,8 +3886,8 @@
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
       <c r="H55" s="6"/>
-      <c r="I55" s="50"/>
-      <c r="J55" s="51"/>
+      <c r="I55" s="46"/>
+      <c r="J55" s="47"/>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
     </row>
@@ -3977,8 +3902,8 @@
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
       <c r="H56" s="6"/>
-      <c r="I56" s="50"/>
-      <c r="J56" s="51"/>
+      <c r="I56" s="46"/>
+      <c r="J56" s="47"/>
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
     </row>
@@ -3993,8 +3918,8 @@
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
       <c r="H57" s="6"/>
-      <c r="I57" s="50"/>
-      <c r="J57" s="51"/>
+      <c r="I57" s="46"/>
+      <c r="J57" s="47"/>
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
     </row>
@@ -4009,8 +3934,8 @@
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
       <c r="H58" s="6"/>
-      <c r="I58" s="50"/>
-      <c r="J58" s="51"/>
+      <c r="I58" s="46"/>
+      <c r="J58" s="47"/>
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
     </row>
@@ -4025,8 +3950,8 @@
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
       <c r="H59" s="6"/>
-      <c r="I59" s="50"/>
-      <c r="J59" s="51"/>
+      <c r="I59" s="46"/>
+      <c r="J59" s="47"/>
       <c r="K59" s="4"/>
       <c r="L59" s="4"/>
     </row>
@@ -4041,8 +3966,8 @@
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
       <c r="H60" s="6"/>
-      <c r="I60" s="50"/>
-      <c r="J60" s="51"/>
+      <c r="I60" s="46"/>
+      <c r="J60" s="47"/>
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
     </row>

</xml_diff>

<commit_message>
#13 Sign in link returns the user to the sign up page
</commit_message>
<xml_diff>
--- a/documents/Testing Schedule.xlsx
+++ b/documents/Testing Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Node\Timelog\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D72B6C7-4FB3-4940-B43E-34F244B4D5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695C0E51-4417-4078-A485-E3708EEC73C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{9AAAF6DA-95E7-49F0-B7DD-46373E33B9E7}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="128">
   <si>
     <t>RMPC Timelog Testing Schedule</t>
   </si>
@@ -412,6 +412,15 @@
   </si>
   <si>
     <t>#6</t>
+  </si>
+  <si>
+    <t>Unique</t>
+  </si>
+  <si>
+    <t>#12</t>
+  </si>
+  <si>
+    <t>User is returned to the sign up page</t>
   </si>
 </sst>
 </file>
@@ -694,7 +703,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -812,6 +821,27 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -929,9 +959,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -944,6 +971,9 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -980,10 +1010,13 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1305,11 +1338,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDA5C5C7-8B67-4FAF-9315-0E07B94A4E72}">
-  <dimension ref="B2:Q77"/>
+  <dimension ref="B2:Q78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M23" sqref="M23"/>
+      <pane ySplit="5" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1319,50 +1352,49 @@
     <col min="3" max="7" width="10.7109375" style="2" customWidth="1"/>
     <col min="8" max="8" width="35.5703125" style="2" customWidth="1"/>
     <col min="9" max="9" width="62.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="3" customWidth="1"/>
-    <col min="11" max="12" width="9.7109375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="49.140625" style="92" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="49.140625" style="85" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="99" customWidth="1"/>
+    <col min="11" max="12" width="9.7109375" style="99" customWidth="1"/>
+    <col min="13" max="13" width="49.140625" style="107" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="49.140625" style="91" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="97" t="s">
         <v>113</v>
       </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="P2" s="87"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="P2" s="94"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="104" t="s">
         <v>112</v>
       </c>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="96"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="103"/>
       <c r="H3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I3" s="1"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="92"/>
-      <c r="O3" s="85"/>
-      <c r="Q3" s="88"/>
+      <c r="N3" s="99"/>
+      <c r="O3" s="91"/>
+      <c r="Q3" s="95"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="98" t="s">
         <v>111</v>
       </c>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="P4" s="89"/>
+      <c r="P4" s="96"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
@@ -1379,13 +1411,13 @@
       <c r="I6" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="J6" s="16" t="s">
+      <c r="J6" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="K6" s="80" t="s">
+      <c r="K6" s="87" t="s">
         <v>114</v>
       </c>
-      <c r="L6" s="81"/>
+      <c r="L6" s="88"/>
       <c r="M6" s="17" t="s">
         <v>105</v>
       </c>
@@ -1395,19 +1427,19 @@
       <c r="B7" s="11">
         <v>1</v>
       </c>
-      <c r="C7" s="79" t="s">
+      <c r="C7" s="86" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="48"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
       <c r="I7" s="4"/>
-      <c r="J7" s="93"/>
-      <c r="K7" s="93"/>
-      <c r="L7" s="93"/>
-      <c r="M7" s="45"/>
+      <c r="J7" s="100"/>
+      <c r="K7" s="100"/>
+      <c r="L7" s="100"/>
+      <c r="M7" s="106"/>
       <c r="N7" s="2"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
@@ -1416,27 +1448,27 @@
         <v>2</v>
       </c>
       <c r="C8" s="41"/>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
       <c r="I8" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="J8" s="84" t="s">
+      <c r="J8" s="90" t="s">
         <v>70</v>
       </c>
-      <c r="K8" s="84"/>
-      <c r="L8" s="84"/>
-      <c r="M8" s="45"/>
+      <c r="K8" s="90"/>
+      <c r="L8" s="90"/>
+      <c r="M8" s="106"/>
       <c r="N8" s="2"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="11">
-        <f t="shared" ref="B9:B72" si="0">B8+1</f>
+        <f t="shared" ref="B9:B73" si="0">B8+1</f>
         <v>3</v>
       </c>
       <c r="C9" s="41"/>
@@ -1448,10 +1480,10 @@
       <c r="G9" s="42"/>
       <c r="H9" s="42"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="93"/>
-      <c r="K9" s="93"/>
-      <c r="L9" s="93"/>
-      <c r="M9" s="45"/>
+      <c r="J9" s="100"/>
+      <c r="K9" s="100"/>
+      <c r="L9" s="100"/>
+      <c r="M9" s="106"/>
       <c r="N9" s="2"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
@@ -1467,17 +1499,17 @@
       <c r="F10" s="42"/>
       <c r="G10" s="42"/>
       <c r="H10" s="42"/>
-      <c r="I10" s="45" t="s">
+      <c r="I10" s="52" t="s">
         <v>95</v>
       </c>
-      <c r="J10" s="98" t="s">
+      <c r="J10" s="90" t="s">
         <v>70</v>
       </c>
-      <c r="K10" s="99" t="s">
+      <c r="K10" s="93" t="s">
         <v>117</v>
       </c>
-      <c r="L10" s="98"/>
-      <c r="M10" s="100" t="s">
+      <c r="L10" s="105"/>
+      <c r="M10" s="108" t="s">
         <v>109</v>
       </c>
       <c r="N10" s="2"/>
@@ -1495,15 +1527,15 @@
       <c r="F11" s="42"/>
       <c r="G11" s="42"/>
       <c r="H11" s="42"/>
-      <c r="I11" s="45" t="s">
+      <c r="I11" s="52" t="s">
         <v>95</v>
       </c>
-      <c r="J11" s="98" t="s">
+      <c r="J11" s="90" t="s">
         <v>70</v>
       </c>
-      <c r="K11" s="99"/>
-      <c r="L11" s="98"/>
-      <c r="M11" s="100"/>
+      <c r="K11" s="93"/>
+      <c r="L11" s="105"/>
+      <c r="M11" s="108"/>
       <c r="N11" s="2"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
@@ -1519,15 +1551,15 @@
       <c r="F12" s="42"/>
       <c r="G12" s="42"/>
       <c r="H12" s="42"/>
-      <c r="I12" s="45" t="s">
+      <c r="I12" s="52" t="s">
         <v>95</v>
       </c>
-      <c r="J12" s="98" t="s">
+      <c r="J12" s="90" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="99"/>
-      <c r="L12" s="98"/>
-      <c r="M12" s="100"/>
+      <c r="K12" s="93"/>
+      <c r="L12" s="105"/>
+      <c r="M12" s="108"/>
       <c r="N12" s="2"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
@@ -1535,77 +1567,73 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C13" s="41"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42" t="s">
+      <c r="C13" s="43"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="45" t="s">
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="52" t="s">
         <v>95</v>
       </c>
-      <c r="J13" s="98" t="s">
+      <c r="J13" s="90" t="s">
         <v>70</v>
       </c>
-      <c r="K13" s="99"/>
-      <c r="L13" s="98"/>
-      <c r="M13" s="100"/>
+      <c r="K13" s="93"/>
+      <c r="L13" s="105"/>
+      <c r="M13" s="108"/>
       <c r="N13" s="2"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="11">
+      <c r="B14" s="22">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42" t="s">
+      <c r="C14" s="43"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="70" t="s">
         <v>100</v>
       </c>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="45" t="s">
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="J14" s="98" t="s">
+      <c r="J14" s="90" t="s">
         <v>70</v>
       </c>
-      <c r="K14" s="84" t="s">
+      <c r="K14" s="90" t="s">
         <v>116</v>
       </c>
-      <c r="L14" s="98" t="s">
+      <c r="L14" s="90" t="s">
         <v>117</v>
       </c>
-      <c r="M14" s="100"/>
+      <c r="M14" s="108"/>
       <c r="N14" s="2"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="11">
+      <c r="B15" s="22">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42" t="s">
-        <v>101</v>
-      </c>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="45" t="s">
-        <v>96</v>
-      </c>
-      <c r="J15" s="98" t="s">
-        <v>70</v>
-      </c>
-      <c r="K15" s="98" t="s">
-        <v>117</v>
-      </c>
-      <c r="L15" s="98"/>
-      <c r="M15" s="100"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="49" t="s">
+        <v>125</v>
+      </c>
+      <c r="J15" s="89" t="s">
+        <v>110</v>
+      </c>
+      <c r="K15" s="90"/>
+      <c r="L15" s="105"/>
+      <c r="M15" s="108"/>
       <c r="N15" s="2"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
@@ -1613,77 +1641,73 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42" t="s">
-        <v>102</v>
-      </c>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="J16" s="84" t="s">
+      <c r="C16" s="46"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47" t="s">
+        <v>101</v>
+      </c>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="J16" s="90" t="s">
         <v>70</v>
       </c>
-      <c r="K16" s="84" t="s">
-        <v>115</v>
-      </c>
-      <c r="L16" s="84"/>
-      <c r="M16" s="45" t="s">
-        <v>118</v>
-      </c>
+      <c r="K16" s="90" t="s">
+        <v>117</v>
+      </c>
+      <c r="L16" s="105"/>
+      <c r="M16" s="108"/>
       <c r="N16" s="2"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="11">
-        <f>B16+1</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="C17" s="41"/>
-      <c r="D17" s="42" t="s">
-        <v>103</v>
-      </c>
-      <c r="E17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42" t="s">
+        <v>102</v>
+      </c>
       <c r="F17" s="42"/>
       <c r="G17" s="42"/>
       <c r="H17" s="42"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="93"/>
-      <c r="K17" s="93"/>
-      <c r="L17" s="93"/>
-      <c r="M17" s="45"/>
+      <c r="I17" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J17" s="90" t="s">
+        <v>70</v>
+      </c>
+      <c r="K17" s="90" t="s">
+        <v>115</v>
+      </c>
+      <c r="L17" s="90"/>
+      <c r="M17" s="106" t="s">
+        <v>118</v>
+      </c>
       <c r="N17" s="2"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="11">
-        <f t="shared" si="0"/>
+        <f>B17+1</f>
         <v>12</v>
       </c>
       <c r="C18" s="41"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42" t="s">
-        <v>108</v>
-      </c>
+      <c r="D18" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18" s="42"/>
       <c r="F18" s="42"/>
       <c r="G18" s="42"/>
       <c r="H18" s="42"/>
-      <c r="I18" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="J18" s="83" t="s">
-        <v>110</v>
-      </c>
-      <c r="K18" s="84" t="s">
-        <v>123</v>
-      </c>
-      <c r="L18" s="83" t="s">
-        <v>124</v>
-      </c>
-      <c r="M18" s="45" t="s">
-        <v>122</v>
-      </c>
+      <c r="I18" s="4"/>
+      <c r="J18" s="100"/>
+      <c r="K18" s="100"/>
+      <c r="L18" s="100"/>
+      <c r="M18" s="106"/>
       <c r="N18" s="2"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
@@ -1694,16 +1718,26 @@
       <c r="C19" s="41"/>
       <c r="D19" s="42"/>
       <c r="E19" s="42" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="F19" s="42"/>
       <c r="G19" s="42"/>
       <c r="H19" s="42"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="93"/>
-      <c r="K19" s="93"/>
-      <c r="L19" s="93"/>
-      <c r="M19" s="45"/>
+      <c r="I19" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="J19" s="89" t="s">
+        <v>110</v>
+      </c>
+      <c r="K19" s="90" t="s">
+        <v>123</v>
+      </c>
+      <c r="L19" s="89" t="s">
+        <v>124</v>
+      </c>
+      <c r="M19" s="106" t="s">
+        <v>122</v>
+      </c>
       <c r="N19" s="2"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
@@ -1713,19 +1747,17 @@
       </c>
       <c r="C20" s="41"/>
       <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42" t="s">
-        <v>121</v>
-      </c>
+      <c r="E20" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="F20" s="42"/>
       <c r="G20" s="42"/>
       <c r="H20" s="42"/>
-      <c r="I20" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="J20" s="93"/>
-      <c r="K20" s="93"/>
-      <c r="L20" s="93"/>
-      <c r="M20" s="45"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="100"/>
+      <c r="K20" s="100"/>
+      <c r="L20" s="100"/>
+      <c r="M20" s="106"/>
       <c r="N20" s="2"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
@@ -1733,19 +1765,21 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C21" s="79" t="s">
-        <v>90</v>
-      </c>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="48"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="82"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="93"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="J21" s="100"/>
+      <c r="K21" s="100"/>
+      <c r="L21" s="100"/>
+      <c r="M21" s="106"/>
       <c r="N21" s="2"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
@@ -1753,21 +1787,19 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="48" t="s">
-        <v>88</v>
-      </c>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="48"/>
-      <c r="I22" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="J22" s="82"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="93"/>
+      <c r="C22" s="86" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="55"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="55"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="100"/>
+      <c r="K22" s="100"/>
+      <c r="L22" s="100"/>
+      <c r="M22" s="106"/>
       <c r="N22" s="2"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
@@ -1776,20 +1808,26 @@
         <v>17</v>
       </c>
       <c r="C23" s="5"/>
-      <c r="D23" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
+      <c r="D23" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" s="55"/>
+      <c r="F23" s="55"/>
+      <c r="G23" s="55"/>
+      <c r="H23" s="55"/>
       <c r="I23" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J23" s="82"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="93"/>
+        <v>89</v>
+      </c>
+      <c r="J23" s="90" t="s">
+        <v>70</v>
+      </c>
+      <c r="K23" s="90" t="s">
+        <v>126</v>
+      </c>
+      <c r="L23" s="100"/>
+      <c r="M23" s="106" t="s">
+        <v>127</v>
+      </c>
       <c r="N23" s="2"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
@@ -1797,21 +1835,21 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C24" s="71" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="63"/>
-      <c r="E24" s="63"/>
-      <c r="F24" s="63"/>
-      <c r="G24" s="63"/>
-      <c r="H24" s="63"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
       <c r="I24" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J24" s="82"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="93"/>
+        <v>5</v>
+      </c>
+      <c r="J24" s="100"/>
+      <c r="K24" s="100"/>
+      <c r="L24" s="100"/>
+      <c r="M24" s="106"/>
       <c r="N24" s="2"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
@@ -1819,19 +1857,21 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C25" s="73"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="67"/>
-      <c r="F25" s="67"/>
-      <c r="G25" s="67"/>
-      <c r="H25" s="67"/>
+      <c r="C25" s="78" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="70"/>
+      <c r="E25" s="70"/>
+      <c r="F25" s="70"/>
+      <c r="G25" s="70"/>
+      <c r="H25" s="70"/>
       <c r="I25" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J25" s="82"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="93"/>
+        <v>16</v>
+      </c>
+      <c r="J25" s="100"/>
+      <c r="K25" s="100"/>
+      <c r="L25" s="100"/>
+      <c r="M25" s="106"/>
       <c r="N25" s="2"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
@@ -1839,21 +1879,19 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C26" s="57"/>
-      <c r="D26" s="63" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="63"/>
-      <c r="F26" s="63"/>
-      <c r="G26" s="63"/>
-      <c r="H26" s="63"/>
+      <c r="C26" s="80"/>
+      <c r="D26" s="74"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="74"/>
+      <c r="G26" s="74"/>
+      <c r="H26" s="74"/>
       <c r="I26" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J26" s="82"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="93"/>
+        <v>25</v>
+      </c>
+      <c r="J26" s="100"/>
+      <c r="K26" s="100"/>
+      <c r="L26" s="100"/>
+      <c r="M26" s="106"/>
       <c r="N26" s="2"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
@@ -1861,19 +1899,21 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C27" s="61"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="67"/>
-      <c r="F27" s="67"/>
-      <c r="G27" s="67"/>
-      <c r="H27" s="67"/>
+      <c r="C27" s="64"/>
+      <c r="D27" s="70" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="70"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="70"/>
+      <c r="H27" s="70"/>
       <c r="I27" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J27" s="82"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="93"/>
+        <v>14</v>
+      </c>
+      <c r="J27" s="100"/>
+      <c r="K27" s="100"/>
+      <c r="L27" s="100"/>
+      <c r="M27" s="106"/>
       <c r="N27" s="2"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
@@ -1881,21 +1921,19 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="C28" s="57"/>
-      <c r="D28" s="63" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="63"/>
-      <c r="F28" s="63"/>
-      <c r="G28" s="63"/>
-      <c r="H28" s="63"/>
+      <c r="C28" s="68"/>
+      <c r="D28" s="74"/>
+      <c r="E28" s="74"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="74"/>
+      <c r="H28" s="74"/>
       <c r="I28" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J28" s="82"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="93"/>
+        <v>49</v>
+      </c>
+      <c r="J28" s="100"/>
+      <c r="K28" s="100"/>
+      <c r="L28" s="100"/>
+      <c r="M28" s="106"/>
       <c r="N28" s="2"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
@@ -1903,19 +1941,21 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="C29" s="59"/>
-      <c r="D29" s="65"/>
-      <c r="E29" s="65"/>
-      <c r="F29" s="65"/>
-      <c r="G29" s="65"/>
-      <c r="H29" s="65"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="70" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29" s="70"/>
+      <c r="F29" s="70"/>
+      <c r="G29" s="70"/>
+      <c r="H29" s="70"/>
       <c r="I29" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="J29" s="82"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="93"/>
+        <v>28</v>
+      </c>
+      <c r="J29" s="100"/>
+      <c r="K29" s="100"/>
+      <c r="L29" s="100"/>
+      <c r="M29" s="106"/>
       <c r="N29" s="2"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
@@ -1923,19 +1963,19 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C30" s="61"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="67"/>
-      <c r="G30" s="67"/>
-      <c r="H30" s="67"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="72"/>
+      <c r="E30" s="72"/>
+      <c r="F30" s="72"/>
+      <c r="G30" s="72"/>
+      <c r="H30" s="72"/>
       <c r="I30" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="J30" s="82"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="93"/>
+        <v>50</v>
+      </c>
+      <c r="J30" s="100"/>
+      <c r="K30" s="100"/>
+      <c r="L30" s="100"/>
+      <c r="M30" s="106"/>
       <c r="N30" s="2"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
@@ -1943,21 +1983,19 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="C31" s="44"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="48" t="s">
-        <v>20</v>
-      </c>
-      <c r="F31" s="48"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="48"/>
+      <c r="C31" s="68"/>
+      <c r="D31" s="74"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="74"/>
+      <c r="G31" s="74"/>
+      <c r="H31" s="74"/>
       <c r="I31" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="J31" s="82"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="93"/>
+        <v>54</v>
+      </c>
+      <c r="J31" s="100"/>
+      <c r="K31" s="100"/>
+      <c r="L31" s="100"/>
+      <c r="M31" s="106"/>
       <c r="N31" s="2"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
@@ -1965,21 +2003,21 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="C32" s="57"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="58"/>
-      <c r="F32" s="63" t="s">
-        <v>10</v>
-      </c>
-      <c r="G32" s="63"/>
-      <c r="H32" s="63"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="55"/>
+      <c r="G32" s="55"/>
+      <c r="H32" s="55"/>
       <c r="I32" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J32" s="82"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="93"/>
+        <v>57</v>
+      </c>
+      <c r="J32" s="100"/>
+      <c r="K32" s="100"/>
+      <c r="L32" s="100"/>
+      <c r="M32" s="106"/>
       <c r="N32" s="2"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
@@ -1987,19 +2025,21 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="C33" s="59"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="60"/>
-      <c r="F33" s="65"/>
-      <c r="G33" s="65"/>
-      <c r="H33" s="65"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="65"/>
+      <c r="E33" s="65"/>
+      <c r="F33" s="70" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="70"/>
+      <c r="H33" s="70"/>
       <c r="I33" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J33" s="82"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="J33" s="100"/>
+      <c r="K33" s="100"/>
+      <c r="L33" s="100"/>
+      <c r="M33" s="106"/>
       <c r="N33" s="2"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
@@ -2007,19 +2047,19 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="C34" s="59"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="60"/>
-      <c r="F34" s="65"/>
-      <c r="G34" s="65"/>
-      <c r="H34" s="65"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="67"/>
+      <c r="E34" s="67"/>
+      <c r="F34" s="72"/>
+      <c r="G34" s="72"/>
+      <c r="H34" s="72"/>
       <c r="I34" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="J34" s="82"/>
-      <c r="K34" s="93"/>
-      <c r="L34" s="93"/>
-      <c r="M34" s="45"/>
+        <v>33</v>
+      </c>
+      <c r="J34" s="100"/>
+      <c r="K34" s="100"/>
+      <c r="L34" s="100"/>
+      <c r="M34" s="106"/>
       <c r="N34" s="2"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
@@ -2027,19 +2067,19 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="C35" s="59"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="60"/>
-      <c r="F35" s="65"/>
-      <c r="G35" s="65"/>
-      <c r="H35" s="65"/>
+      <c r="C35" s="66"/>
+      <c r="D35" s="67"/>
+      <c r="E35" s="67"/>
+      <c r="F35" s="72"/>
+      <c r="G35" s="72"/>
+      <c r="H35" s="72"/>
       <c r="I35" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J35" s="82"/>
-      <c r="K35" s="93"/>
-      <c r="L35" s="93"/>
-      <c r="M35" s="45"/>
+        <v>32</v>
+      </c>
+      <c r="J35" s="100"/>
+      <c r="K35" s="100"/>
+      <c r="L35" s="100"/>
+      <c r="M35" s="106"/>
       <c r="N35" s="2"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
@@ -2047,21 +2087,19 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="C36" s="61"/>
-      <c r="D36" s="62"/>
-      <c r="E36" s="62"/>
-      <c r="F36" s="67"/>
-      <c r="G36" s="67"/>
-      <c r="H36" s="67"/>
+      <c r="C36" s="66"/>
+      <c r="D36" s="67"/>
+      <c r="E36" s="67"/>
+      <c r="F36" s="72"/>
+      <c r="G36" s="72"/>
+      <c r="H36" s="72"/>
       <c r="I36" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J36" s="83"/>
-      <c r="K36" s="83"/>
-      <c r="L36" s="83"/>
-      <c r="M36" s="45" t="s">
-        <v>36</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="J36" s="100"/>
+      <c r="K36" s="100"/>
+      <c r="L36" s="100"/>
+      <c r="M36" s="106"/>
       <c r="N36" s="2"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
@@ -2069,21 +2107,21 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="C37" s="52"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="48" t="s">
-        <v>21</v>
-      </c>
-      <c r="F37" s="48"/>
-      <c r="G37" s="48"/>
-      <c r="H37" s="48"/>
+      <c r="C37" s="68"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="74"/>
+      <c r="G37" s="74"/>
+      <c r="H37" s="74"/>
       <c r="I37" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="J37" s="82"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="93"/>
+        <v>35</v>
+      </c>
+      <c r="J37" s="89"/>
+      <c r="K37" s="89"/>
+      <c r="L37" s="89"/>
+      <c r="M37" s="106" t="s">
+        <v>36</v>
+      </c>
       <c r="N37" s="2"/>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
@@ -2091,21 +2129,21 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="C38" s="57"/>
-      <c r="D38" s="58"/>
-      <c r="E38" s="58"/>
-      <c r="F38" s="63" t="s">
-        <v>7</v>
-      </c>
-      <c r="G38" s="63"/>
-      <c r="H38" s="63"/>
+      <c r="C38" s="59"/>
+      <c r="D38" s="60"/>
+      <c r="E38" s="55" t="s">
+        <v>21</v>
+      </c>
+      <c r="F38" s="55"/>
+      <c r="G38" s="55"/>
+      <c r="H38" s="55"/>
       <c r="I38" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J38" s="82"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="93"/>
+        <v>56</v>
+      </c>
+      <c r="J38" s="100"/>
+      <c r="K38" s="100"/>
+      <c r="L38" s="100"/>
+      <c r="M38" s="106"/>
       <c r="N38" s="2"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
@@ -2113,19 +2151,21 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="C39" s="61"/>
-      <c r="D39" s="62"/>
-      <c r="E39" s="62"/>
-      <c r="F39" s="67"/>
-      <c r="G39" s="67"/>
-      <c r="H39" s="67"/>
+      <c r="C39" s="64"/>
+      <c r="D39" s="65"/>
+      <c r="E39" s="65"/>
+      <c r="F39" s="70" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" s="70"/>
+      <c r="H39" s="70"/>
       <c r="I39" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J39" s="82"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="93"/>
+        <v>55</v>
+      </c>
+      <c r="J39" s="100"/>
+      <c r="K39" s="100"/>
+      <c r="L39" s="100"/>
+      <c r="M39" s="106"/>
       <c r="N39" s="2"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
@@ -2133,21 +2173,19 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="C40" s="5"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="G40" s="48"/>
-      <c r="H40" s="48"/>
+      <c r="C40" s="68"/>
+      <c r="D40" s="69"/>
+      <c r="E40" s="69"/>
+      <c r="F40" s="74"/>
+      <c r="G40" s="74"/>
+      <c r="H40" s="74"/>
       <c r="I40" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J40" s="82"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="4"/>
-      <c r="M40" s="93"/>
+        <v>35</v>
+      </c>
+      <c r="J40" s="100"/>
+      <c r="K40" s="100"/>
+      <c r="L40" s="100"/>
+      <c r="M40" s="106"/>
       <c r="N40" s="2"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.25">
@@ -2155,21 +2193,21 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="C41" s="57"/>
-      <c r="D41" s="58"/>
-      <c r="E41" s="58"/>
-      <c r="F41" s="63" t="s">
-        <v>8</v>
-      </c>
-      <c r="G41" s="63"/>
-      <c r="H41" s="63"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="G41" s="55"/>
+      <c r="H41" s="55"/>
       <c r="I41" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J41" s="82"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="4"/>
-      <c r="M41" s="93"/>
+        <v>18</v>
+      </c>
+      <c r="J41" s="100"/>
+      <c r="K41" s="100"/>
+      <c r="L41" s="100"/>
+      <c r="M41" s="106"/>
       <c r="N41" s="2"/>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
@@ -2177,19 +2215,21 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="C42" s="61"/>
-      <c r="D42" s="62"/>
-      <c r="E42" s="62"/>
-      <c r="F42" s="67"/>
-      <c r="G42" s="67"/>
-      <c r="H42" s="67"/>
+      <c r="C42" s="64"/>
+      <c r="D42" s="65"/>
+      <c r="E42" s="65"/>
+      <c r="F42" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" s="70"/>
+      <c r="H42" s="70"/>
       <c r="I42" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="J42" s="82"/>
-      <c r="K42" s="4"/>
-      <c r="L42" s="4"/>
-      <c r="M42" s="93"/>
+        <v>9</v>
+      </c>
+      <c r="J42" s="100"/>
+      <c r="K42" s="100"/>
+      <c r="L42" s="100"/>
+      <c r="M42" s="106"/>
       <c r="N42" s="2"/>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
@@ -2197,21 +2237,19 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="C43" s="71"/>
-      <c r="D43" s="63"/>
-      <c r="E43" s="63"/>
-      <c r="F43" s="63" t="s">
-        <v>10</v>
-      </c>
-      <c r="G43" s="63"/>
-      <c r="H43" s="63"/>
+      <c r="C43" s="68"/>
+      <c r="D43" s="69"/>
+      <c r="E43" s="69"/>
+      <c r="F43" s="74"/>
+      <c r="G43" s="74"/>
+      <c r="H43" s="74"/>
       <c r="I43" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J43" s="82"/>
-      <c r="K43" s="4"/>
-      <c r="L43" s="4"/>
-      <c r="M43" s="93"/>
+        <v>37</v>
+      </c>
+      <c r="J43" s="100"/>
+      <c r="K43" s="100"/>
+      <c r="L43" s="100"/>
+      <c r="M43" s="106"/>
       <c r="N43" s="2"/>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.25">
@@ -2219,19 +2257,21 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="C44" s="72"/>
-      <c r="D44" s="65"/>
-      <c r="E44" s="65"/>
-      <c r="F44" s="65"/>
-      <c r="G44" s="65"/>
-      <c r="H44" s="65"/>
+      <c r="C44" s="78"/>
+      <c r="D44" s="70"/>
+      <c r="E44" s="70"/>
+      <c r="F44" s="70" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" s="70"/>
+      <c r="H44" s="70"/>
       <c r="I44" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J44" s="82"/>
-      <c r="K44" s="4"/>
-      <c r="L44" s="4"/>
-      <c r="M44" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="J44" s="100"/>
+      <c r="K44" s="100"/>
+      <c r="L44" s="100"/>
+      <c r="M44" s="106"/>
       <c r="N44" s="2"/>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.25">
@@ -2239,19 +2279,19 @@
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="C45" s="72"/>
-      <c r="D45" s="65"/>
-      <c r="E45" s="65"/>
-      <c r="F45" s="65"/>
-      <c r="G45" s="65"/>
-      <c r="H45" s="65"/>
+      <c r="C45" s="79"/>
+      <c r="D45" s="72"/>
+      <c r="E45" s="72"/>
+      <c r="F45" s="72"/>
+      <c r="G45" s="72"/>
+      <c r="H45" s="72"/>
       <c r="I45" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="J45" s="82"/>
-      <c r="K45" s="93"/>
-      <c r="L45" s="93"/>
-      <c r="M45" s="45"/>
+        <v>33</v>
+      </c>
+      <c r="J45" s="100"/>
+      <c r="K45" s="100"/>
+      <c r="L45" s="100"/>
+      <c r="M45" s="106"/>
       <c r="N45" s="2"/>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.25">
@@ -2259,19 +2299,19 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="C46" s="72"/>
-      <c r="D46" s="65"/>
-      <c r="E46" s="65"/>
-      <c r="F46" s="65"/>
-      <c r="G46" s="65"/>
-      <c r="H46" s="65"/>
+      <c r="C46" s="79"/>
+      <c r="D46" s="72"/>
+      <c r="E46" s="72"/>
+      <c r="F46" s="72"/>
+      <c r="G46" s="72"/>
+      <c r="H46" s="72"/>
       <c r="I46" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J46" s="82"/>
-      <c r="K46" s="93"/>
-      <c r="L46" s="93"/>
-      <c r="M46" s="45"/>
+        <v>32</v>
+      </c>
+      <c r="J46" s="100"/>
+      <c r="K46" s="100"/>
+      <c r="L46" s="100"/>
+      <c r="M46" s="106"/>
       <c r="N46" s="2"/>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.25">
@@ -2279,21 +2319,19 @@
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="C47" s="73"/>
-      <c r="D47" s="67"/>
-      <c r="E47" s="67"/>
-      <c r="F47" s="67"/>
-      <c r="G47" s="67"/>
-      <c r="H47" s="67"/>
+      <c r="C47" s="79"/>
+      <c r="D47" s="72"/>
+      <c r="E47" s="72"/>
+      <c r="F47" s="72"/>
+      <c r="G47" s="72"/>
+      <c r="H47" s="72"/>
       <c r="I47" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J47" s="83"/>
-      <c r="K47" s="83"/>
-      <c r="L47" s="83"/>
-      <c r="M47" s="45" t="s">
-        <v>36</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="J47" s="100"/>
+      <c r="K47" s="100"/>
+      <c r="L47" s="100"/>
+      <c r="M47" s="106"/>
       <c r="N47" s="2"/>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.25">
@@ -2301,21 +2339,21 @@
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="C48" s="73" t="s">
-        <v>11</v>
-      </c>
-      <c r="D48" s="67"/>
-      <c r="E48" s="67"/>
-      <c r="F48" s="67"/>
-      <c r="G48" s="67"/>
-      <c r="H48" s="48"/>
+      <c r="C48" s="80"/>
+      <c r="D48" s="74"/>
+      <c r="E48" s="74"/>
+      <c r="F48" s="74"/>
+      <c r="G48" s="74"/>
+      <c r="H48" s="74"/>
       <c r="I48" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J48" s="82"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
-      <c r="M48" s="93"/>
+        <v>35</v>
+      </c>
+      <c r="J48" s="89"/>
+      <c r="K48" s="89"/>
+      <c r="L48" s="89"/>
+      <c r="M48" s="106" t="s">
+        <v>36</v>
+      </c>
       <c r="N48" s="2"/>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.25">
@@ -2323,21 +2361,21 @@
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="C49" s="57"/>
-      <c r="D49" s="63" t="s">
-        <v>41</v>
-      </c>
-      <c r="E49" s="63"/>
-      <c r="F49" s="63"/>
-      <c r="G49" s="63"/>
-      <c r="H49" s="63"/>
+      <c r="C49" s="80" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="74"/>
+      <c r="E49" s="74"/>
+      <c r="F49" s="74"/>
+      <c r="G49" s="74"/>
+      <c r="H49" s="55"/>
       <c r="I49" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J49" s="82"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
-      <c r="M49" s="93"/>
+        <v>15</v>
+      </c>
+      <c r="J49" s="100"/>
+      <c r="K49" s="100"/>
+      <c r="L49" s="100"/>
+      <c r="M49" s="106"/>
       <c r="N49" s="2"/>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.25">
@@ -2345,19 +2383,21 @@
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="C50" s="61"/>
-      <c r="D50" s="67"/>
-      <c r="E50" s="67"/>
-      <c r="F50" s="67"/>
-      <c r="G50" s="67"/>
-      <c r="H50" s="67"/>
+      <c r="C50" s="64"/>
+      <c r="D50" s="70" t="s">
+        <v>41</v>
+      </c>
+      <c r="E50" s="70"/>
+      <c r="F50" s="70"/>
+      <c r="G50" s="70"/>
+      <c r="H50" s="70"/>
       <c r="I50" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J50" s="82"/>
-      <c r="K50" s="4"/>
-      <c r="L50" s="4"/>
-      <c r="M50" s="93"/>
+        <v>14</v>
+      </c>
+      <c r="J50" s="100"/>
+      <c r="K50" s="100"/>
+      <c r="L50" s="100"/>
+      <c r="M50" s="106"/>
       <c r="N50" s="2"/>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.25">
@@ -2365,19 +2405,19 @@
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="C51" s="5"/>
-      <c r="D51" s="48" t="s">
-        <v>42</v>
-      </c>
-      <c r="E51" s="48"/>
-      <c r="F51" s="48"/>
-      <c r="G51" s="48"/>
-      <c r="H51" s="48"/>
-      <c r="I51" s="4"/>
-      <c r="J51" s="82"/>
-      <c r="K51" s="4"/>
-      <c r="L51" s="4"/>
-      <c r="M51" s="4"/>
+      <c r="C51" s="68"/>
+      <c r="D51" s="74"/>
+      <c r="E51" s="74"/>
+      <c r="F51" s="74"/>
+      <c r="G51" s="74"/>
+      <c r="H51" s="74"/>
+      <c r="I51" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J51" s="100"/>
+      <c r="K51" s="100"/>
+      <c r="L51" s="100"/>
+      <c r="M51" s="106"/>
       <c r="N51" s="2"/>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.25">
@@ -2385,21 +2425,19 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="C52" s="57"/>
-      <c r="D52" s="58"/>
-      <c r="E52" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="F52" s="63"/>
-      <c r="G52" s="63"/>
-      <c r="H52" s="63"/>
-      <c r="I52" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J52" s="82"/>
-      <c r="K52" s="4"/>
-      <c r="L52" s="4"/>
-      <c r="M52" s="93"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="E52" s="55"/>
+      <c r="F52" s="55"/>
+      <c r="G52" s="55"/>
+      <c r="H52" s="55"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="100"/>
+      <c r="K52" s="100"/>
+      <c r="L52" s="100"/>
+      <c r="M52" s="106"/>
       <c r="N52" s="2"/>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.25">
@@ -2407,21 +2445,21 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="C53" s="59"/>
-      <c r="D53" s="60"/>
-      <c r="E53" s="65"/>
-      <c r="F53" s="65"/>
-      <c r="G53" s="65"/>
-      <c r="H53" s="65"/>
+      <c r="C53" s="64"/>
+      <c r="D53" s="65"/>
+      <c r="E53" s="70" t="s">
+        <v>20</v>
+      </c>
+      <c r="F53" s="70"/>
+      <c r="G53" s="70"/>
+      <c r="H53" s="70"/>
       <c r="I53" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J53" s="82"/>
-      <c r="K53" s="20"/>
-      <c r="L53" s="20"/>
-      <c r="M53" s="86" t="s">
-        <v>28</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="J53" s="100"/>
+      <c r="K53" s="100"/>
+      <c r="L53" s="100"/>
+      <c r="M53" s="106"/>
       <c r="N53" s="2"/>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.25">
@@ -2429,19 +2467,21 @@
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="C54" s="59"/>
-      <c r="D54" s="60"/>
-      <c r="E54" s="65"/>
-      <c r="F54" s="65"/>
-      <c r="G54" s="65"/>
-      <c r="H54" s="65"/>
+      <c r="C54" s="66"/>
+      <c r="D54" s="67"/>
+      <c r="E54" s="72"/>
+      <c r="F54" s="72"/>
+      <c r="G54" s="72"/>
+      <c r="H54" s="72"/>
       <c r="I54" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J54" s="82"/>
-      <c r="K54" s="4"/>
-      <c r="L54" s="4"/>
-      <c r="M54" s="45"/>
+        <v>26</v>
+      </c>
+      <c r="J54" s="100"/>
+      <c r="K54" s="90"/>
+      <c r="L54" s="90"/>
+      <c r="M54" s="92" t="s">
+        <v>28</v>
+      </c>
       <c r="N54" s="2"/>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.25">
@@ -2449,21 +2489,19 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="C55" s="61"/>
-      <c r="D55" s="62"/>
-      <c r="E55" s="67"/>
-      <c r="F55" s="67"/>
-      <c r="G55" s="67"/>
-      <c r="H55" s="67"/>
+      <c r="C55" s="66"/>
+      <c r="D55" s="67"/>
+      <c r="E55" s="72"/>
+      <c r="F55" s="72"/>
+      <c r="G55" s="72"/>
+      <c r="H55" s="72"/>
       <c r="I55" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J55" s="82"/>
-      <c r="K55" s="20"/>
-      <c r="L55" s="20"/>
-      <c r="M55" s="86" t="s">
-        <v>29</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="J55" s="100"/>
+      <c r="K55" s="100"/>
+      <c r="L55" s="100"/>
+      <c r="M55" s="106"/>
       <c r="N55" s="2"/>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.25">
@@ -2471,21 +2509,21 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="C56" s="5"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="G56" s="48"/>
-      <c r="H56" s="48"/>
+      <c r="C56" s="68"/>
+      <c r="D56" s="69"/>
+      <c r="E56" s="74"/>
+      <c r="F56" s="74"/>
+      <c r="G56" s="74"/>
+      <c r="H56" s="74"/>
       <c r="I56" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J56" s="82"/>
-      <c r="K56" s="4"/>
-      <c r="L56" s="4"/>
-      <c r="M56" s="93"/>
+        <v>43</v>
+      </c>
+      <c r="J56" s="100"/>
+      <c r="K56" s="90"/>
+      <c r="L56" s="90"/>
+      <c r="M56" s="92" t="s">
+        <v>29</v>
+      </c>
       <c r="N56" s="2"/>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.25">
@@ -2493,21 +2531,21 @@
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="C57" s="57"/>
-      <c r="D57" s="58"/>
-      <c r="E57" s="63" t="s">
-        <v>21</v>
-      </c>
-      <c r="F57" s="63"/>
-      <c r="G57" s="63"/>
-      <c r="H57" s="63"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="G57" s="55"/>
+      <c r="H57" s="55"/>
       <c r="I57" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J57" s="82"/>
-      <c r="K57" s="4"/>
-      <c r="L57" s="4"/>
-      <c r="M57" s="93"/>
+        <v>22</v>
+      </c>
+      <c r="J57" s="100"/>
+      <c r="K57" s="100"/>
+      <c r="L57" s="100"/>
+      <c r="M57" s="106"/>
       <c r="N57" s="2"/>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.25">
@@ -2515,19 +2553,21 @@
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="C58" s="59"/>
-      <c r="D58" s="60"/>
-      <c r="E58" s="65"/>
-      <c r="F58" s="65"/>
-      <c r="G58" s="65"/>
-      <c r="H58" s="65"/>
+      <c r="C58" s="64"/>
+      <c r="D58" s="65"/>
+      <c r="E58" s="70" t="s">
+        <v>21</v>
+      </c>
+      <c r="F58" s="70"/>
+      <c r="G58" s="70"/>
+      <c r="H58" s="70"/>
       <c r="I58" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J58" s="82"/>
-      <c r="K58" s="4"/>
-      <c r="L58" s="4"/>
-      <c r="M58" s="93"/>
+        <v>25</v>
+      </c>
+      <c r="J58" s="100"/>
+      <c r="K58" s="100"/>
+      <c r="L58" s="100"/>
+      <c r="M58" s="106"/>
       <c r="N58" s="2"/>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.25">
@@ -2535,19 +2575,19 @@
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="C59" s="59"/>
-      <c r="D59" s="60"/>
-      <c r="E59" s="65"/>
-      <c r="F59" s="65"/>
-      <c r="G59" s="65"/>
-      <c r="H59" s="65"/>
+      <c r="C59" s="66"/>
+      <c r="D59" s="67"/>
+      <c r="E59" s="72"/>
+      <c r="F59" s="72"/>
+      <c r="G59" s="72"/>
+      <c r="H59" s="72"/>
       <c r="I59" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="J59" s="82"/>
-      <c r="K59" s="4"/>
-      <c r="L59" s="4"/>
-      <c r="M59" s="93"/>
+        <v>28</v>
+      </c>
+      <c r="J59" s="100"/>
+      <c r="K59" s="100"/>
+      <c r="L59" s="100"/>
+      <c r="M59" s="106"/>
       <c r="N59" s="2"/>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.25">
@@ -2555,19 +2595,19 @@
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="C60" s="59"/>
-      <c r="D60" s="60"/>
-      <c r="E60" s="65"/>
-      <c r="F60" s="65"/>
-      <c r="G60" s="65"/>
-      <c r="H60" s="65"/>
+      <c r="C60" s="66"/>
+      <c r="D60" s="67"/>
+      <c r="E60" s="72"/>
+      <c r="F60" s="72"/>
+      <c r="G60" s="72"/>
+      <c r="H60" s="72"/>
       <c r="I60" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J60" s="82"/>
-      <c r="K60" s="4"/>
-      <c r="L60" s="4"/>
-      <c r="M60" s="93"/>
+        <v>40</v>
+      </c>
+      <c r="J60" s="100"/>
+      <c r="K60" s="100"/>
+      <c r="L60" s="100"/>
+      <c r="M60" s="106"/>
       <c r="N60" s="2"/>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.25">
@@ -2575,19 +2615,19 @@
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="C61" s="59"/>
-      <c r="D61" s="60"/>
-      <c r="E61" s="65"/>
-      <c r="F61" s="65"/>
-      <c r="G61" s="65"/>
-      <c r="H61" s="65"/>
+      <c r="C61" s="66"/>
+      <c r="D61" s="67"/>
+      <c r="E61" s="72"/>
+      <c r="F61" s="72"/>
+      <c r="G61" s="72"/>
+      <c r="H61" s="72"/>
       <c r="I61" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J61" s="82"/>
-      <c r="K61" s="4"/>
-      <c r="L61" s="4"/>
-      <c r="M61" s="93"/>
+        <v>27</v>
+      </c>
+      <c r="J61" s="100"/>
+      <c r="K61" s="100"/>
+      <c r="L61" s="100"/>
+      <c r="M61" s="106"/>
       <c r="N61" s="2"/>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.25">
@@ -2595,21 +2635,19 @@
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="C62" s="57"/>
-      <c r="D62" s="58"/>
-      <c r="E62" s="58"/>
-      <c r="F62" s="63" t="s">
-        <v>44</v>
-      </c>
-      <c r="G62" s="63"/>
-      <c r="H62" s="63"/>
+      <c r="C62" s="66"/>
+      <c r="D62" s="67"/>
+      <c r="E62" s="72"/>
+      <c r="F62" s="72"/>
+      <c r="G62" s="72"/>
+      <c r="H62" s="72"/>
       <c r="I62" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="J62" s="82"/>
-      <c r="K62" s="4"/>
-      <c r="L62" s="4"/>
-      <c r="M62" s="93"/>
+        <v>43</v>
+      </c>
+      <c r="J62" s="100"/>
+      <c r="K62" s="100"/>
+      <c r="L62" s="100"/>
+      <c r="M62" s="106"/>
       <c r="N62" s="2"/>
     </row>
     <row r="63" spans="2:14" x14ac:dyDescent="0.25">
@@ -2617,19 +2655,21 @@
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="C63" s="59"/>
-      <c r="D63" s="60"/>
-      <c r="E63" s="60"/>
-      <c r="F63" s="65"/>
-      <c r="G63" s="65"/>
-      <c r="H63" s="65"/>
+      <c r="C63" s="64"/>
+      <c r="D63" s="65"/>
+      <c r="E63" s="65"/>
+      <c r="F63" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="G63" s="70"/>
+      <c r="H63" s="70"/>
       <c r="I63" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="J63" s="82"/>
-      <c r="K63" s="4"/>
-      <c r="L63" s="4"/>
-      <c r="M63" s="93"/>
+        <v>45</v>
+      </c>
+      <c r="J63" s="100"/>
+      <c r="K63" s="100"/>
+      <c r="L63" s="100"/>
+      <c r="M63" s="106"/>
       <c r="N63" s="2"/>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.25">
@@ -2637,19 +2677,19 @@
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="C64" s="59"/>
-      <c r="D64" s="60"/>
-      <c r="E64" s="60"/>
-      <c r="F64" s="65"/>
-      <c r="G64" s="65"/>
-      <c r="H64" s="65"/>
+      <c r="C64" s="66"/>
+      <c r="D64" s="67"/>
+      <c r="E64" s="67"/>
+      <c r="F64" s="72"/>
+      <c r="G64" s="72"/>
+      <c r="H64" s="72"/>
       <c r="I64" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="J64" s="82"/>
-      <c r="K64" s="4"/>
-      <c r="L64" s="4"/>
-      <c r="M64" s="93"/>
+        <v>46</v>
+      </c>
+      <c r="J64" s="100"/>
+      <c r="K64" s="100"/>
+      <c r="L64" s="100"/>
+      <c r="M64" s="106"/>
       <c r="N64" s="2"/>
     </row>
     <row r="65" spans="2:14" x14ac:dyDescent="0.25">
@@ -2657,21 +2697,19 @@
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="C65" s="61"/>
-      <c r="D65" s="62"/>
-      <c r="E65" s="62"/>
-      <c r="F65" s="67"/>
-      <c r="G65" s="67"/>
-      <c r="H65" s="67"/>
+      <c r="C65" s="66"/>
+      <c r="D65" s="67"/>
+      <c r="E65" s="67"/>
+      <c r="F65" s="72"/>
+      <c r="G65" s="72"/>
+      <c r="H65" s="72"/>
       <c r="I65" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="J65" s="82"/>
-      <c r="K65" s="10"/>
-      <c r="L65" s="10"/>
-      <c r="M65" s="45" t="s">
-        <v>59</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="J65" s="100"/>
+      <c r="K65" s="100"/>
+      <c r="L65" s="100"/>
+      <c r="M65" s="106"/>
       <c r="N65" s="2"/>
     </row>
     <row r="66" spans="2:14" x14ac:dyDescent="0.25">
@@ -2679,21 +2717,21 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="C66" s="5"/>
-      <c r="D66" s="9"/>
-      <c r="E66" s="9"/>
-      <c r="F66" s="9"/>
-      <c r="G66" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="H66" s="48"/>
+      <c r="C66" s="68"/>
+      <c r="D66" s="69"/>
+      <c r="E66" s="69"/>
+      <c r="F66" s="74"/>
+      <c r="G66" s="74"/>
+      <c r="H66" s="74"/>
       <c r="I66" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="J66" s="82"/>
-      <c r="K66" s="4"/>
-      <c r="L66" s="4"/>
-      <c r="M66" s="93"/>
+        <v>58</v>
+      </c>
+      <c r="J66" s="100"/>
+      <c r="K66" s="89"/>
+      <c r="L66" s="89"/>
+      <c r="M66" s="106" t="s">
+        <v>59</v>
+      </c>
       <c r="N66" s="2"/>
     </row>
     <row r="67" spans="2:14" x14ac:dyDescent="0.25">
@@ -2701,19 +2739,21 @@
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="C67" s="52"/>
-      <c r="D67" s="53"/>
-      <c r="E67" s="53"/>
-      <c r="F67" s="53"/>
-      <c r="G67" s="48" t="s">
-        <v>48</v>
-      </c>
-      <c r="H67" s="48"/>
-      <c r="I67" s="4"/>
-      <c r="J67" s="82"/>
-      <c r="K67" s="4"/>
-      <c r="L67" s="4"/>
-      <c r="M67" s="93"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="H67" s="55"/>
+      <c r="I67" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J67" s="100"/>
+      <c r="K67" s="100"/>
+      <c r="L67" s="100"/>
+      <c r="M67" s="106"/>
       <c r="N67" s="2"/>
     </row>
     <row r="68" spans="2:14" x14ac:dyDescent="0.25">
@@ -2721,17 +2761,19 @@
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="C68" s="5"/>
-      <c r="D68" s="9"/>
-      <c r="E68" s="9"/>
-      <c r="F68" s="9"/>
-      <c r="G68" s="9"/>
-      <c r="H68" s="9"/>
+      <c r="C68" s="59"/>
+      <c r="D68" s="60"/>
+      <c r="E68" s="60"/>
+      <c r="F68" s="60"/>
+      <c r="G68" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="H68" s="55"/>
       <c r="I68" s="4"/>
-      <c r="J68" s="82"/>
-      <c r="K68" s="4"/>
-      <c r="L68" s="4"/>
-      <c r="M68" s="93"/>
+      <c r="J68" s="100"/>
+      <c r="K68" s="100"/>
+      <c r="L68" s="100"/>
+      <c r="M68" s="106"/>
       <c r="N68" s="2"/>
     </row>
     <row r="69" spans="2:14" x14ac:dyDescent="0.25">
@@ -2746,10 +2788,10 @@
       <c r="G69" s="9"/>
       <c r="H69" s="9"/>
       <c r="I69" s="4"/>
-      <c r="J69" s="82"/>
-      <c r="K69" s="4"/>
-      <c r="L69" s="4"/>
-      <c r="M69" s="93"/>
+      <c r="J69" s="100"/>
+      <c r="K69" s="100"/>
+      <c r="L69" s="100"/>
+      <c r="M69" s="106"/>
       <c r="N69" s="2"/>
     </row>
     <row r="70" spans="2:14" x14ac:dyDescent="0.25">
@@ -2764,10 +2806,10 @@
       <c r="G70" s="9"/>
       <c r="H70" s="9"/>
       <c r="I70" s="4"/>
-      <c r="J70" s="82"/>
-      <c r="K70" s="4"/>
-      <c r="L70" s="4"/>
-      <c r="M70" s="93"/>
+      <c r="J70" s="100"/>
+      <c r="K70" s="100"/>
+      <c r="L70" s="100"/>
+      <c r="M70" s="106"/>
       <c r="N70" s="2"/>
     </row>
     <row r="71" spans="2:14" x14ac:dyDescent="0.25">
@@ -2782,10 +2824,10 @@
       <c r="G71" s="9"/>
       <c r="H71" s="9"/>
       <c r="I71" s="4"/>
-      <c r="J71" s="82"/>
-      <c r="K71" s="4"/>
-      <c r="L71" s="4"/>
-      <c r="M71" s="93"/>
+      <c r="J71" s="100"/>
+      <c r="K71" s="100"/>
+      <c r="L71" s="100"/>
+      <c r="M71" s="106"/>
       <c r="N71" s="2"/>
     </row>
     <row r="72" spans="2:14" x14ac:dyDescent="0.25">
@@ -2800,15 +2842,15 @@
       <c r="G72" s="9"/>
       <c r="H72" s="9"/>
       <c r="I72" s="4"/>
-      <c r="J72" s="82"/>
-      <c r="K72" s="4"/>
-      <c r="L72" s="4"/>
-      <c r="M72" s="93"/>
+      <c r="J72" s="100"/>
+      <c r="K72" s="100"/>
+      <c r="L72" s="100"/>
+      <c r="M72" s="106"/>
       <c r="N72" s="2"/>
     </row>
     <row r="73" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B73" s="11">
-        <f t="shared" ref="B73:B77" si="1">B72+1</f>
+        <f t="shared" si="0"/>
         <v>67</v>
       </c>
       <c r="C73" s="5"/>
@@ -2818,15 +2860,15 @@
       <c r="G73" s="9"/>
       <c r="H73" s="9"/>
       <c r="I73" s="4"/>
-      <c r="J73" s="82"/>
-      <c r="K73" s="4"/>
-      <c r="L73" s="4"/>
-      <c r="M73" s="93"/>
+      <c r="J73" s="100"/>
+      <c r="K73" s="100"/>
+      <c r="L73" s="100"/>
+      <c r="M73" s="106"/>
       <c r="N73" s="2"/>
     </row>
     <row r="74" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B74" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="B74:B78" si="1">B73+1</f>
         <v>68</v>
       </c>
       <c r="C74" s="5"/>
@@ -2836,10 +2878,10 @@
       <c r="G74" s="9"/>
       <c r="H74" s="9"/>
       <c r="I74" s="4"/>
-      <c r="J74" s="82"/>
-      <c r="K74" s="4"/>
-      <c r="L74" s="4"/>
-      <c r="M74" s="93"/>
+      <c r="J74" s="100"/>
+      <c r="K74" s="100"/>
+      <c r="L74" s="100"/>
+      <c r="M74" s="106"/>
       <c r="N74" s="2"/>
     </row>
     <row r="75" spans="2:14" x14ac:dyDescent="0.25">
@@ -2854,10 +2896,10 @@
       <c r="G75" s="9"/>
       <c r="H75" s="9"/>
       <c r="I75" s="4"/>
-      <c r="J75" s="82"/>
-      <c r="K75" s="4"/>
-      <c r="L75" s="4"/>
-      <c r="M75" s="93"/>
+      <c r="J75" s="100"/>
+      <c r="K75" s="100"/>
+      <c r="L75" s="100"/>
+      <c r="M75" s="106"/>
       <c r="N75" s="2"/>
     </row>
     <row r="76" spans="2:14" x14ac:dyDescent="0.25">
@@ -2872,10 +2914,10 @@
       <c r="G76" s="9"/>
       <c r="H76" s="9"/>
       <c r="I76" s="4"/>
-      <c r="J76" s="82"/>
-      <c r="K76" s="4"/>
-      <c r="L76" s="4"/>
-      <c r="M76" s="93"/>
+      <c r="J76" s="100"/>
+      <c r="K76" s="100"/>
+      <c r="L76" s="100"/>
+      <c r="M76" s="106"/>
       <c r="N76" s="2"/>
     </row>
     <row r="77" spans="2:14" x14ac:dyDescent="0.25">
@@ -2890,55 +2932,74 @@
       <c r="G77" s="9"/>
       <c r="H77" s="9"/>
       <c r="I77" s="4"/>
-      <c r="J77" s="82"/>
-      <c r="K77" s="4"/>
-      <c r="L77" s="4"/>
-      <c r="M77" s="93"/>
+      <c r="J77" s="100"/>
+      <c r="K77" s="100"/>
+      <c r="L77" s="100"/>
+      <c r="M77" s="106"/>
       <c r="N77" s="2"/>
     </row>
+    <row r="78" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B78" s="11">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="C78" s="5"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="9"/>
+      <c r="H78" s="9"/>
+      <c r="I78" s="4"/>
+      <c r="J78" s="100"/>
+      <c r="K78" s="100"/>
+      <c r="L78" s="100"/>
+      <c r="M78" s="106"/>
+      <c r="N78" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="41">
+  <mergeCells count="42">
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="K10:K13"/>
-    <mergeCell ref="M10:M15"/>
+    <mergeCell ref="M10:M16"/>
     <mergeCell ref="K6:L6"/>
+    <mergeCell ref="E14:E15"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="C7:H7"/>
     <mergeCell ref="D8:H8"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="C67:F67"/>
     <mergeCell ref="G67:H67"/>
-    <mergeCell ref="C62:E65"/>
-    <mergeCell ref="F62:H65"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="C57:D61"/>
-    <mergeCell ref="E57:H61"/>
-    <mergeCell ref="C52:D55"/>
-    <mergeCell ref="E52:H55"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="D49:H50"/>
-    <mergeCell ref="D51:H51"/>
-    <mergeCell ref="C43:E47"/>
-    <mergeCell ref="F43:H47"/>
-    <mergeCell ref="C48:H48"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="C41:E42"/>
-    <mergeCell ref="F41:H42"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:H37"/>
-    <mergeCell ref="C38:E39"/>
-    <mergeCell ref="F38:H39"/>
-    <mergeCell ref="E31:H31"/>
-    <mergeCell ref="C32:E36"/>
-    <mergeCell ref="F32:H36"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:H27"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="D28:H30"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="C24:H25"/>
-    <mergeCell ref="D22:H22"/>
+    <mergeCell ref="C68:F68"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="C63:E66"/>
+    <mergeCell ref="F63:H66"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="C58:D62"/>
+    <mergeCell ref="E58:H62"/>
+    <mergeCell ref="C53:D56"/>
+    <mergeCell ref="E53:H56"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:H51"/>
+    <mergeCell ref="D52:H52"/>
+    <mergeCell ref="C44:E48"/>
+    <mergeCell ref="F44:H48"/>
+    <mergeCell ref="C49:H49"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="C42:E43"/>
+    <mergeCell ref="F42:H43"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:H38"/>
+    <mergeCell ref="C39:E40"/>
+    <mergeCell ref="F39:H40"/>
+    <mergeCell ref="E32:H32"/>
+    <mergeCell ref="C33:E37"/>
+    <mergeCell ref="F33:H37"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:H28"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="D29:H31"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C25:H26"/>
+    <mergeCell ref="D23:H23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3004,18 +3065,18 @@
       <c r="B5" s="11">
         <v>1</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="69" t="s">
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="50"/>
+      <c r="J5" s="57"/>
       <c r="K5" s="4" t="s">
         <v>6</v>
       </c>
@@ -3026,14 +3087,14 @@
         <f>B5+1</f>
         <v>2</v>
       </c>
-      <c r="C6" s="79" t="s">
+      <c r="C6" s="86" t="s">
         <v>86</v>
       </c>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="49"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="56"/>
       <c r="I6" s="23"/>
       <c r="J6" s="24"/>
       <c r="K6" s="10" t="s">
@@ -3042,22 +3103,22 @@
       <c r="L6" s="4"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="54">
+      <c r="B7" s="61">
         <f>B6+1</f>
         <v>3</v>
       </c>
-      <c r="C7" s="71" t="s">
+      <c r="C7" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="64"/>
-      <c r="I7" s="69" t="s">
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="71"/>
+      <c r="I7" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="50"/>
+      <c r="J7" s="57"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="N7" s="20" t="s">
@@ -3065,17 +3126,17 @@
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="56"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="68"/>
-      <c r="I8" s="69" t="s">
+      <c r="B8" s="63"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="74"/>
+      <c r="G8" s="74"/>
+      <c r="H8" s="75"/>
+      <c r="I8" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="J8" s="50"/>
+      <c r="J8" s="57"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="N8" s="4" t="s">
@@ -3083,22 +3144,22 @@
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="54">
+      <c r="B9" s="61">
         <f>B7+1</f>
         <v>4</v>
       </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="63" t="s">
+      <c r="C9" s="64"/>
+      <c r="D9" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="64"/>
-      <c r="I9" s="69" t="s">
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="50"/>
+      <c r="J9" s="57"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="N9" s="10" t="s">
@@ -3106,67 +3167,67 @@
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="56"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="68"/>
-      <c r="I10" s="69" t="s">
+      <c r="B10" s="63"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="75"/>
+      <c r="I10" s="76" t="s">
         <v>49</v>
       </c>
-      <c r="J10" s="50"/>
+      <c r="J10" s="57"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="54">
+      <c r="B11" s="61">
         <f>B9+1</f>
         <v>5</v>
       </c>
-      <c r="C11" s="57"/>
-      <c r="D11" s="63" t="s">
+      <c r="C11" s="64"/>
+      <c r="D11" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="64"/>
-      <c r="I11" s="69" t="s">
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="50"/>
+      <c r="J11" s="57"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="55"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="65"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="65"/>
-      <c r="H12" s="66"/>
-      <c r="I12" s="69" t="s">
+      <c r="B12" s="62"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="72"/>
+      <c r="H12" s="73"/>
+      <c r="I12" s="76" t="s">
         <v>50</v>
       </c>
-      <c r="J12" s="50"/>
+      <c r="J12" s="57"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="56"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="68"/>
-      <c r="I13" s="69" t="s">
+      <c r="B13" s="63"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="75"/>
+      <c r="I13" s="76" t="s">
         <v>54</v>
       </c>
-      <c r="J13" s="50"/>
+      <c r="J13" s="57"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
     </row>
@@ -3177,62 +3238,62 @@
       </c>
       <c r="C14" s="26"/>
       <c r="D14" s="25"/>
-      <c r="E14" s="48" t="s">
+      <c r="E14" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="69" t="s">
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="56"/>
+      <c r="I14" s="76" t="s">
         <v>57</v>
       </c>
-      <c r="J14" s="50"/>
+      <c r="J14" s="57"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="54">
+      <c r="B15" s="61">
         <f>B14+1</f>
         <v>7</v>
       </c>
-      <c r="C15" s="57"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="63" t="s">
+      <c r="C15" s="64"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="63"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="69" t="s">
+      <c r="G15" s="70"/>
+      <c r="H15" s="71"/>
+      <c r="I15" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="J15" s="50"/>
+      <c r="J15" s="57"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="55"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="66"/>
-      <c r="I16" s="69" t="s">
+      <c r="B16" s="62"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="72"/>
+      <c r="G16" s="72"/>
+      <c r="H16" s="73"/>
+      <c r="I16" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="J16" s="74"/>
-      <c r="K16" s="74"/>
-      <c r="L16" s="74"/>
+      <c r="J16" s="81"/>
+      <c r="K16" s="81"/>
+      <c r="L16" s="81"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="55"/>
-      <c r="C17" s="59"/>
-      <c r="D17" s="60"/>
-      <c r="E17" s="60"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="66"/>
+      <c r="B17" s="62"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="72"/>
+      <c r="G17" s="72"/>
+      <c r="H17" s="73"/>
       <c r="I17" s="7"/>
       <c r="J17" s="8" t="s">
         <v>32</v>
@@ -3241,13 +3302,13 @@
       <c r="L17" s="4"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="55"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="65"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="66"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="72"/>
+      <c r="H18" s="73"/>
       <c r="I18" s="7"/>
       <c r="J18" s="8" t="s">
         <v>34</v>
@@ -3256,13 +3317,13 @@
       <c r="L18" s="4"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="56"/>
-      <c r="C19" s="61"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="62"/>
-      <c r="F19" s="67"/>
-      <c r="G19" s="67"/>
-      <c r="H19" s="68"/>
+      <c r="B19" s="63"/>
+      <c r="C19" s="68"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="74"/>
+      <c r="G19" s="74"/>
+      <c r="H19" s="75"/>
       <c r="I19" s="7"/>
       <c r="J19" s="8" t="s">
         <v>35</v>
@@ -3277,53 +3338,53 @@
         <f>B15+1</f>
         <v>8</v>
       </c>
-      <c r="C20" s="52"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="48" t="s">
+      <c r="C20" s="59"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="69" t="s">
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="76" t="s">
         <v>56</v>
       </c>
-      <c r="J20" s="50"/>
+      <c r="J20" s="57"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="54">
+      <c r="B21" s="61">
         <f>B20+1</f>
         <v>9</v>
       </c>
-      <c r="C21" s="57"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="58"/>
-      <c r="F21" s="63" t="s">
+      <c r="C21" s="64"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="65"/>
+      <c r="F21" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="63"/>
-      <c r="H21" s="64"/>
-      <c r="I21" s="69" t="s">
+      <c r="G21" s="70"/>
+      <c r="H21" s="71"/>
+      <c r="I21" s="76" t="s">
         <v>55</v>
       </c>
-      <c r="J21" s="50"/>
+      <c r="J21" s="57"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="56"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="67"/>
-      <c r="G22" s="67"/>
-      <c r="H22" s="68"/>
-      <c r="I22" s="69" t="s">
+      <c r="B22" s="63"/>
+      <c r="C22" s="68"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="74"/>
+      <c r="G22" s="74"/>
+      <c r="H22" s="75"/>
+      <c r="I22" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="J22" s="50"/>
+      <c r="J22" s="57"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
     </row>
@@ -3335,96 +3396,96 @@
       <c r="C23" s="5"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
-      <c r="F23" s="48" t="s">
+      <c r="F23" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="G23" s="48"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="69" t="s">
+      <c r="G23" s="55"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="J23" s="50"/>
+      <c r="J23" s="57"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="54">
+      <c r="B24" s="61">
         <f t="shared" ref="B24:B40" si="0">B23+1</f>
         <v>11</v>
       </c>
-      <c r="C24" s="57"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="58"/>
-      <c r="F24" s="63" t="s">
+      <c r="C24" s="64"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="G24" s="63"/>
-      <c r="H24" s="64"/>
-      <c r="I24" s="77" t="s">
+      <c r="G24" s="70"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="J24" s="78"/>
+      <c r="J24" s="85"/>
       <c r="K24" s="18"/>
       <c r="L24" s="18"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="56"/>
-      <c r="C25" s="61"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="62"/>
-      <c r="F25" s="67"/>
-      <c r="G25" s="67"/>
-      <c r="H25" s="68"/>
-      <c r="I25" s="69" t="s">
+      <c r="B25" s="63"/>
+      <c r="C25" s="68"/>
+      <c r="D25" s="69"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="75"/>
+      <c r="I25" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="J25" s="50"/>
+      <c r="J25" s="57"/>
       <c r="K25" s="18"/>
       <c r="L25" s="18"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="54">
+      <c r="B26" s="61">
         <f>B24+1</f>
         <v>12</v>
       </c>
-      <c r="C26" s="71"/>
-      <c r="D26" s="63"/>
-      <c r="E26" s="63"/>
-      <c r="F26" s="63" t="s">
+      <c r="C26" s="78"/>
+      <c r="D26" s="70"/>
+      <c r="E26" s="70"/>
+      <c r="F26" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="G26" s="63"/>
-      <c r="H26" s="64"/>
-      <c r="I26" s="69" t="s">
+      <c r="G26" s="70"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="J26" s="50"/>
+      <c r="J26" s="57"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="55"/>
-      <c r="C27" s="72"/>
-      <c r="D27" s="65"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="65"/>
-      <c r="G27" s="65"/>
-      <c r="H27" s="66"/>
-      <c r="I27" s="69" t="s">
+      <c r="B27" s="62"/>
+      <c r="C27" s="79"/>
+      <c r="D27" s="72"/>
+      <c r="E27" s="72"/>
+      <c r="F27" s="72"/>
+      <c r="G27" s="72"/>
+      <c r="H27" s="73"/>
+      <c r="I27" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="J27" s="74"/>
-      <c r="K27" s="74"/>
-      <c r="L27" s="74"/>
+      <c r="J27" s="81"/>
+      <c r="K27" s="81"/>
+      <c r="L27" s="81"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="55"/>
-      <c r="C28" s="72"/>
-      <c r="D28" s="65"/>
-      <c r="E28" s="65"/>
-      <c r="F28" s="65"/>
-      <c r="G28" s="65"/>
-      <c r="H28" s="66"/>
+      <c r="B28" s="62"/>
+      <c r="C28" s="79"/>
+      <c r="D28" s="72"/>
+      <c r="E28" s="72"/>
+      <c r="F28" s="72"/>
+      <c r="G28" s="72"/>
+      <c r="H28" s="73"/>
       <c r="I28" s="7"/>
       <c r="J28" s="8" t="s">
         <v>32</v>
@@ -3433,13 +3494,13 @@
       <c r="L28" s="4"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="55"/>
-      <c r="C29" s="72"/>
-      <c r="D29" s="65"/>
-      <c r="E29" s="65"/>
-      <c r="F29" s="65"/>
-      <c r="G29" s="65"/>
-      <c r="H29" s="66"/>
+      <c r="B29" s="62"/>
+      <c r="C29" s="79"/>
+      <c r="D29" s="72"/>
+      <c r="E29" s="72"/>
+      <c r="F29" s="72"/>
+      <c r="G29" s="72"/>
+      <c r="H29" s="73"/>
       <c r="I29" s="7"/>
       <c r="J29" s="8" t="s">
         <v>34</v>
@@ -3448,13 +3509,13 @@
       <c r="L29" s="4"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B30" s="56"/>
-      <c r="C30" s="73"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="67"/>
-      <c r="G30" s="67"/>
-      <c r="H30" s="68"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="80"/>
+      <c r="D30" s="74"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="74"/>
+      <c r="G30" s="74"/>
+      <c r="H30" s="75"/>
       <c r="I30" s="7"/>
       <c r="J30" s="8" t="s">
         <v>35</v>
@@ -3469,53 +3530,53 @@
         <f>B26+1</f>
         <v>13</v>
       </c>
-      <c r="C31" s="73" t="s">
+      <c r="C31" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="67"/>
-      <c r="E31" s="67"/>
-      <c r="F31" s="67"/>
-      <c r="G31" s="67"/>
-      <c r="H31" s="49"/>
-      <c r="I31" s="75" t="s">
+      <c r="D31" s="74"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="74"/>
+      <c r="G31" s="74"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="J31" s="76"/>
+      <c r="J31" s="83"/>
       <c r="K31" s="19"/>
       <c r="L31" s="19"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="54">
+      <c r="B32" s="61">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C32" s="57"/>
-      <c r="D32" s="63" t="s">
+      <c r="C32" s="64"/>
+      <c r="D32" s="70" t="s">
         <v>41</v>
       </c>
-      <c r="E32" s="63"/>
-      <c r="F32" s="63"/>
-      <c r="G32" s="63"/>
-      <c r="H32" s="64"/>
-      <c r="I32" s="69" t="s">
+      <c r="E32" s="70"/>
+      <c r="F32" s="70"/>
+      <c r="G32" s="70"/>
+      <c r="H32" s="71"/>
+      <c r="I32" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="J32" s="50"/>
+      <c r="J32" s="57"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B33" s="56"/>
-      <c r="C33" s="61"/>
-      <c r="D33" s="67"/>
-      <c r="E33" s="67"/>
-      <c r="F33" s="67"/>
-      <c r="G33" s="67"/>
-      <c r="H33" s="68"/>
-      <c r="I33" s="69" t="s">
+      <c r="B33" s="63"/>
+      <c r="C33" s="68"/>
+      <c r="D33" s="74"/>
+      <c r="E33" s="74"/>
+      <c r="F33" s="74"/>
+      <c r="G33" s="74"/>
+      <c r="H33" s="75"/>
+      <c r="I33" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="J33" s="50"/>
+      <c r="J33" s="57"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
     </row>
@@ -3525,82 +3586,82 @@
         <v>15</v>
       </c>
       <c r="C34" s="5"/>
-      <c r="D34" s="48" t="s">
+      <c r="D34" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="48"/>
-      <c r="F34" s="48"/>
-      <c r="G34" s="48"/>
-      <c r="H34" s="49"/>
-      <c r="I34" s="46"/>
-      <c r="J34" s="70"/>
-      <c r="K34" s="70"/>
-      <c r="L34" s="70"/>
+      <c r="E34" s="55"/>
+      <c r="F34" s="55"/>
+      <c r="G34" s="55"/>
+      <c r="H34" s="56"/>
+      <c r="I34" s="53"/>
+      <c r="J34" s="77"/>
+      <c r="K34" s="77"/>
+      <c r="L34" s="77"/>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B35" s="54">
+      <c r="B35" s="61">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C35" s="57"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="63" t="s">
+      <c r="C35" s="64"/>
+      <c r="D35" s="65"/>
+      <c r="E35" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="F35" s="63"/>
-      <c r="G35" s="63"/>
-      <c r="H35" s="64"/>
-      <c r="I35" s="69" t="s">
+      <c r="F35" s="70"/>
+      <c r="G35" s="70"/>
+      <c r="H35" s="71"/>
+      <c r="I35" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="J35" s="50"/>
+      <c r="J35" s="57"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B36" s="55"/>
-      <c r="C36" s="59"/>
-      <c r="D36" s="60"/>
-      <c r="E36" s="65"/>
-      <c r="F36" s="65"/>
-      <c r="G36" s="65"/>
-      <c r="H36" s="66"/>
-      <c r="I36" s="69" t="s">
+      <c r="B36" s="62"/>
+      <c r="C36" s="66"/>
+      <c r="D36" s="67"/>
+      <c r="E36" s="72"/>
+      <c r="F36" s="72"/>
+      <c r="G36" s="72"/>
+      <c r="H36" s="73"/>
+      <c r="I36" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="J36" s="50"/>
+      <c r="J36" s="57"/>
       <c r="K36" s="20"/>
       <c r="L36" s="21" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B37" s="55"/>
-      <c r="C37" s="59"/>
-      <c r="D37" s="60"/>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
-      <c r="G37" s="65"/>
-      <c r="H37" s="66"/>
-      <c r="I37" s="69" t="s">
+      <c r="B37" s="62"/>
+      <c r="C37" s="66"/>
+      <c r="D37" s="67"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="72"/>
+      <c r="G37" s="72"/>
+      <c r="H37" s="73"/>
+      <c r="I37" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="J37" s="50"/>
+      <c r="J37" s="57"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B38" s="56"/>
-      <c r="C38" s="61"/>
-      <c r="D38" s="62"/>
-      <c r="E38" s="67"/>
-      <c r="F38" s="67"/>
-      <c r="G38" s="67"/>
-      <c r="H38" s="68"/>
-      <c r="I38" s="69" t="s">
+      <c r="B38" s="63"/>
+      <c r="C38" s="68"/>
+      <c r="D38" s="69"/>
+      <c r="E38" s="74"/>
+      <c r="F38" s="74"/>
+      <c r="G38" s="74"/>
+      <c r="H38" s="75"/>
+      <c r="I38" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="J38" s="50"/>
+      <c r="J38" s="57"/>
       <c r="K38" s="20"/>
       <c r="L38" s="21" t="s">
         <v>29</v>
@@ -3614,160 +3675,160 @@
       <c r="C39" s="5"/>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
-      <c r="F39" s="48" t="s">
+      <c r="F39" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="G39" s="48"/>
-      <c r="H39" s="49"/>
-      <c r="I39" s="69" t="s">
+      <c r="G39" s="55"/>
+      <c r="H39" s="56"/>
+      <c r="I39" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="J39" s="50"/>
+      <c r="J39" s="57"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B40" s="54">
+      <c r="B40" s="61">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C40" s="57"/>
-      <c r="D40" s="58"/>
-      <c r="E40" s="63" t="s">
+      <c r="C40" s="64"/>
+      <c r="D40" s="65"/>
+      <c r="E40" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="F40" s="63"/>
-      <c r="G40" s="63"/>
-      <c r="H40" s="64"/>
-      <c r="I40" s="69" t="s">
+      <c r="F40" s="70"/>
+      <c r="G40" s="70"/>
+      <c r="H40" s="71"/>
+      <c r="I40" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="J40" s="50"/>
+      <c r="J40" s="57"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B41" s="55"/>
-      <c r="C41" s="59"/>
-      <c r="D41" s="60"/>
-      <c r="E41" s="65"/>
-      <c r="F41" s="65"/>
-      <c r="G41" s="65"/>
-      <c r="H41" s="66"/>
-      <c r="I41" s="69" t="s">
+      <c r="B41" s="62"/>
+      <c r="C41" s="66"/>
+      <c r="D41" s="67"/>
+      <c r="E41" s="72"/>
+      <c r="F41" s="72"/>
+      <c r="G41" s="72"/>
+      <c r="H41" s="73"/>
+      <c r="I41" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="J41" s="50"/>
+      <c r="J41" s="57"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B42" s="55"/>
-      <c r="C42" s="59"/>
-      <c r="D42" s="60"/>
-      <c r="E42" s="65"/>
-      <c r="F42" s="65"/>
-      <c r="G42" s="65"/>
-      <c r="H42" s="66"/>
-      <c r="I42" s="69" t="s">
+      <c r="B42" s="62"/>
+      <c r="C42" s="66"/>
+      <c r="D42" s="67"/>
+      <c r="E42" s="72"/>
+      <c r="F42" s="72"/>
+      <c r="G42" s="72"/>
+      <c r="H42" s="73"/>
+      <c r="I42" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="J42" s="50"/>
+      <c r="J42" s="57"/>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B43" s="55"/>
-      <c r="C43" s="59"/>
-      <c r="D43" s="60"/>
-      <c r="E43" s="65"/>
-      <c r="F43" s="65"/>
-      <c r="G43" s="65"/>
-      <c r="H43" s="66"/>
-      <c r="I43" s="69" t="s">
+      <c r="B43" s="62"/>
+      <c r="C43" s="66"/>
+      <c r="D43" s="67"/>
+      <c r="E43" s="72"/>
+      <c r="F43" s="72"/>
+      <c r="G43" s="72"/>
+      <c r="H43" s="73"/>
+      <c r="I43" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="J43" s="50"/>
+      <c r="J43" s="57"/>
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B44" s="56"/>
-      <c r="C44" s="59"/>
-      <c r="D44" s="60"/>
-      <c r="E44" s="65"/>
-      <c r="F44" s="65"/>
-      <c r="G44" s="65"/>
-      <c r="H44" s="66"/>
-      <c r="I44" s="69" t="s">
+      <c r="B44" s="63"/>
+      <c r="C44" s="66"/>
+      <c r="D44" s="67"/>
+      <c r="E44" s="72"/>
+      <c r="F44" s="72"/>
+      <c r="G44" s="72"/>
+      <c r="H44" s="73"/>
+      <c r="I44" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="J44" s="50"/>
+      <c r="J44" s="57"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B45" s="54">
+      <c r="B45" s="61">
         <f>B40+1</f>
         <v>19</v>
       </c>
-      <c r="C45" s="57"/>
-      <c r="D45" s="58"/>
-      <c r="E45" s="58"/>
-      <c r="F45" s="63" t="s">
+      <c r="C45" s="64"/>
+      <c r="D45" s="65"/>
+      <c r="E45" s="65"/>
+      <c r="F45" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="G45" s="63"/>
-      <c r="H45" s="64"/>
-      <c r="I45" s="50" t="s">
+      <c r="G45" s="70"/>
+      <c r="H45" s="71"/>
+      <c r="I45" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="J45" s="51"/>
+      <c r="J45" s="58"/>
       <c r="K45" s="4"/>
       <c r="L45" s="4"/>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B46" s="55"/>
-      <c r="C46" s="59"/>
-      <c r="D46" s="60"/>
-      <c r="E46" s="60"/>
-      <c r="F46" s="65"/>
-      <c r="G46" s="65"/>
-      <c r="H46" s="66"/>
-      <c r="I46" s="69" t="s">
+      <c r="B46" s="62"/>
+      <c r="C46" s="66"/>
+      <c r="D46" s="67"/>
+      <c r="E46" s="67"/>
+      <c r="F46" s="72"/>
+      <c r="G46" s="72"/>
+      <c r="H46" s="73"/>
+      <c r="I46" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="J46" s="50"/>
+      <c r="J46" s="57"/>
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B47" s="55"/>
-      <c r="C47" s="59"/>
-      <c r="D47" s="60"/>
-      <c r="E47" s="60"/>
-      <c r="F47" s="65"/>
-      <c r="G47" s="65"/>
-      <c r="H47" s="66"/>
-      <c r="I47" s="69" t="s">
+      <c r="B47" s="62"/>
+      <c r="C47" s="66"/>
+      <c r="D47" s="67"/>
+      <c r="E47" s="67"/>
+      <c r="F47" s="72"/>
+      <c r="G47" s="72"/>
+      <c r="H47" s="73"/>
+      <c r="I47" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="J47" s="50"/>
+      <c r="J47" s="57"/>
       <c r="K47" s="4"/>
       <c r="L47" s="4"/>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B48" s="56"/>
-      <c r="C48" s="61"/>
-      <c r="D48" s="62"/>
-      <c r="E48" s="62"/>
-      <c r="F48" s="67"/>
-      <c r="G48" s="67"/>
-      <c r="H48" s="68"/>
-      <c r="I48" s="69" t="s">
+      <c r="B48" s="63"/>
+      <c r="C48" s="68"/>
+      <c r="D48" s="69"/>
+      <c r="E48" s="69"/>
+      <c r="F48" s="74"/>
+      <c r="G48" s="74"/>
+      <c r="H48" s="75"/>
+      <c r="I48" s="76" t="s">
         <v>58</v>
       </c>
-      <c r="J48" s="50"/>
+      <c r="J48" s="57"/>
       <c r="K48" s="10"/>
       <c r="L48" s="4" t="s">
         <v>59</v>
@@ -3782,14 +3843,14 @@
       <c r="D49" s="9"/>
       <c r="E49" s="9"/>
       <c r="F49" s="9"/>
-      <c r="G49" s="48" t="s">
+      <c r="G49" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="H49" s="49"/>
-      <c r="I49" s="50" t="s">
+      <c r="H49" s="56"/>
+      <c r="I49" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="J49" s="51"/>
+      <c r="J49" s="58"/>
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
     </row>
@@ -3798,16 +3859,16 @@
         <f t="shared" ref="B50:B60" si="1">B49+1</f>
         <v>21</v>
       </c>
-      <c r="C50" s="52"/>
-      <c r="D50" s="53"/>
-      <c r="E50" s="53"/>
-      <c r="F50" s="53"/>
-      <c r="G50" s="48" t="s">
+      <c r="C50" s="59"/>
+      <c r="D50" s="60"/>
+      <c r="E50" s="60"/>
+      <c r="F50" s="60"/>
+      <c r="G50" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="H50" s="49"/>
-      <c r="I50" s="46"/>
-      <c r="J50" s="47"/>
+      <c r="H50" s="56"/>
+      <c r="I50" s="53"/>
+      <c r="J50" s="54"/>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
     </row>
@@ -3822,8 +3883,8 @@
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
       <c r="H51" s="6"/>
-      <c r="I51" s="46"/>
-      <c r="J51" s="47"/>
+      <c r="I51" s="53"/>
+      <c r="J51" s="54"/>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
     </row>
@@ -3838,8 +3899,8 @@
       <c r="F52" s="9"/>
       <c r="G52" s="9"/>
       <c r="H52" s="6"/>
-      <c r="I52" s="46"/>
-      <c r="J52" s="47"/>
+      <c r="I52" s="53"/>
+      <c r="J52" s="54"/>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
     </row>
@@ -3854,8 +3915,8 @@
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
       <c r="H53" s="6"/>
-      <c r="I53" s="46"/>
-      <c r="J53" s="47"/>
+      <c r="I53" s="53"/>
+      <c r="J53" s="54"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
     </row>
@@ -3870,8 +3931,8 @@
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
       <c r="H54" s="6"/>
-      <c r="I54" s="46"/>
-      <c r="J54" s="47"/>
+      <c r="I54" s="53"/>
+      <c r="J54" s="54"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
     </row>
@@ -3886,8 +3947,8 @@
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
       <c r="H55" s="6"/>
-      <c r="I55" s="46"/>
-      <c r="J55" s="47"/>
+      <c r="I55" s="53"/>
+      <c r="J55" s="54"/>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
     </row>
@@ -3902,8 +3963,8 @@
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
       <c r="H56" s="6"/>
-      <c r="I56" s="46"/>
-      <c r="J56" s="47"/>
+      <c r="I56" s="53"/>
+      <c r="J56" s="54"/>
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
     </row>
@@ -3918,8 +3979,8 @@
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
       <c r="H57" s="6"/>
-      <c r="I57" s="46"/>
-      <c r="J57" s="47"/>
+      <c r="I57" s="53"/>
+      <c r="J57" s="54"/>
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
     </row>
@@ -3934,8 +3995,8 @@
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
       <c r="H58" s="6"/>
-      <c r="I58" s="46"/>
-      <c r="J58" s="47"/>
+      <c r="I58" s="53"/>
+      <c r="J58" s="54"/>
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
     </row>
@@ -3950,8 +4011,8 @@
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
       <c r="H59" s="6"/>
-      <c r="I59" s="46"/>
-      <c r="J59" s="47"/>
+      <c r="I59" s="53"/>
+      <c r="J59" s="54"/>
       <c r="K59" s="4"/>
       <c r="L59" s="4"/>
     </row>
@@ -3966,8 +4027,8 @@
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
       <c r="H60" s="6"/>
-      <c r="I60" s="46"/>
-      <c r="J60" s="47"/>
+      <c r="I60" s="53"/>
+      <c r="J60" s="54"/>
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
     </row>

</xml_diff>

<commit_message>
#27 Create default account
</commit_message>
<xml_diff>
--- a/documents/Testing Schedule.xlsx
+++ b/documents/Testing Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Node\Timelog\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A09B90-B402-40B0-9949-651E631E2DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695DA108-C727-4D69-9730-FD8F3FC7A00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{9AAAF6DA-95E7-49F0-B7DD-46373E33B9E7}"/>
   </bookViews>
@@ -1417,7 +1417,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M31" sqref="M31"/>
+      <selection pane="bottomLeft" activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Version 1.1.4.0 - Cleaned up default test account code used for debugging
</commit_message>
<xml_diff>
--- a/documents/Testing Schedule.xlsx
+++ b/documents/Testing Schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Node\Timelog\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Node\Timelog\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CE1356-90C2-4837-8BF1-2F5971AC94B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312FB08C-68A6-4704-B9F0-C55C905888D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{9AAAF6DA-95E7-49F0-B7DD-46373E33B9E7}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="133">
   <si>
     <t>RMPC Timelog Testing Schedule</t>
   </si>
@@ -397,9 +397,6 @@
     <t>Home page</t>
   </si>
   <si>
-    <t>No error message transition</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -415,39 +412,12 @@
     <t>Issue #</t>
   </si>
   <si>
-    <t>#1</t>
-  </si>
-  <si>
-    <t>#2</t>
-  </si>
-  <si>
-    <t>#3</t>
-  </si>
-  <si>
     <t>Create</t>
   </si>
   <si>
-    <t>Script error</t>
-  </si>
-  <si>
-    <t>#5</t>
-  </si>
-  <si>
-    <t>#6</t>
-  </si>
-  <si>
     <t>Unique</t>
   </si>
   <si>
-    <t>#12</t>
-  </si>
-  <si>
-    <t>User is returned to the sign up page</t>
-  </si>
-  <si>
-    <t>User name used as company name</t>
-  </si>
-  <si>
     <t>Database table entries</t>
   </si>
   <si>
@@ -466,21 +436,12 @@
     <t>projects (limit of 1)</t>
   </si>
   <si>
-    <t>#17</t>
-  </si>
-  <si>
     <t>Menu Item: Logging</t>
   </si>
   <si>
     <t>User is taken to the "Logging" page</t>
   </si>
   <si>
-    <t>Showstopper</t>
-  </si>
-  <si>
-    <t>Related to #7 above</t>
-  </si>
-  <si>
     <t>Required - only if both missing (otherwise match error)</t>
   </si>
   <si>
@@ -490,12 +451,6 @@
     <t>Displays correctly</t>
   </si>
   <si>
-    <t>Client label shows</t>
-  </si>
-  <si>
-    <t>#31</t>
-  </si>
-  <si>
     <t>Details</t>
   </si>
   <si>
@@ -506,6 +461,15 @@
   </si>
   <si>
     <t>Action</t>
+  </si>
+  <si>
+    <t>Reinstate and test</t>
+  </si>
+  <si>
+    <t>Funky behaviour - error message shows</t>
+  </si>
+  <si>
+    <t>#135</t>
   </si>
 </sst>
 </file>
@@ -801,7 +765,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -875,7 +839,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -931,254 +895,218 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1499,11 +1427,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDA5C5C7-8B67-4FAF-9315-0E07B94A4E72}">
-  <dimension ref="B2:R88"/>
+  <dimension ref="B2:Q88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I19" sqref="I19"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1511,55 +1439,54 @@
     <col min="1" max="1" width="5.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="5.7109375" style="3" customWidth="1"/>
     <col min="3" max="7" width="10.7109375" style="2" customWidth="1"/>
-    <col min="8" max="9" width="35.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="35.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" style="2" customWidth="1"/>
     <col min="10" max="10" width="62.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="67" customWidth="1"/>
-    <col min="12" max="13" width="9.7109375" style="67" customWidth="1"/>
-    <col min="14" max="14" width="49.140625" style="72" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="49.140625" style="61" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="57" customWidth="1"/>
+    <col min="12" max="13" width="9.7109375" style="57" customWidth="1"/>
+    <col min="14" max="15" width="49.140625" style="53" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="89" t="s">
-        <v>112</v>
-      </c>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="Q2" s="64"/>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="86" t="s">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B2" s="82" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="69"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="Q2" s="55"/>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B3" s="79" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="59"/>
       <c r="H3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="O3" s="67"/>
-      <c r="P3" s="61"/>
-      <c r="R3" s="65"/>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="79" t="s">
-        <v>110</v>
-      </c>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="53"/>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B4" s="93" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="93"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="Q4" s="66"/>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="Q4" s="56"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
         <v>30</v>
       </c>
@@ -1572,7 +1499,7 @@
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
       <c r="I6" s="16" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="J6" s="16" t="s">
         <v>79</v>
@@ -1580,63 +1507,63 @@
       <c r="K6" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="L6" s="82" t="s">
-        <v>113</v>
-      </c>
-      <c r="M6" s="83"/>
+      <c r="L6" s="95" t="s">
+        <v>112</v>
+      </c>
+      <c r="M6" s="96"/>
       <c r="N6" s="17" t="s">
         <v>104</v>
       </c>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="11">
         <v>1</v>
       </c>
-      <c r="C7" s="90" t="s">
+      <c r="C7" s="83" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="91"/>
-      <c r="E7" s="91"/>
-      <c r="F7" s="91"/>
-      <c r="G7" s="91"/>
-      <c r="H7" s="91"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="73"/>
       <c r="I7" s="4"/>
-      <c r="J7" s="114"/>
-      <c r="K7" s="115"/>
-      <c r="L7" s="115"/>
-      <c r="M7" s="115"/>
-      <c r="N7" s="119"/>
+      <c r="J7" s="97"/>
+      <c r="K7" s="98"/>
+      <c r="L7" s="98"/>
+      <c r="M7" s="98"/>
+      <c r="N7" s="99"/>
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="11">
         <f>B7+1</f>
         <v>2</v>
       </c>
       <c r="C8" s="41"/>
-      <c r="D8" s="91" t="s">
+      <c r="D8" s="73" t="s">
         <v>103</v>
       </c>
-      <c r="E8" s="91"/>
-      <c r="F8" s="91"/>
-      <c r="G8" s="91"/>
-      <c r="H8" s="91"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="73"/>
       <c r="I8" s="4" t="s">
         <v>105</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="K8" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="K8" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="L8" s="60"/>
-      <c r="M8" s="60"/>
-      <c r="N8" s="71"/>
+      <c r="L8" s="52"/>
+      <c r="M8" s="52"/>
+      <c r="N8" s="47"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="11">
         <f t="shared" ref="B9:B83" si="0">B8+1</f>
         <v>3</v>
@@ -1650,14 +1577,14 @@
       <c r="G9" s="42"/>
       <c r="H9" s="42"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="114"/>
-      <c r="K9" s="115"/>
-      <c r="L9" s="115"/>
-      <c r="M9" s="115"/>
-      <c r="N9" s="119"/>
+      <c r="J9" s="97"/>
+      <c r="K9" s="98"/>
+      <c r="L9" s="98"/>
+      <c r="M9" s="98"/>
+      <c r="N9" s="99"/>
       <c r="O9" s="2"/>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" s="11">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1671,22 +1598,18 @@
       <c r="G10" s="42"/>
       <c r="H10" s="42"/>
       <c r="I10" s="4"/>
-      <c r="J10" s="50" t="s">
+      <c r="J10" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="K10" s="60" t="s">
+      <c r="K10" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="L10" s="80" t="s">
-        <v>116</v>
-      </c>
-      <c r="M10" s="70"/>
-      <c r="N10" s="81" t="s">
-        <v>108</v>
-      </c>
+      <c r="L10" s="94"/>
+      <c r="M10" s="60"/>
+      <c r="N10" s="115"/>
       <c r="O10" s="2"/>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" s="11">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1700,18 +1623,18 @@
       <c r="G11" s="42"/>
       <c r="H11" s="42"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="54" t="s">
+      <c r="J11" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="K11" s="63" t="s">
+      <c r="K11" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="L11" s="80"/>
-      <c r="M11" s="70"/>
-      <c r="N11" s="81"/>
+      <c r="L11" s="94"/>
+      <c r="M11" s="60"/>
+      <c r="N11" s="115"/>
       <c r="O11" s="2"/>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="11">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1725,18 +1648,18 @@
       <c r="G12" s="42"/>
       <c r="H12" s="42"/>
       <c r="I12" s="4"/>
-      <c r="J12" s="123" t="s">
-        <v>136</v>
-      </c>
-      <c r="K12" s="125" t="s">
+      <c r="J12" s="91" t="s">
+        <v>123</v>
+      </c>
+      <c r="K12" s="88" t="s">
         <v>70</v>
       </c>
-      <c r="L12" s="80"/>
-      <c r="M12" s="70"/>
-      <c r="N12" s="81"/>
+      <c r="L12" s="94"/>
+      <c r="M12" s="60"/>
+      <c r="N12" s="115"/>
       <c r="O12" s="2"/>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="11">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1750,66 +1673,64 @@
       <c r="G13" s="44"/>
       <c r="H13" s="44"/>
       <c r="I13" s="4"/>
-      <c r="J13" s="120"/>
-      <c r="K13" s="122"/>
-      <c r="L13" s="80"/>
-      <c r="M13" s="70"/>
-      <c r="N13" s="81"/>
+      <c r="J13" s="92"/>
+      <c r="K13" s="89"/>
+      <c r="L13" s="94"/>
+      <c r="M13" s="60"/>
+      <c r="N13" s="115"/>
       <c r="O13" s="2"/>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" s="22">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="C14" s="43"/>
       <c r="D14" s="44"/>
-      <c r="E14" s="84" t="s">
+      <c r="E14" s="69" t="s">
         <v>99</v>
       </c>
       <c r="F14" s="44"/>
       <c r="G14" s="44"/>
-      <c r="H14" s="55"/>
+      <c r="H14" s="44"/>
       <c r="I14" s="4"/>
-      <c r="J14" s="47" t="s">
+      <c r="J14" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="K14" s="60" t="s">
+      <c r="K14" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="L14" s="60" t="s">
-        <v>115</v>
-      </c>
-      <c r="M14" s="60" t="s">
-        <v>116</v>
-      </c>
-      <c r="N14" s="81"/>
+      <c r="L14" s="52"/>
+      <c r="M14" s="52"/>
+      <c r="N14" s="115"/>
       <c r="O14" s="2"/>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" s="22">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C15" s="45"/>
       <c r="D15" s="46"/>
-      <c r="E15" s="85"/>
+      <c r="E15" s="70"/>
       <c r="F15" s="46"/>
       <c r="G15" s="46"/>
-      <c r="H15" s="56"/>
+      <c r="H15" s="46"/>
       <c r="I15" s="4"/>
-      <c r="J15" s="47" t="s">
-        <v>121</v>
-      </c>
-      <c r="K15" s="59" t="s">
-        <v>109</v>
-      </c>
-      <c r="L15" s="60"/>
-      <c r="M15" s="70"/>
-      <c r="N15" s="81"/>
+      <c r="J15" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="K15" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="L15" s="52"/>
+      <c r="M15" s="60"/>
+      <c r="N15" s="115" t="s">
+        <v>130</v>
+      </c>
       <c r="O15" s="2"/>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1823,17 +1744,15 @@
       <c r="G16" s="46"/>
       <c r="H16" s="46"/>
       <c r="I16" s="4"/>
-      <c r="J16" s="50" t="s">
+      <c r="J16" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="K16" s="60" t="s">
+      <c r="K16" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="L16" s="60" t="s">
-        <v>116</v>
-      </c>
-      <c r="M16" s="70"/>
-      <c r="N16" s="81"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="60"/>
+      <c r="N16" s="115"/>
       <c r="O16" s="2"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
@@ -1851,16 +1770,14 @@
       <c r="H17" s="42"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="K17" s="60" t="s">
+        <v>124</v>
+      </c>
+      <c r="K17" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="L17" s="60" t="s">
-        <v>114</v>
-      </c>
-      <c r="M17" s="60"/>
-      <c r="N17" s="71"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="52"/>
+      <c r="N17" s="47"/>
       <c r="O17" s="2"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
@@ -1877,11 +1794,17 @@
       <c r="G18" s="42"/>
       <c r="H18" s="42"/>
       <c r="I18" s="4"/>
-      <c r="J18" s="114"/>
-      <c r="K18" s="115"/>
-      <c r="L18" s="115"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="116" t="s">
+        <v>70</v>
+      </c>
+      <c r="L18" s="117" t="s">
+        <v>132</v>
+      </c>
       <c r="M18" s="115"/>
-      <c r="N18" s="119"/>
+      <c r="N18" s="115" t="s">
+        <v>131</v>
+      </c>
       <c r="O18" s="2"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
@@ -1901,18 +1824,10 @@
       <c r="J19" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="K19" s="60" t="s">
-        <v>70</v>
-      </c>
-      <c r="L19" s="60" t="s">
-        <v>119</v>
-      </c>
-      <c r="M19" s="60" t="s">
-        <v>120</v>
-      </c>
-      <c r="N19" s="71" t="s">
-        <v>118</v>
-      </c>
+      <c r="K19" s="52"/>
+      <c r="L19" s="52"/>
+      <c r="M19" s="52"/>
+      <c r="N19" s="47"/>
       <c r="O19" s="2"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
@@ -1923,17 +1838,17 @@
       <c r="C20" s="41"/>
       <c r="D20" s="42"/>
       <c r="E20" s="42" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="F20" s="42"/>
       <c r="G20" s="42"/>
       <c r="H20" s="42"/>
       <c r="I20" s="4"/>
-      <c r="J20" s="114"/>
-      <c r="K20" s="115"/>
-      <c r="L20" s="115"/>
-      <c r="M20" s="115"/>
-      <c r="N20" s="119"/>
+      <c r="J20" s="97"/>
+      <c r="K20" s="98"/>
+      <c r="L20" s="98"/>
+      <c r="M20" s="98"/>
+      <c r="N20" s="99"/>
       <c r="O20" s="2"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
@@ -1945,22 +1860,18 @@
       <c r="D21" s="42"/>
       <c r="E21" s="42"/>
       <c r="F21" s="42" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="G21" s="42"/>
       <c r="H21" s="42"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="K21" s="60" t="s">
-        <v>70</v>
-      </c>
-      <c r="L21" s="68"/>
-      <c r="M21" s="68"/>
-      <c r="N21" s="71" t="s">
-        <v>124</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="K21" s="52"/>
+      <c r="L21" s="58"/>
+      <c r="M21" s="58"/>
+      <c r="N21" s="47"/>
       <c r="O21" s="2"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
@@ -1972,22 +1883,16 @@
       <c r="D22" s="42"/>
       <c r="E22" s="42"/>
       <c r="F22" s="42" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="G22" s="42"/>
       <c r="H22" s="42"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
-      <c r="K22" s="63" t="s">
-        <v>70</v>
-      </c>
-      <c r="L22" s="121" t="s">
-        <v>131</v>
-      </c>
-      <c r="M22" s="68"/>
-      <c r="N22" s="126" t="s">
-        <v>134</v>
-      </c>
+      <c r="K22" s="52"/>
+      <c r="L22" s="87"/>
+      <c r="M22" s="58"/>
+      <c r="N22" s="90"/>
       <c r="O22" s="2"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
@@ -1999,18 +1904,16 @@
       <c r="D23" s="42"/>
       <c r="E23" s="42"/>
       <c r="F23" s="42" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="G23" s="42"/>
       <c r="H23" s="42"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
-      <c r="K23" s="63" t="s">
-        <v>70</v>
-      </c>
-      <c r="L23" s="125"/>
-      <c r="M23" s="68"/>
-      <c r="N23" s="127"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="88"/>
+      <c r="M23" s="58"/>
+      <c r="N23" s="91"/>
       <c r="O23" s="2"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
@@ -2022,18 +1925,16 @@
       <c r="D24" s="42"/>
       <c r="E24" s="42"/>
       <c r="F24" s="42" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="G24" s="42"/>
       <c r="H24" s="42"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
-      <c r="K24" s="63" t="s">
-        <v>70</v>
-      </c>
-      <c r="L24" s="125"/>
-      <c r="M24" s="68"/>
-      <c r="N24" s="127"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="88"/>
+      <c r="M24" s="58"/>
+      <c r="N24" s="91"/>
       <c r="O24" s="2"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
@@ -2045,120 +1946,110 @@
       <c r="D25" s="42"/>
       <c r="E25" s="42"/>
       <c r="F25" s="42" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="G25" s="42"/>
       <c r="H25" s="42"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
-      <c r="K25" s="63" t="s">
-        <v>70</v>
-      </c>
-      <c r="L25" s="122"/>
-      <c r="M25" s="68"/>
-      <c r="N25" s="128"/>
+      <c r="K25" s="52"/>
+      <c r="L25" s="89"/>
+      <c r="M25" s="58"/>
+      <c r="N25" s="92"/>
       <c r="O25" s="2"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" s="11"/>
-      <c r="C26" s="58"/>
-      <c r="D26" s="53" t="s">
+      <c r="C26" s="41"/>
+      <c r="D26" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="E26" s="53"/>
-      <c r="F26" s="53"/>
-      <c r="G26" s="53"/>
-      <c r="H26" s="53"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="K26" s="63" t="s">
-        <v>70</v>
-      </c>
-      <c r="L26" s="124"/>
-      <c r="M26" s="68"/>
-      <c r="N26" s="129"/>
+        <v>125</v>
+      </c>
+      <c r="K26" s="52"/>
+      <c r="L26" s="66"/>
+      <c r="M26" s="58"/>
+      <c r="N26" s="65"/>
       <c r="O26" s="2"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" s="11"/>
-      <c r="C27" s="58"/>
-      <c r="D27" s="53" t="s">
+      <c r="C27" s="41"/>
+      <c r="D27" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="E27" s="53"/>
-      <c r="F27" s="53"/>
-      <c r="G27" s="53"/>
-      <c r="H27" s="53"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="K27" s="59" t="s">
-        <v>109</v>
-      </c>
-      <c r="L27" s="59" t="s">
-        <v>140</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="K27" s="51"/>
+      <c r="L27" s="51"/>
       <c r="M27" s="4"/>
-      <c r="N27" s="4" t="s">
-        <v>139</v>
-      </c>
+      <c r="N27" s="4"/>
       <c r="O27" s="2"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B28" s="11"/>
-      <c r="C28" s="58"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="53" t="s">
-        <v>142</v>
-      </c>
-      <c r="F28" s="53"/>
-      <c r="G28" s="53"/>
-      <c r="H28" s="53"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42" t="s">
+        <v>127</v>
+      </c>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
       <c r="I28" s="4"/>
-      <c r="J28" s="51" t="s">
-        <v>143</v>
-      </c>
-      <c r="K28" s="57"/>
-      <c r="L28" s="57"/>
-      <c r="M28" s="57"/>
-      <c r="N28" s="52"/>
+      <c r="J28" s="48" t="s">
+        <v>128</v>
+      </c>
+      <c r="K28" s="50"/>
+      <c r="L28" s="50"/>
+      <c r="M28" s="50"/>
+      <c r="N28" s="49"/>
       <c r="O28" s="2"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B29" s="11"/>
-      <c r="C29" s="58"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="53" t="s">
-        <v>141</v>
-      </c>
-      <c r="G29" s="53"/>
-      <c r="H29" s="53"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="G29" s="42"/>
+      <c r="H29" s="42"/>
       <c r="I29" s="4"/>
-      <c r="J29" s="51"/>
-      <c r="K29" s="57"/>
-      <c r="L29" s="57"/>
-      <c r="M29" s="57"/>
-      <c r="N29" s="52"/>
+      <c r="J29" s="48"/>
+      <c r="K29" s="50"/>
+      <c r="L29" s="50"/>
+      <c r="M29" s="50"/>
+      <c r="N29" s="49"/>
       <c r="O29" s="2"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B30" s="11"/>
-      <c r="C30" s="58"/>
-      <c r="D30" s="53"/>
-      <c r="E30" s="53"/>
-      <c r="F30" s="53"/>
-      <c r="G30" s="53"/>
-      <c r="H30" s="53"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="42"/>
       <c r="I30" s="4"/>
-      <c r="J30" s="51"/>
-      <c r="K30" s="57"/>
-      <c r="L30" s="57"/>
-      <c r="M30" s="57"/>
-      <c r="N30" s="52"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="50"/>
+      <c r="L30" s="50"/>
+      <c r="M30" s="50"/>
+      <c r="N30" s="49"/>
       <c r="O30" s="2"/>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
@@ -2176,10 +2067,10 @@
       <c r="H31" s="9"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
-      <c r="K31" s="68"/>
-      <c r="L31" s="68"/>
-      <c r="M31" s="68"/>
-      <c r="N31" s="71"/>
+      <c r="K31" s="58"/>
+      <c r="L31" s="58"/>
+      <c r="M31" s="58"/>
+      <c r="N31" s="47"/>
       <c r="O31" s="2"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
@@ -2188,27 +2079,21 @@
         <v>21</v>
       </c>
       <c r="C32" s="5"/>
-      <c r="D32" s="91" t="s">
+      <c r="D32" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="E32" s="91"/>
-      <c r="F32" s="91"/>
-      <c r="G32" s="91"/>
-      <c r="H32" s="91"/>
+      <c r="E32" s="73"/>
+      <c r="F32" s="73"/>
+      <c r="G32" s="73"/>
+      <c r="H32" s="73"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="K32" s="60" t="s">
-        <v>70</v>
-      </c>
-      <c r="L32" s="60" t="s">
-        <v>122</v>
-      </c>
-      <c r="M32" s="68"/>
-      <c r="N32" s="71" t="s">
-        <v>123</v>
-      </c>
+      <c r="K32" s="52"/>
+      <c r="L32" s="52"/>
+      <c r="M32" s="58"/>
+      <c r="N32" s="47"/>
       <c r="O32" s="2"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
@@ -2228,12 +2113,10 @@
       <c r="J33" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K33" s="60" t="s">
-        <v>70</v>
-      </c>
-      <c r="L33" s="68"/>
-      <c r="M33" s="68"/>
-      <c r="N33" s="71"/>
+      <c r="K33" s="52"/>
+      <c r="L33" s="58"/>
+      <c r="M33" s="58"/>
+      <c r="N33" s="47"/>
       <c r="O33" s="2"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
@@ -2241,26 +2124,22 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="C34" s="73"/>
-      <c r="D34" s="74" t="s">
-        <v>132</v>
-      </c>
-      <c r="E34" s="74"/>
-      <c r="F34" s="74"/>
-      <c r="G34" s="74"/>
-      <c r="H34" s="74"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="62" t="s">
+        <v>121</v>
+      </c>
+      <c r="E34" s="62"/>
+      <c r="F34" s="62"/>
+      <c r="G34" s="62"/>
+      <c r="H34" s="62"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="K34" s="59" t="s">
-        <v>109</v>
-      </c>
-      <c r="L34" s="68"/>
-      <c r="M34" s="68"/>
-      <c r="N34" s="71" t="s">
-        <v>135</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="K34" s="51"/>
+      <c r="L34" s="58"/>
+      <c r="M34" s="58"/>
+      <c r="N34" s="47"/>
       <c r="O34" s="2"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
@@ -2268,22 +2147,22 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="C35" s="73"/>
-      <c r="D35" s="77" t="s">
+      <c r="C35" s="61"/>
+      <c r="D35" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="E35" s="74"/>
-      <c r="F35" s="74"/>
-      <c r="G35" s="74"/>
-      <c r="H35" s="74"/>
+      <c r="E35" s="62"/>
+      <c r="F35" s="62"/>
+      <c r="G35" s="62"/>
+      <c r="H35" s="62"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="K35" s="68"/>
-      <c r="L35" s="68"/>
-      <c r="M35" s="68"/>
-      <c r="N35" s="71"/>
+      <c r="K35" s="58"/>
+      <c r="L35" s="58"/>
+      <c r="M35" s="58"/>
+      <c r="N35" s="47"/>
       <c r="O35" s="2"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
@@ -2291,20 +2170,20 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="C36" s="75"/>
-      <c r="D36" s="78"/>
-      <c r="E36" s="76"/>
-      <c r="F36" s="76"/>
-      <c r="G36" s="76"/>
-      <c r="H36" s="76"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="77"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="64"/>
+      <c r="G36" s="64"/>
+      <c r="H36" s="64"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K36" s="68"/>
-      <c r="L36" s="68"/>
-      <c r="M36" s="68"/>
-      <c r="N36" s="71"/>
+      <c r="K36" s="58"/>
+      <c r="L36" s="58"/>
+      <c r="M36" s="58"/>
+      <c r="N36" s="47"/>
       <c r="O36" s="2"/>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
@@ -2312,22 +2191,22 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="C37" s="94"/>
-      <c r="D37" s="84" t="s">
+      <c r="C37" s="67"/>
+      <c r="D37" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="E37" s="84"/>
-      <c r="F37" s="84"/>
-      <c r="G37" s="84"/>
-      <c r="H37" s="84"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="69"/>
+      <c r="G37" s="69"/>
+      <c r="H37" s="69"/>
       <c r="I37" s="4"/>
       <c r="J37" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K37" s="68"/>
-      <c r="L37" s="68"/>
-      <c r="M37" s="68"/>
-      <c r="N37" s="71"/>
+      <c r="K37" s="58"/>
+      <c r="L37" s="58"/>
+      <c r="M37" s="58"/>
+      <c r="N37" s="47"/>
       <c r="O37" s="2"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
@@ -2335,20 +2214,20 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="C38" s="97"/>
-      <c r="D38" s="85"/>
-      <c r="E38" s="85"/>
-      <c r="F38" s="85"/>
-      <c r="G38" s="85"/>
-      <c r="H38" s="85"/>
+      <c r="C38" s="68"/>
+      <c r="D38" s="70"/>
+      <c r="E38" s="70"/>
+      <c r="F38" s="70"/>
+      <c r="G38" s="70"/>
+      <c r="H38" s="70"/>
       <c r="I38" s="4"/>
       <c r="J38" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="K38" s="68"/>
-      <c r="L38" s="68"/>
-      <c r="M38" s="68"/>
-      <c r="N38" s="71"/>
+      <c r="K38" s="58"/>
+      <c r="L38" s="58"/>
+      <c r="M38" s="58"/>
+      <c r="N38" s="47"/>
       <c r="O38" s="2"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
@@ -2356,22 +2235,22 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="C39" s="94"/>
-      <c r="D39" s="84" t="s">
+      <c r="C39" s="67"/>
+      <c r="D39" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="E39" s="84"/>
-      <c r="F39" s="84"/>
-      <c r="G39" s="84"/>
-      <c r="H39" s="84"/>
+      <c r="E39" s="69"/>
+      <c r="F39" s="69"/>
+      <c r="G39" s="69"/>
+      <c r="H39" s="69"/>
       <c r="I39" s="4"/>
       <c r="J39" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K39" s="68"/>
-      <c r="L39" s="68"/>
-      <c r="M39" s="68"/>
-      <c r="N39" s="71"/>
+      <c r="K39" s="58"/>
+      <c r="L39" s="58"/>
+      <c r="M39" s="58"/>
+      <c r="N39" s="47"/>
       <c r="O39" s="2"/>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
@@ -2379,20 +2258,20 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="C40" s="95"/>
-      <c r="D40" s="98"/>
-      <c r="E40" s="98"/>
-      <c r="F40" s="98"/>
-      <c r="G40" s="98"/>
-      <c r="H40" s="98"/>
+      <c r="C40" s="71"/>
+      <c r="D40" s="72"/>
+      <c r="E40" s="72"/>
+      <c r="F40" s="72"/>
+      <c r="G40" s="72"/>
+      <c r="H40" s="72"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="K40" s="68"/>
-      <c r="L40" s="68"/>
-      <c r="M40" s="68"/>
-      <c r="N40" s="71"/>
+      <c r="K40" s="58"/>
+      <c r="L40" s="58"/>
+      <c r="M40" s="58"/>
+      <c r="N40" s="47"/>
       <c r="O40" s="2"/>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
@@ -2400,20 +2279,20 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="C41" s="97"/>
-      <c r="D41" s="85"/>
-      <c r="E41" s="85"/>
-      <c r="F41" s="85"/>
-      <c r="G41" s="85"/>
-      <c r="H41" s="85"/>
+      <c r="C41" s="68"/>
+      <c r="D41" s="70"/>
+      <c r="E41" s="70"/>
+      <c r="F41" s="70"/>
+      <c r="G41" s="70"/>
+      <c r="H41" s="70"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="K41" s="68"/>
-      <c r="L41" s="68"/>
-      <c r="M41" s="68"/>
-      <c r="N41" s="71"/>
+      <c r="K41" s="58"/>
+      <c r="L41" s="58"/>
+      <c r="M41" s="58"/>
+      <c r="N41" s="47"/>
       <c r="O41" s="2"/>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
@@ -2421,22 +2300,22 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="C42" s="49"/>
-      <c r="D42" s="48"/>
-      <c r="E42" s="91" t="s">
+      <c r="C42" s="26"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="F42" s="91"/>
-      <c r="G42" s="91"/>
-      <c r="H42" s="91"/>
+      <c r="F42" s="73"/>
+      <c r="G42" s="73"/>
+      <c r="H42" s="73"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K42" s="68"/>
-      <c r="L42" s="68"/>
-      <c r="M42" s="68"/>
-      <c r="N42" s="71"/>
+      <c r="K42" s="58"/>
+      <c r="L42" s="58"/>
+      <c r="M42" s="58"/>
+      <c r="N42" s="47"/>
       <c r="O42" s="2"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
@@ -2444,22 +2323,22 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="C43" s="94"/>
-      <c r="D43" s="77"/>
-      <c r="E43" s="77"/>
-      <c r="F43" s="84" t="s">
+      <c r="C43" s="67"/>
+      <c r="D43" s="76"/>
+      <c r="E43" s="76"/>
+      <c r="F43" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="G43" s="84"/>
-      <c r="H43" s="84"/>
+      <c r="G43" s="69"/>
+      <c r="H43" s="69"/>
       <c r="I43" s="4"/>
       <c r="J43" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="K43" s="68"/>
-      <c r="L43" s="68"/>
-      <c r="M43" s="68"/>
-      <c r="N43" s="71"/>
+      <c r="K43" s="58"/>
+      <c r="L43" s="58"/>
+      <c r="M43" s="58"/>
+      <c r="N43" s="47"/>
       <c r="O43" s="2"/>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
@@ -2467,20 +2346,20 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="C44" s="95"/>
-      <c r="D44" s="96"/>
-      <c r="E44" s="96"/>
-      <c r="F44" s="98"/>
-      <c r="G44" s="98"/>
-      <c r="H44" s="98"/>
+      <c r="C44" s="71"/>
+      <c r="D44" s="78"/>
+      <c r="E44" s="78"/>
+      <c r="F44" s="72"/>
+      <c r="G44" s="72"/>
+      <c r="H44" s="72"/>
       <c r="I44" s="4"/>
       <c r="J44" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="K44" s="68"/>
-      <c r="L44" s="68"/>
-      <c r="M44" s="68"/>
-      <c r="N44" s="71"/>
+      <c r="K44" s="58"/>
+      <c r="L44" s="58"/>
+      <c r="M44" s="58"/>
+      <c r="N44" s="47"/>
       <c r="O44" s="2"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
@@ -2488,20 +2367,20 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="C45" s="95"/>
-      <c r="D45" s="96"/>
-      <c r="E45" s="96"/>
-      <c r="F45" s="98"/>
-      <c r="G45" s="98"/>
-      <c r="H45" s="98"/>
+      <c r="C45" s="71"/>
+      <c r="D45" s="78"/>
+      <c r="E45" s="78"/>
+      <c r="F45" s="72"/>
+      <c r="G45" s="72"/>
+      <c r="H45" s="72"/>
       <c r="I45" s="4"/>
       <c r="J45" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="K45" s="68"/>
-      <c r="L45" s="68"/>
-      <c r="M45" s="68"/>
-      <c r="N45" s="71"/>
+      <c r="K45" s="58"/>
+      <c r="L45" s="58"/>
+      <c r="M45" s="58"/>
+      <c r="N45" s="47"/>
       <c r="O45" s="2"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
@@ -2509,20 +2388,20 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="C46" s="95"/>
-      <c r="D46" s="96"/>
-      <c r="E46" s="96"/>
-      <c r="F46" s="98"/>
-      <c r="G46" s="98"/>
-      <c r="H46" s="98"/>
+      <c r="C46" s="71"/>
+      <c r="D46" s="78"/>
+      <c r="E46" s="78"/>
+      <c r="F46" s="72"/>
+      <c r="G46" s="72"/>
+      <c r="H46" s="72"/>
       <c r="I46" s="4"/>
       <c r="J46" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="K46" s="68"/>
-      <c r="L46" s="68"/>
-      <c r="M46" s="68"/>
-      <c r="N46" s="71"/>
+      <c r="K46" s="58"/>
+      <c r="L46" s="58"/>
+      <c r="M46" s="58"/>
+      <c r="N46" s="47"/>
       <c r="O46" s="2"/>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
@@ -2530,22 +2409,20 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="C47" s="97"/>
-      <c r="D47" s="78"/>
-      <c r="E47" s="78"/>
-      <c r="F47" s="85"/>
-      <c r="G47" s="85"/>
-      <c r="H47" s="85"/>
+      <c r="C47" s="68"/>
+      <c r="D47" s="77"/>
+      <c r="E47" s="77"/>
+      <c r="F47" s="70"/>
+      <c r="G47" s="70"/>
+      <c r="H47" s="70"/>
       <c r="I47" s="4"/>
       <c r="J47" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K47" s="59"/>
-      <c r="L47" s="59"/>
-      <c r="M47" s="59"/>
-      <c r="N47" s="71" t="s">
-        <v>36</v>
-      </c>
+      <c r="K47" s="51"/>
+      <c r="L47" s="51"/>
+      <c r="M47" s="51"/>
+      <c r="N47" s="47"/>
       <c r="O47" s="2"/>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
@@ -2553,22 +2430,22 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="C48" s="92"/>
-      <c r="D48" s="93"/>
-      <c r="E48" s="91" t="s">
+      <c r="C48" s="74"/>
+      <c r="D48" s="75"/>
+      <c r="E48" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="F48" s="91"/>
-      <c r="G48" s="91"/>
-      <c r="H48" s="91"/>
+      <c r="F48" s="73"/>
+      <c r="G48" s="73"/>
+      <c r="H48" s="73"/>
       <c r="I48" s="4"/>
       <c r="J48" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="K48" s="68"/>
-      <c r="L48" s="68"/>
-      <c r="M48" s="68"/>
-      <c r="N48" s="71"/>
+      <c r="K48" s="58"/>
+      <c r="L48" s="58"/>
+      <c r="M48" s="58"/>
+      <c r="N48" s="47"/>
       <c r="O48" s="2"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
@@ -2576,22 +2453,22 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="C49" s="94"/>
-      <c r="D49" s="77"/>
-      <c r="E49" s="77"/>
-      <c r="F49" s="84" t="s">
+      <c r="C49" s="67"/>
+      <c r="D49" s="76"/>
+      <c r="E49" s="76"/>
+      <c r="F49" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="G49" s="84"/>
-      <c r="H49" s="84"/>
+      <c r="G49" s="69"/>
+      <c r="H49" s="69"/>
       <c r="I49" s="4"/>
       <c r="J49" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="K49" s="68"/>
-      <c r="L49" s="68"/>
-      <c r="M49" s="68"/>
-      <c r="N49" s="71"/>
+      <c r="K49" s="58"/>
+      <c r="L49" s="58"/>
+      <c r="M49" s="58"/>
+      <c r="N49" s="47"/>
       <c r="O49" s="2"/>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.25">
@@ -2599,20 +2476,20 @@
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="C50" s="97"/>
-      <c r="D50" s="78"/>
-      <c r="E50" s="78"/>
-      <c r="F50" s="85"/>
-      <c r="G50" s="85"/>
-      <c r="H50" s="85"/>
+      <c r="C50" s="68"/>
+      <c r="D50" s="77"/>
+      <c r="E50" s="77"/>
+      <c r="F50" s="70"/>
+      <c r="G50" s="70"/>
+      <c r="H50" s="70"/>
       <c r="I50" s="4"/>
       <c r="J50" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K50" s="68"/>
-      <c r="L50" s="68"/>
-      <c r="M50" s="68"/>
-      <c r="N50" s="71"/>
+      <c r="K50" s="58"/>
+      <c r="L50" s="58"/>
+      <c r="M50" s="58"/>
+      <c r="N50" s="47"/>
       <c r="O50" s="2"/>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
@@ -2623,19 +2500,19 @@
       <c r="C51" s="5"/>
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
-      <c r="F51" s="91" t="s">
+      <c r="F51" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="G51" s="91"/>
-      <c r="H51" s="91"/>
+      <c r="G51" s="73"/>
+      <c r="H51" s="73"/>
       <c r="I51" s="4"/>
       <c r="J51" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K51" s="68"/>
-      <c r="L51" s="68"/>
-      <c r="M51" s="68"/>
-      <c r="N51" s="71"/>
+      <c r="K51" s="58"/>
+      <c r="L51" s="58"/>
+      <c r="M51" s="58"/>
+      <c r="N51" s="47"/>
       <c r="O51" s="2"/>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
@@ -2643,22 +2520,22 @@
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="C52" s="94"/>
-      <c r="D52" s="77"/>
-      <c r="E52" s="77"/>
-      <c r="F52" s="84" t="s">
+      <c r="C52" s="67"/>
+      <c r="D52" s="76"/>
+      <c r="E52" s="76"/>
+      <c r="F52" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="G52" s="84"/>
-      <c r="H52" s="84"/>
+      <c r="G52" s="69"/>
+      <c r="H52" s="69"/>
       <c r="I52" s="4"/>
       <c r="J52" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K52" s="68"/>
-      <c r="L52" s="68"/>
-      <c r="M52" s="68"/>
-      <c r="N52" s="71"/>
+      <c r="K52" s="58"/>
+      <c r="L52" s="58"/>
+      <c r="M52" s="58"/>
+      <c r="N52" s="47"/>
       <c r="O52" s="2"/>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
@@ -2666,20 +2543,20 @@
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="C53" s="97"/>
-      <c r="D53" s="78"/>
-      <c r="E53" s="78"/>
-      <c r="F53" s="85"/>
-      <c r="G53" s="85"/>
-      <c r="H53" s="85"/>
+      <c r="C53" s="68"/>
+      <c r="D53" s="77"/>
+      <c r="E53" s="77"/>
+      <c r="F53" s="70"/>
+      <c r="G53" s="70"/>
+      <c r="H53" s="70"/>
       <c r="I53" s="4"/>
       <c r="J53" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K53" s="68"/>
-      <c r="L53" s="68"/>
-      <c r="M53" s="68"/>
-      <c r="N53" s="71"/>
+      <c r="K53" s="58"/>
+      <c r="L53" s="58"/>
+      <c r="M53" s="58"/>
+      <c r="N53" s="47"/>
       <c r="O53" s="2"/>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.25">
@@ -2687,22 +2564,22 @@
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="C54" s="99"/>
-      <c r="D54" s="84"/>
-      <c r="E54" s="84"/>
-      <c r="F54" s="84" t="s">
+      <c r="C54" s="84"/>
+      <c r="D54" s="69"/>
+      <c r="E54" s="69"/>
+      <c r="F54" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="G54" s="84"/>
-      <c r="H54" s="84"/>
+      <c r="G54" s="69"/>
+      <c r="H54" s="69"/>
       <c r="I54" s="4"/>
       <c r="J54" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="K54" s="68"/>
-      <c r="L54" s="68"/>
-      <c r="M54" s="68"/>
-      <c r="N54" s="71"/>
+      <c r="K54" s="58"/>
+      <c r="L54" s="58"/>
+      <c r="M54" s="58"/>
+      <c r="N54" s="47"/>
       <c r="O54" s="2"/>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
@@ -2710,20 +2587,20 @@
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="C55" s="100"/>
-      <c r="D55" s="98"/>
-      <c r="E55" s="98"/>
-      <c r="F55" s="98"/>
-      <c r="G55" s="98"/>
-      <c r="H55" s="98"/>
+      <c r="C55" s="85"/>
+      <c r="D55" s="72"/>
+      <c r="E55" s="72"/>
+      <c r="F55" s="72"/>
+      <c r="G55" s="72"/>
+      <c r="H55" s="72"/>
       <c r="I55" s="4"/>
       <c r="J55" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="K55" s="68"/>
-      <c r="L55" s="68"/>
-      <c r="M55" s="68"/>
-      <c r="N55" s="71"/>
+      <c r="K55" s="58"/>
+      <c r="L55" s="58"/>
+      <c r="M55" s="58"/>
+      <c r="N55" s="47"/>
       <c r="O55" s="2"/>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
@@ -2731,20 +2608,20 @@
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="C56" s="100"/>
-      <c r="D56" s="98"/>
-      <c r="E56" s="98"/>
-      <c r="F56" s="98"/>
-      <c r="G56" s="98"/>
-      <c r="H56" s="98"/>
+      <c r="C56" s="85"/>
+      <c r="D56" s="72"/>
+      <c r="E56" s="72"/>
+      <c r="F56" s="72"/>
+      <c r="G56" s="72"/>
+      <c r="H56" s="72"/>
       <c r="I56" s="4"/>
       <c r="J56" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="K56" s="68"/>
-      <c r="L56" s="68"/>
-      <c r="M56" s="68"/>
-      <c r="N56" s="71"/>
+      <c r="K56" s="58"/>
+      <c r="L56" s="58"/>
+      <c r="M56" s="58"/>
+      <c r="N56" s="47"/>
       <c r="O56" s="2"/>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
@@ -2752,20 +2629,20 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="C57" s="100"/>
-      <c r="D57" s="98"/>
-      <c r="E57" s="98"/>
-      <c r="F57" s="98"/>
-      <c r="G57" s="98"/>
-      <c r="H57" s="98"/>
+      <c r="C57" s="85"/>
+      <c r="D57" s="72"/>
+      <c r="E57" s="72"/>
+      <c r="F57" s="72"/>
+      <c r="G57" s="72"/>
+      <c r="H57" s="72"/>
       <c r="I57" s="4"/>
       <c r="J57" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="K57" s="68"/>
-      <c r="L57" s="68"/>
-      <c r="M57" s="68"/>
-      <c r="N57" s="71"/>
+      <c r="K57" s="58"/>
+      <c r="L57" s="58"/>
+      <c r="M57" s="58"/>
+      <c r="N57" s="47"/>
       <c r="O57" s="2"/>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
@@ -2773,22 +2650,20 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="C58" s="101"/>
-      <c r="D58" s="85"/>
-      <c r="E58" s="85"/>
-      <c r="F58" s="85"/>
-      <c r="G58" s="85"/>
-      <c r="H58" s="85"/>
+      <c r="C58" s="86"/>
+      <c r="D58" s="70"/>
+      <c r="E58" s="70"/>
+      <c r="F58" s="70"/>
+      <c r="G58" s="70"/>
+      <c r="H58" s="70"/>
       <c r="I58" s="4"/>
       <c r="J58" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K58" s="59"/>
-      <c r="L58" s="59"/>
-      <c r="M58" s="59"/>
-      <c r="N58" s="71" t="s">
-        <v>36</v>
-      </c>
+      <c r="K58" s="51"/>
+      <c r="L58" s="51"/>
+      <c r="M58" s="51"/>
+      <c r="N58" s="47"/>
       <c r="O58" s="2"/>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.25">
@@ -2796,22 +2671,22 @@
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="C59" s="101" t="s">
+      <c r="C59" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="D59" s="85"/>
-      <c r="E59" s="85"/>
-      <c r="F59" s="85"/>
-      <c r="G59" s="85"/>
-      <c r="H59" s="91"/>
+      <c r="D59" s="70"/>
+      <c r="E59" s="70"/>
+      <c r="F59" s="70"/>
+      <c r="G59" s="70"/>
+      <c r="H59" s="73"/>
       <c r="I59" s="4"/>
       <c r="J59" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K59" s="68"/>
-      <c r="L59" s="68"/>
-      <c r="M59" s="68"/>
-      <c r="N59" s="71"/>
+      <c r="K59" s="58"/>
+      <c r="L59" s="58"/>
+      <c r="M59" s="58"/>
+      <c r="N59" s="47"/>
       <c r="O59" s="2"/>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.25">
@@ -2819,22 +2694,22 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="C60" s="94"/>
-      <c r="D60" s="84" t="s">
+      <c r="C60" s="67"/>
+      <c r="D60" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="E60" s="84"/>
-      <c r="F60" s="84"/>
-      <c r="G60" s="84"/>
-      <c r="H60" s="84"/>
+      <c r="E60" s="69"/>
+      <c r="F60" s="69"/>
+      <c r="G60" s="69"/>
+      <c r="H60" s="69"/>
       <c r="I60" s="4"/>
       <c r="J60" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K60" s="68"/>
-      <c r="L60" s="68"/>
-      <c r="M60" s="68"/>
-      <c r="N60" s="71"/>
+      <c r="K60" s="58"/>
+      <c r="L60" s="58"/>
+      <c r="M60" s="58"/>
+      <c r="N60" s="47"/>
       <c r="O60" s="2"/>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.25">
@@ -2842,20 +2717,20 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="C61" s="97"/>
-      <c r="D61" s="85"/>
-      <c r="E61" s="85"/>
-      <c r="F61" s="85"/>
-      <c r="G61" s="85"/>
-      <c r="H61" s="85"/>
+      <c r="C61" s="68"/>
+      <c r="D61" s="70"/>
+      <c r="E61" s="70"/>
+      <c r="F61" s="70"/>
+      <c r="G61" s="70"/>
+      <c r="H61" s="70"/>
       <c r="I61" s="4"/>
       <c r="J61" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K61" s="68"/>
-      <c r="L61" s="68"/>
-      <c r="M61" s="68"/>
-      <c r="N61" s="71"/>
+      <c r="K61" s="58"/>
+      <c r="L61" s="58"/>
+      <c r="M61" s="58"/>
+      <c r="N61" s="47"/>
       <c r="O61" s="2"/>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
@@ -2864,19 +2739,19 @@
         <v>51</v>
       </c>
       <c r="C62" s="5"/>
-      <c r="D62" s="91" t="s">
+      <c r="D62" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="E62" s="91"/>
-      <c r="F62" s="91"/>
-      <c r="G62" s="91"/>
-      <c r="H62" s="91"/>
+      <c r="E62" s="73"/>
+      <c r="F62" s="73"/>
+      <c r="G62" s="73"/>
+      <c r="H62" s="73"/>
       <c r="I62" s="4"/>
       <c r="J62" s="4"/>
-      <c r="K62" s="68"/>
-      <c r="L62" s="68"/>
-      <c r="M62" s="68"/>
-      <c r="N62" s="71"/>
+      <c r="K62" s="58"/>
+      <c r="L62" s="58"/>
+      <c r="M62" s="58"/>
+      <c r="N62" s="47"/>
       <c r="O62" s="2"/>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.25">
@@ -2884,22 +2759,22 @@
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="C63" s="94"/>
-      <c r="D63" s="77"/>
-      <c r="E63" s="84" t="s">
+      <c r="C63" s="67"/>
+      <c r="D63" s="76"/>
+      <c r="E63" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="F63" s="84"/>
-      <c r="G63" s="84"/>
-      <c r="H63" s="84"/>
+      <c r="F63" s="69"/>
+      <c r="G63" s="69"/>
+      <c r="H63" s="69"/>
       <c r="I63" s="4"/>
       <c r="J63" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K63" s="68"/>
-      <c r="L63" s="68"/>
-      <c r="M63" s="68"/>
-      <c r="N63" s="71"/>
+      <c r="K63" s="58"/>
+      <c r="L63" s="58"/>
+      <c r="M63" s="58"/>
+      <c r="N63" s="47"/>
       <c r="O63" s="2"/>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.25">
@@ -2907,22 +2782,20 @@
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="C64" s="95"/>
-      <c r="D64" s="96"/>
-      <c r="E64" s="98"/>
-      <c r="F64" s="98"/>
-      <c r="G64" s="98"/>
-      <c r="H64" s="98"/>
+      <c r="C64" s="71"/>
+      <c r="D64" s="78"/>
+      <c r="E64" s="72"/>
+      <c r="F64" s="72"/>
+      <c r="G64" s="72"/>
+      <c r="H64" s="72"/>
       <c r="I64" s="4"/>
       <c r="J64" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K64" s="68"/>
-      <c r="L64" s="60"/>
-      <c r="M64" s="60"/>
-      <c r="N64" s="62" t="s">
-        <v>28</v>
-      </c>
+      <c r="K64" s="58"/>
+      <c r="L64" s="52"/>
+      <c r="M64" s="52"/>
+      <c r="N64" s="54"/>
       <c r="O64" s="2"/>
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
@@ -2930,20 +2803,20 @@
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="C65" s="95"/>
-      <c r="D65" s="96"/>
-      <c r="E65" s="98"/>
-      <c r="F65" s="98"/>
-      <c r="G65" s="98"/>
-      <c r="H65" s="98"/>
+      <c r="C65" s="71"/>
+      <c r="D65" s="78"/>
+      <c r="E65" s="72"/>
+      <c r="F65" s="72"/>
+      <c r="G65" s="72"/>
+      <c r="H65" s="72"/>
       <c r="I65" s="4"/>
       <c r="J65" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K65" s="68"/>
-      <c r="L65" s="68"/>
-      <c r="M65" s="68"/>
-      <c r="N65" s="71"/>
+      <c r="K65" s="58"/>
+      <c r="L65" s="58"/>
+      <c r="M65" s="58"/>
+      <c r="N65" s="47"/>
       <c r="O65" s="2"/>
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
@@ -2951,22 +2824,20 @@
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="C66" s="97"/>
-      <c r="D66" s="78"/>
-      <c r="E66" s="85"/>
-      <c r="F66" s="85"/>
-      <c r="G66" s="85"/>
-      <c r="H66" s="85"/>
+      <c r="C66" s="68"/>
+      <c r="D66" s="77"/>
+      <c r="E66" s="70"/>
+      <c r="F66" s="70"/>
+      <c r="G66" s="70"/>
+      <c r="H66" s="70"/>
       <c r="I66" s="4"/>
       <c r="J66" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="K66" s="68"/>
-      <c r="L66" s="60"/>
-      <c r="M66" s="60"/>
-      <c r="N66" s="62" t="s">
-        <v>29</v>
-      </c>
+      <c r="K66" s="58"/>
+      <c r="L66" s="52"/>
+      <c r="M66" s="52"/>
+      <c r="N66" s="54"/>
       <c r="O66" s="2"/>
     </row>
     <row r="67" spans="2:15" x14ac:dyDescent="0.25">
@@ -2977,19 +2848,19 @@
       <c r="C67" s="5"/>
       <c r="D67" s="9"/>
       <c r="E67" s="9"/>
-      <c r="F67" s="91" t="s">
+      <c r="F67" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="G67" s="91"/>
-      <c r="H67" s="91"/>
+      <c r="G67" s="73"/>
+      <c r="H67" s="73"/>
       <c r="I67" s="4"/>
       <c r="J67" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K67" s="68"/>
-      <c r="L67" s="68"/>
-      <c r="M67" s="68"/>
-      <c r="N67" s="71"/>
+      <c r="K67" s="58"/>
+      <c r="L67" s="58"/>
+      <c r="M67" s="58"/>
+      <c r="N67" s="47"/>
       <c r="O67" s="2"/>
     </row>
     <row r="68" spans="2:15" x14ac:dyDescent="0.25">
@@ -2997,22 +2868,22 @@
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="C68" s="94"/>
-      <c r="D68" s="77"/>
-      <c r="E68" s="84" t="s">
+      <c r="C68" s="67"/>
+      <c r="D68" s="76"/>
+      <c r="E68" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="F68" s="84"/>
-      <c r="G68" s="84"/>
-      <c r="H68" s="84"/>
+      <c r="F68" s="69"/>
+      <c r="G68" s="69"/>
+      <c r="H68" s="69"/>
       <c r="I68" s="4"/>
       <c r="J68" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K68" s="68"/>
-      <c r="L68" s="68"/>
-      <c r="M68" s="68"/>
-      <c r="N68" s="71"/>
+      <c r="K68" s="58"/>
+      <c r="L68" s="58"/>
+      <c r="M68" s="58"/>
+      <c r="N68" s="47"/>
       <c r="O68" s="2"/>
     </row>
     <row r="69" spans="2:15" x14ac:dyDescent="0.25">
@@ -3020,20 +2891,20 @@
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="C69" s="95"/>
-      <c r="D69" s="96"/>
-      <c r="E69" s="98"/>
-      <c r="F69" s="98"/>
-      <c r="G69" s="98"/>
-      <c r="H69" s="98"/>
+      <c r="C69" s="71"/>
+      <c r="D69" s="78"/>
+      <c r="E69" s="72"/>
+      <c r="F69" s="72"/>
+      <c r="G69" s="72"/>
+      <c r="H69" s="72"/>
       <c r="I69" s="4"/>
       <c r="J69" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K69" s="68"/>
-      <c r="L69" s="68"/>
-      <c r="M69" s="68"/>
-      <c r="N69" s="71"/>
+      <c r="K69" s="58"/>
+      <c r="L69" s="58"/>
+      <c r="M69" s="58"/>
+      <c r="N69" s="47"/>
       <c r="O69" s="2"/>
     </row>
     <row r="70" spans="2:15" x14ac:dyDescent="0.25">
@@ -3041,20 +2912,20 @@
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="C70" s="95"/>
-      <c r="D70" s="96"/>
-      <c r="E70" s="98"/>
-      <c r="F70" s="98"/>
-      <c r="G70" s="98"/>
-      <c r="H70" s="98"/>
+      <c r="C70" s="71"/>
+      <c r="D70" s="78"/>
+      <c r="E70" s="72"/>
+      <c r="F70" s="72"/>
+      <c r="G70" s="72"/>
+      <c r="H70" s="72"/>
       <c r="I70" s="4"/>
       <c r="J70" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K70" s="68"/>
-      <c r="L70" s="68"/>
-      <c r="M70" s="68"/>
-      <c r="N70" s="71"/>
+      <c r="K70" s="58"/>
+      <c r="L70" s="58"/>
+      <c r="M70" s="58"/>
+      <c r="N70" s="47"/>
       <c r="O70" s="2"/>
     </row>
     <row r="71" spans="2:15" x14ac:dyDescent="0.25">
@@ -3062,20 +2933,20 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="C71" s="95"/>
-      <c r="D71" s="96"/>
-      <c r="E71" s="98"/>
-      <c r="F71" s="98"/>
-      <c r="G71" s="98"/>
-      <c r="H71" s="98"/>
+      <c r="C71" s="71"/>
+      <c r="D71" s="78"/>
+      <c r="E71" s="72"/>
+      <c r="F71" s="72"/>
+      <c r="G71" s="72"/>
+      <c r="H71" s="72"/>
       <c r="I71" s="4"/>
       <c r="J71" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K71" s="68"/>
-      <c r="L71" s="68"/>
-      <c r="M71" s="68"/>
-      <c r="N71" s="71"/>
+      <c r="K71" s="58"/>
+      <c r="L71" s="58"/>
+      <c r="M71" s="58"/>
+      <c r="N71" s="47"/>
       <c r="O71" s="2"/>
     </row>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">
@@ -3083,20 +2954,20 @@
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="C72" s="95"/>
-      <c r="D72" s="96"/>
-      <c r="E72" s="98"/>
-      <c r="F72" s="98"/>
-      <c r="G72" s="98"/>
-      <c r="H72" s="98"/>
+      <c r="C72" s="71"/>
+      <c r="D72" s="78"/>
+      <c r="E72" s="72"/>
+      <c r="F72" s="72"/>
+      <c r="G72" s="72"/>
+      <c r="H72" s="72"/>
       <c r="I72" s="4"/>
       <c r="J72" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="K72" s="68"/>
-      <c r="L72" s="68"/>
-      <c r="M72" s="68"/>
-      <c r="N72" s="71"/>
+      <c r="K72" s="58"/>
+      <c r="L72" s="58"/>
+      <c r="M72" s="58"/>
+      <c r="N72" s="47"/>
       <c r="O72" s="2"/>
     </row>
     <row r="73" spans="2:15" x14ac:dyDescent="0.25">
@@ -3104,22 +2975,22 @@
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="C73" s="94"/>
-      <c r="D73" s="77"/>
-      <c r="E73" s="77"/>
-      <c r="F73" s="84" t="s">
+      <c r="C73" s="67"/>
+      <c r="D73" s="76"/>
+      <c r="E73" s="76"/>
+      <c r="F73" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="G73" s="84"/>
-      <c r="H73" s="84"/>
+      <c r="G73" s="69"/>
+      <c r="H73" s="69"/>
       <c r="I73" s="4"/>
       <c r="J73" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="K73" s="68"/>
-      <c r="L73" s="68"/>
-      <c r="M73" s="68"/>
-      <c r="N73" s="71"/>
+      <c r="K73" s="58"/>
+      <c r="L73" s="58"/>
+      <c r="M73" s="58"/>
+      <c r="N73" s="47"/>
       <c r="O73" s="2"/>
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.25">
@@ -3127,20 +2998,20 @@
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="C74" s="95"/>
-      <c r="D74" s="96"/>
-      <c r="E74" s="96"/>
-      <c r="F74" s="98"/>
-      <c r="G74" s="98"/>
-      <c r="H74" s="98"/>
+      <c r="C74" s="71"/>
+      <c r="D74" s="78"/>
+      <c r="E74" s="78"/>
+      <c r="F74" s="72"/>
+      <c r="G74" s="72"/>
+      <c r="H74" s="72"/>
       <c r="I74" s="4"/>
       <c r="J74" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="K74" s="68"/>
-      <c r="L74" s="68"/>
-      <c r="M74" s="68"/>
-      <c r="N74" s="71"/>
+      <c r="K74" s="58"/>
+      <c r="L74" s="58"/>
+      <c r="M74" s="58"/>
+      <c r="N74" s="47"/>
       <c r="O74" s="2"/>
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.25">
@@ -3148,20 +3019,20 @@
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="C75" s="95"/>
-      <c r="D75" s="96"/>
-      <c r="E75" s="96"/>
-      <c r="F75" s="98"/>
-      <c r="G75" s="98"/>
-      <c r="H75" s="98"/>
+      <c r="C75" s="71"/>
+      <c r="D75" s="78"/>
+      <c r="E75" s="78"/>
+      <c r="F75" s="72"/>
+      <c r="G75" s="72"/>
+      <c r="H75" s="72"/>
       <c r="I75" s="4"/>
       <c r="J75" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K75" s="68"/>
-      <c r="L75" s="68"/>
-      <c r="M75" s="68"/>
-      <c r="N75" s="71"/>
+      <c r="K75" s="58"/>
+      <c r="L75" s="58"/>
+      <c r="M75" s="58"/>
+      <c r="N75" s="47"/>
       <c r="O75" s="2"/>
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.25">
@@ -3169,22 +3040,20 @@
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="C76" s="97"/>
-      <c r="D76" s="78"/>
-      <c r="E76" s="78"/>
-      <c r="F76" s="85"/>
-      <c r="G76" s="85"/>
-      <c r="H76" s="85"/>
+      <c r="C76" s="68"/>
+      <c r="D76" s="77"/>
+      <c r="E76" s="77"/>
+      <c r="F76" s="70"/>
+      <c r="G76" s="70"/>
+      <c r="H76" s="70"/>
       <c r="I76" s="4"/>
       <c r="J76" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="K76" s="68"/>
-      <c r="L76" s="59"/>
-      <c r="M76" s="59"/>
-      <c r="N76" s="71" t="s">
-        <v>59</v>
-      </c>
+      <c r="K76" s="58"/>
+      <c r="L76" s="51"/>
+      <c r="M76" s="51"/>
+      <c r="N76" s="47"/>
       <c r="O76" s="2"/>
     </row>
     <row r="77" spans="2:15" x14ac:dyDescent="0.25">
@@ -3196,18 +3065,18 @@
       <c r="D77" s="9"/>
       <c r="E77" s="9"/>
       <c r="F77" s="9"/>
-      <c r="G77" s="91" t="s">
+      <c r="G77" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="H77" s="91"/>
+      <c r="H77" s="73"/>
       <c r="I77" s="4"/>
       <c r="J77" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="K77" s="68"/>
-      <c r="L77" s="68"/>
-      <c r="M77" s="68"/>
-      <c r="N77" s="71"/>
+      <c r="K77" s="58"/>
+      <c r="L77" s="58"/>
+      <c r="M77" s="58"/>
+      <c r="N77" s="47"/>
       <c r="O77" s="2"/>
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.25">
@@ -3215,20 +3084,20 @@
         <f t="shared" si="0"/>
         <v>67</v>
       </c>
-      <c r="C78" s="92"/>
-      <c r="D78" s="93"/>
-      <c r="E78" s="93"/>
-      <c r="F78" s="93"/>
-      <c r="G78" s="91" t="s">
+      <c r="C78" s="74"/>
+      <c r="D78" s="75"/>
+      <c r="E78" s="75"/>
+      <c r="F78" s="75"/>
+      <c r="G78" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="H78" s="91"/>
+      <c r="H78" s="73"/>
       <c r="I78" s="4"/>
       <c r="J78" s="4"/>
-      <c r="K78" s="68"/>
-      <c r="L78" s="68"/>
-      <c r="M78" s="68"/>
-      <c r="N78" s="71"/>
+      <c r="K78" s="58"/>
+      <c r="L78" s="58"/>
+      <c r="M78" s="58"/>
+      <c r="N78" s="47"/>
       <c r="O78" s="2"/>
     </row>
     <row r="79" spans="2:15" x14ac:dyDescent="0.25">
@@ -3244,10 +3113,10 @@
       <c r="H79" s="9"/>
       <c r="I79" s="4"/>
       <c r="J79" s="4"/>
-      <c r="K79" s="68"/>
-      <c r="L79" s="68"/>
-      <c r="M79" s="68"/>
-      <c r="N79" s="71"/>
+      <c r="K79" s="58"/>
+      <c r="L79" s="58"/>
+      <c r="M79" s="58"/>
+      <c r="N79" s="47"/>
       <c r="O79" s="2"/>
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.25">
@@ -3263,10 +3132,10 @@
       <c r="H80" s="9"/>
       <c r="I80" s="4"/>
       <c r="J80" s="4"/>
-      <c r="K80" s="68"/>
-      <c r="L80" s="68"/>
-      <c r="M80" s="68"/>
-      <c r="N80" s="71"/>
+      <c r="K80" s="58"/>
+      <c r="L80" s="58"/>
+      <c r="M80" s="58"/>
+      <c r="N80" s="47"/>
       <c r="O80" s="2"/>
     </row>
     <row r="81" spans="2:15" x14ac:dyDescent="0.25">
@@ -3282,10 +3151,10 @@
       <c r="H81" s="9"/>
       <c r="I81" s="4"/>
       <c r="J81" s="4"/>
-      <c r="K81" s="68"/>
-      <c r="L81" s="68"/>
-      <c r="M81" s="68"/>
-      <c r="N81" s="71"/>
+      <c r="K81" s="58"/>
+      <c r="L81" s="58"/>
+      <c r="M81" s="58"/>
+      <c r="N81" s="47"/>
       <c r="O81" s="2"/>
     </row>
     <row r="82" spans="2:15" x14ac:dyDescent="0.25">
@@ -3301,10 +3170,10 @@
       <c r="H82" s="9"/>
       <c r="I82" s="4"/>
       <c r="J82" s="4"/>
-      <c r="K82" s="68"/>
-      <c r="L82" s="68"/>
-      <c r="M82" s="68"/>
-      <c r="N82" s="71"/>
+      <c r="K82" s="58"/>
+      <c r="L82" s="58"/>
+      <c r="M82" s="58"/>
+      <c r="N82" s="47"/>
       <c r="O82" s="2"/>
     </row>
     <row r="83" spans="2:15" x14ac:dyDescent="0.25">
@@ -3320,10 +3189,10 @@
       <c r="H83" s="9"/>
       <c r="I83" s="4"/>
       <c r="J83" s="4"/>
-      <c r="K83" s="68"/>
-      <c r="L83" s="68"/>
-      <c r="M83" s="68"/>
-      <c r="N83" s="71"/>
+      <c r="K83" s="58"/>
+      <c r="L83" s="58"/>
+      <c r="M83" s="58"/>
+      <c r="N83" s="47"/>
       <c r="O83" s="2"/>
     </row>
     <row r="84" spans="2:15" x14ac:dyDescent="0.25">
@@ -3339,10 +3208,10 @@
       <c r="H84" s="9"/>
       <c r="I84" s="4"/>
       <c r="J84" s="4"/>
-      <c r="K84" s="68"/>
-      <c r="L84" s="68"/>
-      <c r="M84" s="68"/>
-      <c r="N84" s="71"/>
+      <c r="K84" s="58"/>
+      <c r="L84" s="58"/>
+      <c r="M84" s="58"/>
+      <c r="N84" s="47"/>
       <c r="O84" s="2"/>
     </row>
     <row r="85" spans="2:15" x14ac:dyDescent="0.25">
@@ -3358,10 +3227,10 @@
       <c r="H85" s="9"/>
       <c r="I85" s="4"/>
       <c r="J85" s="4"/>
-      <c r="K85" s="68"/>
-      <c r="L85" s="68"/>
-      <c r="M85" s="68"/>
-      <c r="N85" s="71"/>
+      <c r="K85" s="58"/>
+      <c r="L85" s="58"/>
+      <c r="M85" s="58"/>
+      <c r="N85" s="47"/>
       <c r="O85" s="2"/>
     </row>
     <row r="86" spans="2:15" x14ac:dyDescent="0.25">
@@ -3377,10 +3246,10 @@
       <c r="H86" s="9"/>
       <c r="I86" s="4"/>
       <c r="J86" s="4"/>
-      <c r="K86" s="68"/>
-      <c r="L86" s="68"/>
-      <c r="M86" s="68"/>
-      <c r="N86" s="71"/>
+      <c r="K86" s="58"/>
+      <c r="L86" s="58"/>
+      <c r="M86" s="58"/>
+      <c r="N86" s="47"/>
       <c r="O86" s="2"/>
     </row>
     <row r="87" spans="2:15" x14ac:dyDescent="0.25">
@@ -3396,10 +3265,10 @@
       <c r="H87" s="9"/>
       <c r="I87" s="4"/>
       <c r="J87" s="4"/>
-      <c r="K87" s="68"/>
-      <c r="L87" s="68"/>
-      <c r="M87" s="68"/>
-      <c r="N87" s="71"/>
+      <c r="K87" s="58"/>
+      <c r="L87" s="58"/>
+      <c r="M87" s="58"/>
+      <c r="N87" s="47"/>
       <c r="O87" s="2"/>
     </row>
     <row r="88" spans="2:15" x14ac:dyDescent="0.25">
@@ -3415,33 +3284,26 @@
       <c r="H88" s="9"/>
       <c r="I88" s="4"/>
       <c r="J88" s="4"/>
-      <c r="K88" s="68"/>
-      <c r="L88" s="68"/>
-      <c r="M88" s="68"/>
-      <c r="N88" s="71"/>
+      <c r="K88" s="58"/>
+      <c r="L88" s="58"/>
+      <c r="M88" s="58"/>
+      <c r="N88" s="47"/>
       <c r="O88" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="49">
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:H38"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="D39:H41"/>
-    <mergeCell ref="D32:H32"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:H48"/>
-    <mergeCell ref="C49:E50"/>
-    <mergeCell ref="F49:H50"/>
-    <mergeCell ref="E42:H42"/>
-    <mergeCell ref="C43:E47"/>
-    <mergeCell ref="F43:H47"/>
-    <mergeCell ref="C78:F78"/>
-    <mergeCell ref="G78:H78"/>
-    <mergeCell ref="C73:E76"/>
-    <mergeCell ref="F73:H76"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="C68:D72"/>
-    <mergeCell ref="E68:H72"/>
+  <mergeCells count="47">
+    <mergeCell ref="L22:L25"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="N22:N25"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="L10:L13"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="J20:N20"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="J9:N9"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="C7:H7"/>
@@ -3458,20 +3320,25 @@
     <mergeCell ref="F51:H51"/>
     <mergeCell ref="C52:E53"/>
     <mergeCell ref="F52:H53"/>
-    <mergeCell ref="L22:L25"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="N22:N25"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="L10:L13"/>
-    <mergeCell ref="N10:N16"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="J18:N18"/>
-    <mergeCell ref="J20:N20"/>
-    <mergeCell ref="J7:N7"/>
-    <mergeCell ref="J9:N9"/>
+    <mergeCell ref="C78:F78"/>
+    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="C73:E76"/>
+    <mergeCell ref="F73:H76"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="C68:D72"/>
+    <mergeCell ref="E68:H72"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:H48"/>
+    <mergeCell ref="C49:E50"/>
+    <mergeCell ref="F49:H50"/>
+    <mergeCell ref="E42:H42"/>
+    <mergeCell ref="C43:E47"/>
+    <mergeCell ref="F43:H47"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:H38"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="D39:H41"/>
+    <mergeCell ref="D32:H32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3538,18 +3405,18 @@
       <c r="B5" s="11">
         <v>1</v>
       </c>
-      <c r="C5" s="90" t="s">
+      <c r="C5" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
-      <c r="H5" s="102"/>
-      <c r="I5" s="103" t="s">
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="100"/>
+      <c r="I5" s="109" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="104"/>
+      <c r="J5" s="101"/>
       <c r="K5" s="4" t="s">
         <v>6</v>
       </c>
@@ -3560,14 +3427,14 @@
         <f>B5+1</f>
         <v>2</v>
       </c>
-      <c r="C6" s="90" t="s">
+      <c r="C6" s="83" t="s">
         <v>86</v>
       </c>
-      <c r="D6" s="91"/>
-      <c r="E6" s="91"/>
-      <c r="F6" s="91"/>
-      <c r="G6" s="91"/>
-      <c r="H6" s="102"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
+      <c r="G6" s="73"/>
+      <c r="H6" s="100"/>
       <c r="I6" s="23"/>
       <c r="J6" s="24"/>
       <c r="K6" s="10" t="s">
@@ -3576,22 +3443,22 @@
       <c r="L6" s="4"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="105">
+      <c r="B7" s="103">
         <f>B6+1</f>
         <v>3</v>
       </c>
-      <c r="C7" s="99" t="s">
+      <c r="C7" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="107"/>
-      <c r="I7" s="103" t="s">
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="106"/>
+      <c r="I7" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="104"/>
+      <c r="J7" s="101"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="N7" s="20" t="s">
@@ -3599,17 +3466,17 @@
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="106"/>
-      <c r="C8" s="101"/>
-      <c r="D8" s="85"/>
-      <c r="E8" s="85"/>
-      <c r="F8" s="85"/>
-      <c r="G8" s="85"/>
+      <c r="B8" s="105"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="70"/>
       <c r="H8" s="108"/>
-      <c r="I8" s="103" t="s">
+      <c r="I8" s="109" t="s">
         <v>25</v>
       </c>
-      <c r="J8" s="104"/>
+      <c r="J8" s="101"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="N8" s="4" t="s">
@@ -3617,22 +3484,22 @@
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="105">
+      <c r="B9" s="103">
         <f>B7+1</f>
         <v>4</v>
       </c>
-      <c r="C9" s="94"/>
-      <c r="D9" s="84" t="s">
+      <c r="C9" s="67"/>
+      <c r="D9" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="84"/>
-      <c r="H9" s="107"/>
-      <c r="I9" s="103" t="s">
+      <c r="E9" s="69"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="106"/>
+      <c r="I9" s="109" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="104"/>
+      <c r="J9" s="101"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="N9" s="10" t="s">
@@ -3640,67 +3507,67 @@
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="106"/>
-      <c r="C10" s="97"/>
-      <c r="D10" s="85"/>
-      <c r="E10" s="85"/>
-      <c r="F10" s="85"/>
-      <c r="G10" s="85"/>
+      <c r="B10" s="105"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="70"/>
       <c r="H10" s="108"/>
-      <c r="I10" s="103" t="s">
+      <c r="I10" s="109" t="s">
         <v>49</v>
       </c>
-      <c r="J10" s="104"/>
+      <c r="J10" s="101"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="105">
+      <c r="B11" s="103">
         <f>B9+1</f>
         <v>5</v>
       </c>
-      <c r="C11" s="94"/>
-      <c r="D11" s="84" t="s">
+      <c r="C11" s="67"/>
+      <c r="D11" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="84"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="84"/>
-      <c r="H11" s="107"/>
-      <c r="I11" s="103" t="s">
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="69"/>
+      <c r="H11" s="106"/>
+      <c r="I11" s="109" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="104"/>
+      <c r="J11" s="101"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="109"/>
-      <c r="C12" s="95"/>
-      <c r="D12" s="98"/>
-      <c r="E12" s="98"/>
-      <c r="F12" s="98"/>
-      <c r="G12" s="98"/>
-      <c r="H12" s="110"/>
-      <c r="I12" s="103" t="s">
+      <c r="B12" s="104"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="72"/>
+      <c r="H12" s="107"/>
+      <c r="I12" s="109" t="s">
         <v>50</v>
       </c>
-      <c r="J12" s="104"/>
+      <c r="J12" s="101"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="106"/>
-      <c r="C13" s="97"/>
-      <c r="D13" s="85"/>
-      <c r="E13" s="85"/>
-      <c r="F13" s="85"/>
-      <c r="G13" s="85"/>
+      <c r="B13" s="105"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="70"/>
       <c r="H13" s="108"/>
-      <c r="I13" s="103" t="s">
+      <c r="I13" s="109" t="s">
         <v>54</v>
       </c>
-      <c r="J13" s="104"/>
+      <c r="J13" s="101"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
     </row>
@@ -3711,62 +3578,62 @@
       </c>
       <c r="C14" s="26"/>
       <c r="D14" s="25"/>
-      <c r="E14" s="91" t="s">
+      <c r="E14" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="91"/>
-      <c r="G14" s="91"/>
-      <c r="H14" s="102"/>
-      <c r="I14" s="103" t="s">
+      <c r="F14" s="73"/>
+      <c r="G14" s="73"/>
+      <c r="H14" s="100"/>
+      <c r="I14" s="109" t="s">
         <v>57</v>
       </c>
-      <c r="J14" s="104"/>
+      <c r="J14" s="101"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="105">
+      <c r="B15" s="103">
         <f>B14+1</f>
         <v>7</v>
       </c>
-      <c r="C15" s="94"/>
-      <c r="D15" s="77"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="84" t="s">
+      <c r="C15" s="67"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="84"/>
-      <c r="H15" s="107"/>
-      <c r="I15" s="103" t="s">
+      <c r="G15" s="69"/>
+      <c r="H15" s="106"/>
+      <c r="I15" s="109" t="s">
         <v>31</v>
       </c>
-      <c r="J15" s="104"/>
+      <c r="J15" s="101"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="109"/>
-      <c r="C16" s="95"/>
-      <c r="D16" s="96"/>
-      <c r="E16" s="96"/>
-      <c r="F16" s="98"/>
-      <c r="G16" s="98"/>
-      <c r="H16" s="110"/>
-      <c r="I16" s="103" t="s">
+      <c r="B16" s="104"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="72"/>
+      <c r="G16" s="72"/>
+      <c r="H16" s="107"/>
+      <c r="I16" s="109" t="s">
         <v>33</v>
       </c>
-      <c r="J16" s="111"/>
-      <c r="K16" s="111"/>
-      <c r="L16" s="111"/>
+      <c r="J16" s="110"/>
+      <c r="K16" s="110"/>
+      <c r="L16" s="110"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="109"/>
-      <c r="C17" s="95"/>
-      <c r="D17" s="96"/>
-      <c r="E17" s="96"/>
-      <c r="F17" s="98"/>
-      <c r="G17" s="98"/>
-      <c r="H17" s="110"/>
+      <c r="B17" s="104"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="72"/>
+      <c r="G17" s="72"/>
+      <c r="H17" s="107"/>
       <c r="I17" s="7"/>
       <c r="J17" s="8" t="s">
         <v>32</v>
@@ -3775,13 +3642,13 @@
       <c r="L17" s="4"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="109"/>
-      <c r="C18" s="95"/>
-      <c r="D18" s="96"/>
-      <c r="E18" s="96"/>
-      <c r="F18" s="98"/>
-      <c r="G18" s="98"/>
-      <c r="H18" s="110"/>
+      <c r="B18" s="104"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="78"/>
+      <c r="E18" s="78"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="72"/>
+      <c r="H18" s="107"/>
       <c r="I18" s="7"/>
       <c r="J18" s="8" t="s">
         <v>34</v>
@@ -3790,12 +3657,12 @@
       <c r="L18" s="4"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="106"/>
-      <c r="C19" s="97"/>
-      <c r="D19" s="78"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="85"/>
-      <c r="G19" s="85"/>
+      <c r="B19" s="105"/>
+      <c r="C19" s="68"/>
+      <c r="D19" s="77"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="70"/>
+      <c r="G19" s="70"/>
       <c r="H19" s="108"/>
       <c r="I19" s="7"/>
       <c r="J19" s="8" t="s">
@@ -3811,53 +3678,53 @@
         <f>B15+1</f>
         <v>8</v>
       </c>
-      <c r="C20" s="92"/>
-      <c r="D20" s="93"/>
-      <c r="E20" s="91" t="s">
+      <c r="C20" s="74"/>
+      <c r="D20" s="75"/>
+      <c r="E20" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="91"/>
-      <c r="G20" s="91"/>
-      <c r="H20" s="102"/>
-      <c r="I20" s="103" t="s">
+      <c r="F20" s="73"/>
+      <c r="G20" s="73"/>
+      <c r="H20" s="100"/>
+      <c r="I20" s="109" t="s">
         <v>56</v>
       </c>
-      <c r="J20" s="104"/>
+      <c r="J20" s="101"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="105">
+      <c r="B21" s="103">
         <f>B20+1</f>
         <v>9</v>
       </c>
-      <c r="C21" s="94"/>
-      <c r="D21" s="77"/>
-      <c r="E21" s="77"/>
-      <c r="F21" s="84" t="s">
+      <c r="C21" s="67"/>
+      <c r="D21" s="76"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="84"/>
-      <c r="H21" s="107"/>
-      <c r="I21" s="103" t="s">
+      <c r="G21" s="69"/>
+      <c r="H21" s="106"/>
+      <c r="I21" s="109" t="s">
         <v>55</v>
       </c>
-      <c r="J21" s="104"/>
+      <c r="J21" s="101"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="106"/>
-      <c r="C22" s="97"/>
-      <c r="D22" s="78"/>
-      <c r="E22" s="78"/>
-      <c r="F22" s="85"/>
-      <c r="G22" s="85"/>
+      <c r="B22" s="105"/>
+      <c r="C22" s="68"/>
+      <c r="D22" s="77"/>
+      <c r="E22" s="77"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="70"/>
       <c r="H22" s="108"/>
-      <c r="I22" s="103" t="s">
+      <c r="I22" s="109" t="s">
         <v>35</v>
       </c>
-      <c r="J22" s="104"/>
+      <c r="J22" s="101"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
     </row>
@@ -3869,96 +3736,96 @@
       <c r="C23" s="5"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
-      <c r="F23" s="91" t="s">
+      <c r="F23" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="G23" s="91"/>
-      <c r="H23" s="102"/>
-      <c r="I23" s="103" t="s">
+      <c r="G23" s="73"/>
+      <c r="H23" s="100"/>
+      <c r="I23" s="109" t="s">
         <v>18</v>
       </c>
-      <c r="J23" s="104"/>
+      <c r="J23" s="101"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="105">
+      <c r="B24" s="103">
         <f t="shared" ref="B24:B40" si="0">B23+1</f>
         <v>11</v>
       </c>
-      <c r="C24" s="94"/>
-      <c r="D24" s="77"/>
-      <c r="E24" s="77"/>
-      <c r="F24" s="84" t="s">
+      <c r="C24" s="67"/>
+      <c r="D24" s="76"/>
+      <c r="E24" s="76"/>
+      <c r="F24" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="G24" s="84"/>
-      <c r="H24" s="107"/>
-      <c r="I24" s="112" t="s">
+      <c r="G24" s="69"/>
+      <c r="H24" s="106"/>
+      <c r="I24" s="113" t="s">
         <v>9</v>
       </c>
-      <c r="J24" s="113"/>
+      <c r="J24" s="114"/>
       <c r="K24" s="18"/>
       <c r="L24" s="18"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="106"/>
-      <c r="C25" s="97"/>
-      <c r="D25" s="78"/>
-      <c r="E25" s="78"/>
-      <c r="F25" s="85"/>
-      <c r="G25" s="85"/>
+      <c r="B25" s="105"/>
+      <c r="C25" s="68"/>
+      <c r="D25" s="77"/>
+      <c r="E25" s="77"/>
+      <c r="F25" s="70"/>
+      <c r="G25" s="70"/>
       <c r="H25" s="108"/>
-      <c r="I25" s="103" t="s">
+      <c r="I25" s="109" t="s">
         <v>37</v>
       </c>
-      <c r="J25" s="104"/>
+      <c r="J25" s="101"/>
       <c r="K25" s="18"/>
       <c r="L25" s="18"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="105">
+      <c r="B26" s="103">
         <f>B24+1</f>
         <v>12</v>
       </c>
-      <c r="C26" s="99"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="84"/>
-      <c r="F26" s="84" t="s">
+      <c r="C26" s="84"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="G26" s="84"/>
-      <c r="H26" s="107"/>
-      <c r="I26" s="103" t="s">
+      <c r="G26" s="69"/>
+      <c r="H26" s="106"/>
+      <c r="I26" s="109" t="s">
         <v>31</v>
       </c>
-      <c r="J26" s="104"/>
+      <c r="J26" s="101"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="109"/>
-      <c r="C27" s="100"/>
-      <c r="D27" s="98"/>
-      <c r="E27" s="98"/>
-      <c r="F27" s="98"/>
-      <c r="G27" s="98"/>
-      <c r="H27" s="110"/>
-      <c r="I27" s="103" t="s">
+      <c r="B27" s="104"/>
+      <c r="C27" s="85"/>
+      <c r="D27" s="72"/>
+      <c r="E27" s="72"/>
+      <c r="F27" s="72"/>
+      <c r="G27" s="72"/>
+      <c r="H27" s="107"/>
+      <c r="I27" s="109" t="s">
         <v>33</v>
       </c>
-      <c r="J27" s="111"/>
-      <c r="K27" s="111"/>
-      <c r="L27" s="111"/>
+      <c r="J27" s="110"/>
+      <c r="K27" s="110"/>
+      <c r="L27" s="110"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="109"/>
-      <c r="C28" s="100"/>
-      <c r="D28" s="98"/>
-      <c r="E28" s="98"/>
-      <c r="F28" s="98"/>
-      <c r="G28" s="98"/>
-      <c r="H28" s="110"/>
+      <c r="B28" s="104"/>
+      <c r="C28" s="85"/>
+      <c r="D28" s="72"/>
+      <c r="E28" s="72"/>
+      <c r="F28" s="72"/>
+      <c r="G28" s="72"/>
+      <c r="H28" s="107"/>
       <c r="I28" s="7"/>
       <c r="J28" s="8" t="s">
         <v>32</v>
@@ -3967,13 +3834,13 @@
       <c r="L28" s="4"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="109"/>
-      <c r="C29" s="100"/>
-      <c r="D29" s="98"/>
-      <c r="E29" s="98"/>
-      <c r="F29" s="98"/>
-      <c r="G29" s="98"/>
-      <c r="H29" s="110"/>
+      <c r="B29" s="104"/>
+      <c r="C29" s="85"/>
+      <c r="D29" s="72"/>
+      <c r="E29" s="72"/>
+      <c r="F29" s="72"/>
+      <c r="G29" s="72"/>
+      <c r="H29" s="107"/>
       <c r="I29" s="7"/>
       <c r="J29" s="8" t="s">
         <v>34</v>
@@ -3982,12 +3849,12 @@
       <c r="L29" s="4"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B30" s="106"/>
-      <c r="C30" s="101"/>
-      <c r="D30" s="85"/>
-      <c r="E30" s="85"/>
-      <c r="F30" s="85"/>
-      <c r="G30" s="85"/>
+      <c r="B30" s="105"/>
+      <c r="C30" s="86"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="70"/>
+      <c r="F30" s="70"/>
+      <c r="G30" s="70"/>
       <c r="H30" s="108"/>
       <c r="I30" s="7"/>
       <c r="J30" s="8" t="s">
@@ -4003,53 +3870,53 @@
         <f>B26+1</f>
         <v>13</v>
       </c>
-      <c r="C31" s="101" t="s">
+      <c r="C31" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="85"/>
-      <c r="E31" s="85"/>
-      <c r="F31" s="85"/>
-      <c r="G31" s="85"/>
-      <c r="H31" s="102"/>
-      <c r="I31" s="116" t="s">
+      <c r="D31" s="70"/>
+      <c r="E31" s="70"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="100"/>
+      <c r="I31" s="111" t="s">
         <v>15</v>
       </c>
-      <c r="J31" s="117"/>
+      <c r="J31" s="112"/>
       <c r="K31" s="19"/>
       <c r="L31" s="19"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="105">
+      <c r="B32" s="103">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C32" s="94"/>
-      <c r="D32" s="84" t="s">
+      <c r="C32" s="67"/>
+      <c r="D32" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="E32" s="84"/>
-      <c r="F32" s="84"/>
-      <c r="G32" s="84"/>
-      <c r="H32" s="107"/>
-      <c r="I32" s="103" t="s">
+      <c r="E32" s="69"/>
+      <c r="F32" s="69"/>
+      <c r="G32" s="69"/>
+      <c r="H32" s="106"/>
+      <c r="I32" s="109" t="s">
         <v>14</v>
       </c>
-      <c r="J32" s="104"/>
+      <c r="J32" s="101"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B33" s="106"/>
-      <c r="C33" s="97"/>
-      <c r="D33" s="85"/>
-      <c r="E33" s="85"/>
-      <c r="F33" s="85"/>
-      <c r="G33" s="85"/>
+      <c r="B33" s="105"/>
+      <c r="C33" s="68"/>
+      <c r="D33" s="70"/>
+      <c r="E33" s="70"/>
+      <c r="F33" s="70"/>
+      <c r="G33" s="70"/>
       <c r="H33" s="108"/>
-      <c r="I33" s="103" t="s">
+      <c r="I33" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="J33" s="104"/>
+      <c r="J33" s="101"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
     </row>
@@ -4059,82 +3926,82 @@
         <v>15</v>
       </c>
       <c r="C34" s="5"/>
-      <c r="D34" s="91" t="s">
+      <c r="D34" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="91"/>
-      <c r="F34" s="91"/>
-      <c r="G34" s="91"/>
-      <c r="H34" s="102"/>
-      <c r="I34" s="114"/>
-      <c r="J34" s="115"/>
-      <c r="K34" s="115"/>
-      <c r="L34" s="115"/>
+      <c r="E34" s="73"/>
+      <c r="F34" s="73"/>
+      <c r="G34" s="73"/>
+      <c r="H34" s="100"/>
+      <c r="I34" s="97"/>
+      <c r="J34" s="98"/>
+      <c r="K34" s="98"/>
+      <c r="L34" s="98"/>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B35" s="105">
+      <c r="B35" s="103">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C35" s="94"/>
-      <c r="D35" s="77"/>
-      <c r="E35" s="84" t="s">
+      <c r="C35" s="67"/>
+      <c r="D35" s="76"/>
+      <c r="E35" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="F35" s="84"/>
-      <c r="G35" s="84"/>
-      <c r="H35" s="107"/>
-      <c r="I35" s="103" t="s">
+      <c r="F35" s="69"/>
+      <c r="G35" s="69"/>
+      <c r="H35" s="106"/>
+      <c r="I35" s="109" t="s">
         <v>25</v>
       </c>
-      <c r="J35" s="104"/>
+      <c r="J35" s="101"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B36" s="109"/>
-      <c r="C36" s="95"/>
-      <c r="D36" s="96"/>
-      <c r="E36" s="98"/>
-      <c r="F36" s="98"/>
-      <c r="G36" s="98"/>
-      <c r="H36" s="110"/>
-      <c r="I36" s="103" t="s">
+      <c r="B36" s="104"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="78"/>
+      <c r="E36" s="72"/>
+      <c r="F36" s="72"/>
+      <c r="G36" s="72"/>
+      <c r="H36" s="107"/>
+      <c r="I36" s="109" t="s">
         <v>26</v>
       </c>
-      <c r="J36" s="104"/>
+      <c r="J36" s="101"/>
       <c r="K36" s="20"/>
       <c r="L36" s="21" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B37" s="109"/>
-      <c r="C37" s="95"/>
-      <c r="D37" s="96"/>
-      <c r="E37" s="98"/>
-      <c r="F37" s="98"/>
-      <c r="G37" s="98"/>
-      <c r="H37" s="110"/>
-      <c r="I37" s="103" t="s">
+      <c r="B37" s="104"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="78"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="72"/>
+      <c r="G37" s="72"/>
+      <c r="H37" s="107"/>
+      <c r="I37" s="109" t="s">
         <v>27</v>
       </c>
-      <c r="J37" s="104"/>
+      <c r="J37" s="101"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B38" s="106"/>
-      <c r="C38" s="97"/>
-      <c r="D38" s="78"/>
-      <c r="E38" s="85"/>
-      <c r="F38" s="85"/>
-      <c r="G38" s="85"/>
+      <c r="B38" s="105"/>
+      <c r="C38" s="68"/>
+      <c r="D38" s="77"/>
+      <c r="E38" s="70"/>
+      <c r="F38" s="70"/>
+      <c r="G38" s="70"/>
       <c r="H38" s="108"/>
-      <c r="I38" s="103" t="s">
+      <c r="I38" s="109" t="s">
         <v>43</v>
       </c>
-      <c r="J38" s="104"/>
+      <c r="J38" s="101"/>
       <c r="K38" s="20"/>
       <c r="L38" s="21" t="s">
         <v>29</v>
@@ -4148,160 +4015,160 @@
       <c r="C39" s="5"/>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
-      <c r="F39" s="91" t="s">
+      <c r="F39" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="G39" s="91"/>
-      <c r="H39" s="102"/>
-      <c r="I39" s="103" t="s">
+      <c r="G39" s="73"/>
+      <c r="H39" s="100"/>
+      <c r="I39" s="109" t="s">
         <v>22</v>
       </c>
-      <c r="J39" s="104"/>
+      <c r="J39" s="101"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B40" s="105">
+      <c r="B40" s="103">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C40" s="94"/>
-      <c r="D40" s="77"/>
-      <c r="E40" s="84" t="s">
+      <c r="C40" s="67"/>
+      <c r="D40" s="76"/>
+      <c r="E40" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="F40" s="84"/>
-      <c r="G40" s="84"/>
-      <c r="H40" s="107"/>
-      <c r="I40" s="103" t="s">
+      <c r="F40" s="69"/>
+      <c r="G40" s="69"/>
+      <c r="H40" s="106"/>
+      <c r="I40" s="109" t="s">
         <v>25</v>
       </c>
-      <c r="J40" s="104"/>
+      <c r="J40" s="101"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B41" s="109"/>
-      <c r="C41" s="95"/>
-      <c r="D41" s="96"/>
-      <c r="E41" s="98"/>
-      <c r="F41" s="98"/>
-      <c r="G41" s="98"/>
-      <c r="H41" s="110"/>
-      <c r="I41" s="103" t="s">
+      <c r="B41" s="104"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="78"/>
+      <c r="E41" s="72"/>
+      <c r="F41" s="72"/>
+      <c r="G41" s="72"/>
+      <c r="H41" s="107"/>
+      <c r="I41" s="109" t="s">
         <v>28</v>
       </c>
-      <c r="J41" s="104"/>
+      <c r="J41" s="101"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B42" s="109"/>
-      <c r="C42" s="95"/>
-      <c r="D42" s="96"/>
-      <c r="E42" s="98"/>
-      <c r="F42" s="98"/>
-      <c r="G42" s="98"/>
-      <c r="H42" s="110"/>
-      <c r="I42" s="103" t="s">
+      <c r="B42" s="104"/>
+      <c r="C42" s="71"/>
+      <c r="D42" s="78"/>
+      <c r="E42" s="72"/>
+      <c r="F42" s="72"/>
+      <c r="G42" s="72"/>
+      <c r="H42" s="107"/>
+      <c r="I42" s="109" t="s">
         <v>40</v>
       </c>
-      <c r="J42" s="104"/>
+      <c r="J42" s="101"/>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B43" s="109"/>
-      <c r="C43" s="95"/>
-      <c r="D43" s="96"/>
-      <c r="E43" s="98"/>
-      <c r="F43" s="98"/>
-      <c r="G43" s="98"/>
-      <c r="H43" s="110"/>
-      <c r="I43" s="103" t="s">
+      <c r="B43" s="104"/>
+      <c r="C43" s="71"/>
+      <c r="D43" s="78"/>
+      <c r="E43" s="72"/>
+      <c r="F43" s="72"/>
+      <c r="G43" s="72"/>
+      <c r="H43" s="107"/>
+      <c r="I43" s="109" t="s">
         <v>27</v>
       </c>
-      <c r="J43" s="104"/>
+      <c r="J43" s="101"/>
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B44" s="106"/>
-      <c r="C44" s="95"/>
-      <c r="D44" s="96"/>
-      <c r="E44" s="98"/>
-      <c r="F44" s="98"/>
-      <c r="G44" s="98"/>
-      <c r="H44" s="110"/>
-      <c r="I44" s="103" t="s">
+      <c r="B44" s="105"/>
+      <c r="C44" s="71"/>
+      <c r="D44" s="78"/>
+      <c r="E44" s="72"/>
+      <c r="F44" s="72"/>
+      <c r="G44" s="72"/>
+      <c r="H44" s="107"/>
+      <c r="I44" s="109" t="s">
         <v>43</v>
       </c>
-      <c r="J44" s="104"/>
+      <c r="J44" s="101"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B45" s="105">
+      <c r="B45" s="103">
         <f>B40+1</f>
         <v>19</v>
       </c>
-      <c r="C45" s="94"/>
-      <c r="D45" s="77"/>
-      <c r="E45" s="77"/>
-      <c r="F45" s="84" t="s">
+      <c r="C45" s="67"/>
+      <c r="D45" s="76"/>
+      <c r="E45" s="76"/>
+      <c r="F45" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="G45" s="84"/>
-      <c r="H45" s="107"/>
-      <c r="I45" s="104" t="s">
+      <c r="G45" s="69"/>
+      <c r="H45" s="106"/>
+      <c r="I45" s="101" t="s">
         <v>45</v>
       </c>
-      <c r="J45" s="118"/>
+      <c r="J45" s="102"/>
       <c r="K45" s="4"/>
       <c r="L45" s="4"/>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B46" s="109"/>
-      <c r="C46" s="95"/>
-      <c r="D46" s="96"/>
-      <c r="E46" s="96"/>
-      <c r="F46" s="98"/>
-      <c r="G46" s="98"/>
-      <c r="H46" s="110"/>
-      <c r="I46" s="103" t="s">
+      <c r="B46" s="104"/>
+      <c r="C46" s="71"/>
+      <c r="D46" s="78"/>
+      <c r="E46" s="78"/>
+      <c r="F46" s="72"/>
+      <c r="G46" s="72"/>
+      <c r="H46" s="107"/>
+      <c r="I46" s="109" t="s">
         <v>46</v>
       </c>
-      <c r="J46" s="104"/>
+      <c r="J46" s="101"/>
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B47" s="109"/>
-      <c r="C47" s="95"/>
-      <c r="D47" s="96"/>
-      <c r="E47" s="96"/>
-      <c r="F47" s="98"/>
-      <c r="G47" s="98"/>
-      <c r="H47" s="110"/>
-      <c r="I47" s="103" t="s">
+      <c r="B47" s="104"/>
+      <c r="C47" s="71"/>
+      <c r="D47" s="78"/>
+      <c r="E47" s="78"/>
+      <c r="F47" s="72"/>
+      <c r="G47" s="72"/>
+      <c r="H47" s="107"/>
+      <c r="I47" s="109" t="s">
         <v>52</v>
       </c>
-      <c r="J47" s="104"/>
+      <c r="J47" s="101"/>
       <c r="K47" s="4"/>
       <c r="L47" s="4"/>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B48" s="106"/>
-      <c r="C48" s="97"/>
-      <c r="D48" s="78"/>
-      <c r="E48" s="78"/>
-      <c r="F48" s="85"/>
-      <c r="G48" s="85"/>
+      <c r="B48" s="105"/>
+      <c r="C48" s="68"/>
+      <c r="D48" s="77"/>
+      <c r="E48" s="77"/>
+      <c r="F48" s="70"/>
+      <c r="G48" s="70"/>
       <c r="H48" s="108"/>
-      <c r="I48" s="103" t="s">
+      <c r="I48" s="109" t="s">
         <v>58</v>
       </c>
-      <c r="J48" s="104"/>
+      <c r="J48" s="101"/>
       <c r="K48" s="10"/>
       <c r="L48" s="4" t="s">
         <v>59</v>
@@ -4316,14 +4183,14 @@
       <c r="D49" s="9"/>
       <c r="E49" s="9"/>
       <c r="F49" s="9"/>
-      <c r="G49" s="91" t="s">
+      <c r="G49" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="H49" s="102"/>
-      <c r="I49" s="104" t="s">
+      <c r="H49" s="100"/>
+      <c r="I49" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="J49" s="118"/>
+      <c r="J49" s="102"/>
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
     </row>
@@ -4332,16 +4199,16 @@
         <f t="shared" ref="B50:B60" si="1">B49+1</f>
         <v>21</v>
       </c>
-      <c r="C50" s="92"/>
-      <c r="D50" s="93"/>
-      <c r="E50" s="93"/>
-      <c r="F50" s="93"/>
-      <c r="G50" s="91" t="s">
+      <c r="C50" s="74"/>
+      <c r="D50" s="75"/>
+      <c r="E50" s="75"/>
+      <c r="F50" s="75"/>
+      <c r="G50" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="H50" s="102"/>
-      <c r="I50" s="114"/>
-      <c r="J50" s="119"/>
+      <c r="H50" s="100"/>
+      <c r="I50" s="97"/>
+      <c r="J50" s="99"/>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
     </row>
@@ -4356,8 +4223,8 @@
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
       <c r="H51" s="6"/>
-      <c r="I51" s="114"/>
-      <c r="J51" s="119"/>
+      <c r="I51" s="97"/>
+      <c r="J51" s="99"/>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
     </row>
@@ -4372,8 +4239,8 @@
       <c r="F52" s="9"/>
       <c r="G52" s="9"/>
       <c r="H52" s="6"/>
-      <c r="I52" s="114"/>
-      <c r="J52" s="119"/>
+      <c r="I52" s="97"/>
+      <c r="J52" s="99"/>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
     </row>
@@ -4388,8 +4255,8 @@
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
       <c r="H53" s="6"/>
-      <c r="I53" s="114"/>
-      <c r="J53" s="119"/>
+      <c r="I53" s="97"/>
+      <c r="J53" s="99"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
     </row>
@@ -4404,8 +4271,8 @@
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
       <c r="H54" s="6"/>
-      <c r="I54" s="114"/>
-      <c r="J54" s="119"/>
+      <c r="I54" s="97"/>
+      <c r="J54" s="99"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
     </row>
@@ -4420,8 +4287,8 @@
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
       <c r="H55" s="6"/>
-      <c r="I55" s="114"/>
-      <c r="J55" s="119"/>
+      <c r="I55" s="97"/>
+      <c r="J55" s="99"/>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
     </row>
@@ -4436,8 +4303,8 @@
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
       <c r="H56" s="6"/>
-      <c r="I56" s="114"/>
-      <c r="J56" s="119"/>
+      <c r="I56" s="97"/>
+      <c r="J56" s="99"/>
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
     </row>
@@ -4452,8 +4319,8 @@
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
       <c r="H57" s="6"/>
-      <c r="I57" s="114"/>
-      <c r="J57" s="119"/>
+      <c r="I57" s="97"/>
+      <c r="J57" s="99"/>
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
     </row>
@@ -4468,8 +4335,8 @@
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
       <c r="H58" s="6"/>
-      <c r="I58" s="114"/>
-      <c r="J58" s="119"/>
+      <c r="I58" s="97"/>
+      <c r="J58" s="99"/>
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
     </row>
@@ -4484,8 +4351,8 @@
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
       <c r="H59" s="6"/>
-      <c r="I59" s="114"/>
-      <c r="J59" s="119"/>
+      <c r="I59" s="97"/>
+      <c r="J59" s="99"/>
       <c r="K59" s="4"/>
       <c r="L59" s="4"/>
     </row>
@@ -4500,13 +4367,90 @@
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
       <c r="H60" s="6"/>
-      <c r="I60" s="114"/>
-      <c r="J60" s="119"/>
+      <c r="I60" s="97"/>
+      <c r="J60" s="99"/>
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="93">
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:H8"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:H10"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="C15:E19"/>
+    <mergeCell ref="F15:H19"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="D11:H13"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:E22"/>
+    <mergeCell ref="F21:H22"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:E25"/>
+    <mergeCell ref="F24:H25"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="D34:H34"/>
+    <mergeCell ref="I34:L34"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="C26:E30"/>
+    <mergeCell ref="F26:H30"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I27:L27"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:H33"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="C35:D38"/>
+    <mergeCell ref="E35:H38"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="B40:B44"/>
+    <mergeCell ref="C40:D44"/>
+    <mergeCell ref="E40:H44"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="C45:E48"/>
+    <mergeCell ref="F45:H48"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="I48:J48"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="I59:J59"/>
     <mergeCell ref="I60:J60"/>
@@ -4523,83 +4467,6 @@
     <mergeCell ref="G50:H50"/>
     <mergeCell ref="I50:J50"/>
     <mergeCell ref="I51:J51"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="C45:E48"/>
-    <mergeCell ref="F45:H48"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="I48:J48"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="B40:B44"/>
-    <mergeCell ref="C40:D44"/>
-    <mergeCell ref="E40:H44"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="C35:D38"/>
-    <mergeCell ref="E35:H38"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="D34:H34"/>
-    <mergeCell ref="I34:L34"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="C26:E30"/>
-    <mergeCell ref="F26:H30"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I27:L27"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:H33"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:E25"/>
-    <mergeCell ref="F24:H25"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:E22"/>
-    <mergeCell ref="F21:H22"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="C15:E19"/>
-    <mergeCell ref="F15:H19"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I16:L16"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="D11:H13"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:H10"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:H8"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>